<commit_message>
TRY N2 Vocab.xlsx -> Day14 Words are added.
</commit_message>
<xml_diff>
--- a/preparing/TRY N2 Vocab.xlsx
+++ b/preparing/TRY N2 Vocab.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="636">
   <si>
     <t>お知らせ</t>
   </si>
@@ -1806,6 +1806,129 @@
   </si>
   <si>
     <t>Day1 =&gt; kana corrected</t>
+  </si>
+  <si>
+    <t>Day 14</t>
+  </si>
+  <si>
+    <t>就任</t>
+  </si>
+  <si>
+    <t>発展</t>
+  </si>
+  <si>
+    <t>ノーベル賞</t>
+  </si>
+  <si>
+    <t>受賞</t>
+  </si>
+  <si>
+    <t>受験生</t>
+  </si>
+  <si>
+    <t>地域ぐるみ</t>
+  </si>
+  <si>
+    <t>開港</t>
+  </si>
+  <si>
+    <t>～周年</t>
+  </si>
+  <si>
+    <t>企業研究</t>
+  </si>
+  <si>
+    <t>growth (to grow)</t>
+  </si>
+  <si>
+    <t>Nobel Prize</t>
+  </si>
+  <si>
+    <t>receiving a prize (to receive a prize)</t>
+  </si>
+  <si>
+    <t>test taker</t>
+  </si>
+  <si>
+    <t>involving the whole area/region</t>
+  </si>
+  <si>
+    <t>opening a port (to open a port)</t>
+  </si>
+  <si>
+    <t>researching companies</t>
+  </si>
+  <si>
+    <t>～anniversary</t>
+  </si>
+  <si>
+    <t>(1,2,…)+</t>
+  </si>
+  <si>
+    <t>taking a post (to take a post for high position)</t>
+  </si>
+  <si>
+    <t>ရာထူးရယူသည္</t>
+  </si>
+  <si>
+    <t>ဖြံ႔ၿဖိဳးတိုးတက္သည္</t>
+  </si>
+  <si>
+    <t>ဆုလက္ခံရရွိသည္</t>
+  </si>
+  <si>
+    <t>နယ္ေျမတစ္ခုလံုးပါ၀င္မႈ</t>
+  </si>
+  <si>
+    <t>(ေလယာဥ္၊ သေဘၤာ၊…)ဆိပ္ဖြင့္လွစ္သည္</t>
+  </si>
+  <si>
+    <t>～ႏွစ္ပတ္လည္</t>
+  </si>
+  <si>
+    <t>しゅうにん</t>
+  </si>
+  <si>
+    <t>はってん</t>
+  </si>
+  <si>
+    <t>ノーベルしょう</t>
+  </si>
+  <si>
+    <t>じゅしょう</t>
+  </si>
+  <si>
+    <t>じゅけんせい</t>
+  </si>
+  <si>
+    <t>ちいきぐるみ</t>
+  </si>
+  <si>
+    <t>かいこう</t>
+  </si>
+  <si>
+    <t>～しゅうねん</t>
+  </si>
+  <si>
+    <t>ရာထူးရယူသည်</t>
+  </si>
+  <si>
+    <t>ဖွံ့ဖြိုးတိုးတက်သည်</t>
+  </si>
+  <si>
+    <t>ဆုလက်ခံရရှိသည်</t>
+  </si>
+  <si>
+    <t>နယ်မြေတစ်ခုလုံးပါဝင်မှု</t>
+  </si>
+  <si>
+    <t>(လေယာဉ်၊ သင်္ဘော၊…)ဆိပ်ဖွင့်လှစ်သည်</t>
+  </si>
+  <si>
+    <t>～နှစ်ပတ်လည်</t>
+  </si>
+  <si>
+    <t>Day14 added</t>
   </si>
 </sst>
 </file>
@@ -1912,7 +2035,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1949,10 +2072,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1973,6 +2092,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2280,16 +2408,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="19" customWidth="1"/>
-    <col min="5" max="5" width="51.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="17" customWidth="1"/>
+    <col min="5" max="5" width="51.85546875" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2307,238 +2435,246 @@
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="16">
+      <c r="B3" s="14">
         <v>0</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="22" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="16">
+      <c r="B4" s="14">
         <v>1</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="15">
         <v>43481</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="18" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="16">
+      <c r="B5" s="14">
         <v>2</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="15">
         <v>43482</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="18" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="16">
+      <c r="B6" s="14">
         <v>3</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="15">
         <v>43483</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="18" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="16">
+      <c r="B7" s="14">
         <v>4</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="15">
         <v>43486</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="18" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16">
+      <c r="B8" s="14">
         <v>5</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="15">
         <v>43489</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="18" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="16">
+      <c r="B9" s="14">
         <v>6</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="15">
         <v>43490</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="18" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="16">
+      <c r="B10" s="14">
         <v>7</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="15">
         <v>43490</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="18" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="16">
+      <c r="B11" s="14">
         <v>8</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="15">
         <v>43493</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="18" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="16">
+      <c r="B12" s="14">
         <v>9</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="15">
         <v>43494</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="18" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="16">
+      <c r="B13" s="14">
         <v>10</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="15">
         <v>43495</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="23" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="16">
+      <c r="B14" s="14">
         <v>11</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="15">
         <v>43497</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="23" t="s">
         <v>555</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="16">
+      <c r="B15" s="14">
         <v>12</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="15">
         <v>43501</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="23" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="16">
+      <c r="B16" s="14">
         <v>13</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="15">
         <v>43501</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="23" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="16">
+      <c r="B17" s="14">
         <v>14</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="15">
         <v>43501</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="23" t="s">
         <v>594</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="15"/>
+      <c r="B18" s="14">
+        <v>15</v>
+      </c>
+      <c r="C18" s="15">
+        <v>43501</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>635</v>
+      </c>
     </row>
     <row r="19" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="15"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="23"/>
     </row>
     <row r="20" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="15"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="23"/>
     </row>
     <row r="21" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="15"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2547,10 +2683,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I188"/>
+  <dimension ref="A1:I201"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A190" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B198" sqref="B198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.55000000000000004"/>
@@ -2837,7 +2973,7 @@
       <c r="B17" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="21" t="s">
         <v>593</v>
       </c>
       <c r="E17" t="s">
@@ -4610,7 +4746,7 @@
       <c r="C128" t="s">
         <v>384</v>
       </c>
-      <c r="E128" s="21" t="s">
+      <c r="E128" s="19" t="s">
         <v>389</v>
       </c>
       <c r="I128" s="10" t="str">
@@ -4849,7 +4985,7 @@
       <c r="C142" t="s">
         <v>443</v>
       </c>
-      <c r="E142" s="21" t="s">
+      <c r="E142" s="19" t="s">
         <v>535</v>
       </c>
       <c r="F142" s="1" t="s">
@@ -5120,10 +5256,10 @@
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B158" s="23" t="s">
+      <c r="B158" s="21" t="s">
         <v>591</v>
       </c>
-      <c r="C158" s="23" t="s">
+      <c r="C158" s="21" t="s">
         <v>591</v>
       </c>
       <c r="E158" t="s">
@@ -5246,7 +5382,7 @@
       <c r="C165" t="s">
         <v>460</v>
       </c>
-      <c r="E165" s="21" t="s">
+      <c r="E165" s="19" t="s">
         <v>552</v>
       </c>
       <c r="F165" s="1" t="s">
@@ -5352,7 +5488,7 @@
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B172" s="23" t="s">
+      <c r="B172" s="21" t="s">
         <v>590</v>
       </c>
       <c r="C172" t="s">
@@ -5447,7 +5583,7 @@
         <v xml:space="preserve"> engineer (kana)</v>
       </c>
     </row>
-    <row r="177" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B177" t="s">
         <v>434</v>
       </c>
@@ -5468,7 +5604,7 @@
         <v xml:space="preserve"> assumption  ; ကြိုတင်ယူဆချက် ; ႀကိဳတင္ယူဆခ်က္</v>
       </c>
     </row>
-    <row r="178" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B178" t="s">
         <v>435</v>
       </c>
@@ -5492,7 +5628,7 @@
         <v xml:space="preserve"> association; society; acquaintance (する) ; ၁။ပေါင်းသင်းဆက်ဆံသည်၊ ၂။ Date လုပ်သည် ; ၁။ေပါင္းသင္းဆက္ဆံသည္၊ ၂။ Date လုပ္သည္</v>
       </c>
     </row>
-    <row r="179" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B179" t="s">
         <v>436</v>
       </c>
@@ -5503,11 +5639,11 @@
         <v>501</v>
       </c>
       <c r="I179" s="10" t="str">
-        <f t="shared" si="15"/>
+        <f>CONCATENATE(D179," ",E179," ",F179)</f>
         <v xml:space="preserve"> profit </v>
       </c>
     </row>
-    <row r="180" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B180" t="s">
         <v>437</v>
       </c>
@@ -5522,7 +5658,7 @@
         <v xml:space="preserve"> economic activity </v>
       </c>
     </row>
-    <row r="181" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B181" t="s">
         <v>438</v>
       </c>
@@ -5540,7 +5676,7 @@
         <v xml:space="preserve"> hire, use; adoption; acceptance (する)</v>
       </c>
     </row>
-    <row r="182" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B182" t="s">
         <v>439</v>
       </c>
@@ -5555,7 +5691,7 @@
         <v xml:space="preserve"> captain </v>
       </c>
     </row>
-    <row r="183" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B183" t="s">
         <v>440</v>
       </c>
@@ -5570,7 +5706,7 @@
         <v xml:space="preserve"> all together </v>
       </c>
     </row>
-    <row r="184" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B184" t="s">
         <v>557</v>
       </c>
@@ -5591,7 +5727,7 @@
         <v xml:space="preserve"> with all one's strength  ; စိတ်အားရတဲ့အထိ ; စိတ္အားရတဲ႔အထိ</v>
       </c>
     </row>
-    <row r="185" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B185" t="s">
         <v>558</v>
       </c>
@@ -5606,7 +5742,7 @@
         <v xml:space="preserve"> coach, manager </v>
       </c>
     </row>
-    <row r="186" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B186" t="s">
         <v>559</v>
       </c>
@@ -5630,7 +5766,7 @@
         <v xml:space="preserve"> a letter (to submit a letter) (する) ; ကိုယ့်ထင်မြင်ချက်ကို ဖော်ပြတဲ့စာ ; ကိုယ့္ထင္ျမင္ခ်က္ကို ေဖာ္ျပတဲ႔စာ</v>
       </c>
     </row>
-    <row r="187" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B187" t="s">
         <v>560</v>
       </c>
@@ -5645,7 +5781,7 @@
         <v xml:space="preserve"> insect </v>
       </c>
     </row>
-    <row r="188" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B188" t="s">
         <v>561</v>
       </c>
@@ -5655,10 +5791,205 @@
       <c r="E188" t="s">
         <v>588</v>
       </c>
-      <c r="H188" s="22"/>
+      <c r="H188" s="20"/>
       <c r="I188" s="10" t="str">
         <f t="shared" si="15"/>
         <v xml:space="preserve"> Souvenirs Entomologiques (a book name written by Jean-Henri Fabre) </v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A190" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="B190" s="6"/>
+      <c r="C190" s="6"/>
+      <c r="D190" s="7"/>
+      <c r="E190" s="6"/>
+      <c r="F190" s="7"/>
+      <c r="G190" s="12"/>
+      <c r="H190" s="12"/>
+      <c r="I190" s="10" t="str">
+        <f>CONCATENATE(D190," ",E190," ",F190)</f>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B191" t="s">
+        <v>596</v>
+      </c>
+      <c r="C191" t="s">
+        <v>621</v>
+      </c>
+      <c r="E191" t="s">
+        <v>614</v>
+      </c>
+      <c r="F191" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G191" s="10" t="s">
+        <v>629</v>
+      </c>
+      <c r="H191" s="10" t="s">
+        <v>615</v>
+      </c>
+      <c r="I191" s="10" t="str">
+        <f>CONCATENATE(D191," ",E191," ",F191, " ; ",G191," ; ", H191)</f>
+        <v xml:space="preserve"> taking a post (to take a post for high position) (する) ; ရာထူးရယူသည် ; ရာထူးရယူသည္</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B192" t="s">
+        <v>597</v>
+      </c>
+      <c r="C192" t="s">
+        <v>622</v>
+      </c>
+      <c r="E192" t="s">
+        <v>605</v>
+      </c>
+      <c r="F192" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G192" s="10" t="s">
+        <v>630</v>
+      </c>
+      <c r="H192" s="10" t="s">
+        <v>616</v>
+      </c>
+      <c r="I192" s="10" t="str">
+        <f>CONCATENATE(D192," ",E192," ",F192, " ; ",G192," ; ", H192)</f>
+        <v xml:space="preserve"> growth (to grow) (する) ; ဖွံ့ဖြိုးတိုးတက်သည် ; ဖြံ႔ၿဖိဳးတိုးတက္သည္</v>
+      </c>
+    </row>
+    <row r="193" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B193" t="s">
+        <v>598</v>
+      </c>
+      <c r="C193" t="s">
+        <v>623</v>
+      </c>
+      <c r="E193" t="s">
+        <v>606</v>
+      </c>
+      <c r="I193" s="10" t="str">
+        <f>CONCATENATE(D193," ",E193," ",F193)</f>
+        <v xml:space="preserve"> Nobel Prize </v>
+      </c>
+    </row>
+    <row r="194" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B194" t="s">
+        <v>599</v>
+      </c>
+      <c r="C194" t="s">
+        <v>624</v>
+      </c>
+      <c r="E194" t="s">
+        <v>607</v>
+      </c>
+      <c r="F194" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G194" s="10" t="s">
+        <v>631</v>
+      </c>
+      <c r="H194" s="10" t="s">
+        <v>617</v>
+      </c>
+      <c r="I194" s="10" t="str">
+        <f>CONCATENATE(D194," ",E194," ",F194, " ; ",G194," ; ", H194)</f>
+        <v xml:space="preserve"> receiving a prize (to receive a prize) (する) ; ဆုလက်ခံရရှိသည် ; ဆုလက္ခံရရွိသည္</v>
+      </c>
+    </row>
+    <row r="195" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B195" t="s">
+        <v>600</v>
+      </c>
+      <c r="C195" t="s">
+        <v>625</v>
+      </c>
+      <c r="E195" t="s">
+        <v>608</v>
+      </c>
+      <c r="I195" s="10" t="str">
+        <f>CONCATENATE(D195," ",E195," ",F195)</f>
+        <v xml:space="preserve"> test taker </v>
+      </c>
+    </row>
+    <row r="196" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B196" t="s">
+        <v>601</v>
+      </c>
+      <c r="C196" t="s">
+        <v>626</v>
+      </c>
+      <c r="E196" t="s">
+        <v>609</v>
+      </c>
+      <c r="G196" s="10" t="s">
+        <v>632</v>
+      </c>
+      <c r="H196" s="10" t="s">
+        <v>618</v>
+      </c>
+      <c r="I196" s="10" t="str">
+        <f t="shared" ref="I196:I198" si="18">CONCATENATE(D196," ",E196," ",F196, " ; ",G196," ; ", H196)</f>
+        <v xml:space="preserve"> involving the whole area/region  ; နယ်မြေတစ်ခုလုံးပါဝင်မှု ; နယ္ေျမတစ္ခုလံုးပါ၀င္မႈ</v>
+      </c>
+    </row>
+    <row r="197" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B197" t="s">
+        <v>602</v>
+      </c>
+      <c r="C197" t="s">
+        <v>627</v>
+      </c>
+      <c r="E197" t="s">
+        <v>610</v>
+      </c>
+      <c r="F197" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G197" s="10" t="s">
+        <v>633</v>
+      </c>
+      <c r="H197" s="10" t="s">
+        <v>619</v>
+      </c>
+      <c r="I197" s="10" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve"> opening a port (to open a port) (する) ; (လေယာဉ်၊ သင်္ဘော၊…)ဆိပ်ဖွင့်လှစ်သည် ; (ေလယာဥ္၊ သေဘၤာ၊…)ဆိပ္ဖြင့္လွစ္သည္</v>
+      </c>
+    </row>
+    <row r="198" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B198" t="s">
+        <v>603</v>
+      </c>
+      <c r="C198" t="s">
+        <v>628</v>
+      </c>
+      <c r="D198" t="s">
+        <v>613</v>
+      </c>
+      <c r="E198" s="19" t="s">
+        <v>612</v>
+      </c>
+      <c r="G198" s="10" t="s">
+        <v>634</v>
+      </c>
+      <c r="H198" s="10" t="s">
+        <v>620</v>
+      </c>
+      <c r="I198" s="10" t="str">
+        <f t="shared" si="18"/>
+        <v>(1,2,…)+ ～anniversary  ; ～နှစ်ပတ်လည် ; ～ႏွစ္ပတ္လည္</v>
+      </c>
+    </row>
+    <row r="201" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B201" t="s">
+        <v>604</v>
+      </c>
+      <c r="E201" t="s">
+        <v>611</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TRY N2 Vocab.xlsx -> Day15 Words are added.
</commit_message>
<xml_diff>
--- a/preparing/TRY N2 Vocab.xlsx
+++ b/preparing/TRY N2 Vocab.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="681">
   <si>
     <t>お知らせ</t>
   </si>
@@ -1929,6 +1929,141 @@
   </si>
   <si>
     <t>Day14 added</t>
+  </si>
+  <si>
+    <t>パティシエ</t>
+  </si>
+  <si>
+    <t>コンテスト</t>
+  </si>
+  <si>
+    <t>出場</t>
+  </si>
+  <si>
+    <t>三ツ星レストラン</t>
+  </si>
+  <si>
+    <t>扱う</t>
+  </si>
+  <si>
+    <t>期日</t>
+  </si>
+  <si>
+    <t>間に合わせる</t>
+  </si>
+  <si>
+    <t>誇り</t>
+  </si>
+  <si>
+    <t>力を尽くす</t>
+  </si>
+  <si>
+    <t>税金</t>
+  </si>
+  <si>
+    <t>争う</t>
+  </si>
+  <si>
+    <t>きぎょうけんきゅう</t>
+  </si>
+  <si>
+    <t>しゅつじょう</t>
+  </si>
+  <si>
+    <t>みつぼしレストラン</t>
+  </si>
+  <si>
+    <t>あつかう</t>
+  </si>
+  <si>
+    <t>きじつ</t>
+  </si>
+  <si>
+    <t>まにあわせる</t>
+  </si>
+  <si>
+    <t>ほこり</t>
+  </si>
+  <si>
+    <t>ちからをつくす</t>
+  </si>
+  <si>
+    <t>ぜいきん</t>
+  </si>
+  <si>
+    <t>あらそう</t>
+  </si>
+  <si>
+    <t>pastry chef</t>
+  </si>
+  <si>
+    <t>contest</t>
+  </si>
+  <si>
+    <t>entry (to enter)</t>
+  </si>
+  <si>
+    <t>three-star restaurant</t>
+  </si>
+  <si>
+    <t>to handle</t>
+  </si>
+  <si>
+    <t>to meet, be in time</t>
+  </si>
+  <si>
+    <t>pride</t>
+  </si>
+  <si>
+    <t>to make a full effort</t>
+  </si>
+  <si>
+    <t>tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to contest, dispute </t>
+  </si>
+  <si>
+    <t>မုန္႔အခ်ိဳပြဲလုပ္တဲ႔သူ</t>
+  </si>
+  <si>
+    <t>တက္ေရာက္သည္</t>
+  </si>
+  <si>
+    <t>ကိုင္တြယ္သည္</t>
+  </si>
+  <si>
+    <t>ယွဥ္ၿပိဳင္သည္၊ စကားမ်ားသည္</t>
+  </si>
+  <si>
+    <t>အင္အားစိုက္ထုတ္ႀကိဳးပမ္းသည္</t>
+  </si>
+  <si>
+    <t>ဂုဏ္၊ ဂုဏ္ယူျခင္း</t>
+  </si>
+  <si>
+    <t>အခ်ိန္မီ ျဖစ္ေစသည္</t>
+  </si>
+  <si>
+    <t>မုန့်အချိုပွဲလုပ်တဲ့သူ</t>
+  </si>
+  <si>
+    <t>တက်ရောက်သည်</t>
+  </si>
+  <si>
+    <t>အချိန်မီ ဖြစ်စေသည်</t>
+  </si>
+  <si>
+    <t>ဂုဏ်၊ ဂုဏ်ယူခြင်း</t>
+  </si>
+  <si>
+    <t>အင်အားစိုက်ထုတ်ကြိုးပမ်းသည်</t>
+  </si>
+  <si>
+    <t>ယှဉ်ပြိုင်သည်၊ စကားများသည်</t>
+  </si>
+  <si>
+    <t>Day15 added</t>
   </si>
 </sst>
 </file>
@@ -2408,8 +2543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2659,10 +2794,18 @@
       </c>
     </row>
     <row r="19" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="23"/>
+      <c r="B19" s="14">
+        <v>16</v>
+      </c>
+      <c r="C19" s="15">
+        <v>43502</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="20" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
@@ -2683,10 +2826,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I201"/>
+  <dimension ref="A1:I212"/>
   <sheetViews>
-    <sheetView topLeftCell="A190" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B198" sqref="B198"/>
+    <sheetView topLeftCell="A199" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B212" sqref="B212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.55000000000000004"/>
@@ -5988,8 +6131,227 @@
       <c r="B201" t="s">
         <v>604</v>
       </c>
+      <c r="C201" t="s">
+        <v>647</v>
+      </c>
       <c r="E201" t="s">
         <v>611</v>
+      </c>
+    </row>
+    <row r="202" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B202" t="s">
+        <v>636</v>
+      </c>
+      <c r="C202" t="s">
+        <v>636</v>
+      </c>
+      <c r="E202" t="s">
+        <v>657</v>
+      </c>
+      <c r="F202" t="s">
+        <v>587</v>
+      </c>
+      <c r="G202" s="10" t="s">
+        <v>674</v>
+      </c>
+      <c r="H202" s="10" t="s">
+        <v>667</v>
+      </c>
+      <c r="I202" s="10" t="str">
+        <f t="shared" ref="I202" si="19">CONCATENATE(D202," ",E202," ",F202, " ; ",G202," ; ", H202)</f>
+        <v xml:space="preserve"> pastry chef (kana) ; မုန့်အချိုပွဲလုပ်တဲ့သူ ; မုန္႔အခ်ိဳပြဲလုပ္တဲ႔သူ</v>
+      </c>
+    </row>
+    <row r="203" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B203" t="s">
+        <v>637</v>
+      </c>
+      <c r="C203" t="s">
+        <v>637</v>
+      </c>
+      <c r="E203" t="s">
+        <v>658</v>
+      </c>
+      <c r="F203" t="s">
+        <v>587</v>
+      </c>
+      <c r="I203" s="10" t="str">
+        <f>CONCATENATE(D203," ",E203," ",F203)</f>
+        <v xml:space="preserve"> contest (kana)</v>
+      </c>
+    </row>
+    <row r="204" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B204" t="s">
+        <v>638</v>
+      </c>
+      <c r="C204" t="s">
+        <v>648</v>
+      </c>
+      <c r="E204" t="s">
+        <v>659</v>
+      </c>
+      <c r="F204" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G204" s="10" t="s">
+        <v>675</v>
+      </c>
+      <c r="H204" s="10" t="s">
+        <v>668</v>
+      </c>
+      <c r="I204" s="10" t="str">
+        <f t="shared" ref="I204" si="20">CONCATENATE(D204," ",E204," ",F204, " ; ",G204," ; ", H204)</f>
+        <v xml:space="preserve"> entry (to enter) (する) ; တက်ရောက်သည် ; တက္ေရာက္သည္</v>
+      </c>
+    </row>
+    <row r="205" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B205" t="s">
+        <v>639</v>
+      </c>
+      <c r="C205" t="s">
+        <v>649</v>
+      </c>
+      <c r="E205" t="s">
+        <v>660</v>
+      </c>
+      <c r="I205" s="10" t="str">
+        <f>CONCATENATE(D205," ",E205," ",F205)</f>
+        <v xml:space="preserve"> three-star restaurant </v>
+      </c>
+    </row>
+    <row r="206" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B206" t="s">
+        <v>640</v>
+      </c>
+      <c r="C206" t="s">
+        <v>650</v>
+      </c>
+      <c r="E206" t="s">
+        <v>661</v>
+      </c>
+      <c r="G206" s="10" t="s">
+        <v>669</v>
+      </c>
+      <c r="H206" s="10" t="s">
+        <v>669</v>
+      </c>
+      <c r="I206" s="10" t="str">
+        <f t="shared" ref="I206" si="21">CONCATENATE(D206," ",E206," ",F206, " ; ",G206," ; ", H206)</f>
+        <v xml:space="preserve"> to handle  ; ကိုင္တြယ္သည္ ; ကိုင္တြယ္သည္</v>
+      </c>
+    </row>
+    <row r="207" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B207" t="s">
+        <v>641</v>
+      </c>
+      <c r="C207" t="s">
+        <v>651</v>
+      </c>
+      <c r="E207" t="s">
+        <v>265</v>
+      </c>
+      <c r="I207" s="10" t="str">
+        <f>CONCATENATE(D207," ",E207," ",F207)</f>
+        <v xml:space="preserve"> deadline </v>
+      </c>
+    </row>
+    <row r="208" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B208" t="s">
+        <v>642</v>
+      </c>
+      <c r="C208" t="s">
+        <v>652</v>
+      </c>
+      <c r="E208" t="s">
+        <v>662</v>
+      </c>
+      <c r="G208" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="H208" s="10" t="s">
+        <v>673</v>
+      </c>
+      <c r="I208" s="10" t="str">
+        <f t="shared" ref="I208:I210" si="22">CONCATENATE(D208," ",E208," ",F208, " ; ",G208," ; ", H208)</f>
+        <v xml:space="preserve"> to meet, be in time  ; အချိန်မီ ဖြစ်စေသည် ; အခ်ိန္မီ ျဖစ္ေစသည္</v>
+      </c>
+    </row>
+    <row r="209" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B209" t="s">
+        <v>643</v>
+      </c>
+      <c r="C209" t="s">
+        <v>653</v>
+      </c>
+      <c r="E209" t="s">
+        <v>663</v>
+      </c>
+      <c r="G209" s="10" t="s">
+        <v>677</v>
+      </c>
+      <c r="H209" s="10" t="s">
+        <v>672</v>
+      </c>
+      <c r="I209" s="10" t="str">
+        <f t="shared" si="22"/>
+        <v xml:space="preserve"> pride  ; ဂုဏ်၊ ဂုဏ်ယူခြင်း ; ဂုဏ္၊ ဂုဏ္ယူျခင္း</v>
+      </c>
+    </row>
+    <row r="210" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B210" t="s">
+        <v>644</v>
+      </c>
+      <c r="C210" t="s">
+        <v>654</v>
+      </c>
+      <c r="E210" t="s">
+        <v>664</v>
+      </c>
+      <c r="G210" s="10" t="s">
+        <v>678</v>
+      </c>
+      <c r="H210" s="10" t="s">
+        <v>671</v>
+      </c>
+      <c r="I210" s="10" t="str">
+        <f t="shared" si="22"/>
+        <v xml:space="preserve"> to make a full effort  ; အင်အားစိုက်ထုတ်ကြိုးပမ်းသည် ; အင္အားစိုက္ထုတ္ႀကိဳးပမ္းသည္</v>
+      </c>
+    </row>
+    <row r="211" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B211" t="s">
+        <v>645</v>
+      </c>
+      <c r="C211" t="s">
+        <v>655</v>
+      </c>
+      <c r="E211" t="s">
+        <v>665</v>
+      </c>
+      <c r="I211" s="10" t="str">
+        <f>CONCATENATE(D211," ",E211," ",F211)</f>
+        <v xml:space="preserve"> tax </v>
+      </c>
+    </row>
+    <row r="212" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B212" t="s">
+        <v>646</v>
+      </c>
+      <c r="C212" t="s">
+        <v>656</v>
+      </c>
+      <c r="E212" t="s">
+        <v>666</v>
+      </c>
+      <c r="G212" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="H212" s="10" t="s">
+        <v>670</v>
+      </c>
+      <c r="I212" s="10" t="str">
+        <f t="shared" ref="I212" si="23">CONCATENATE(D212," ",E212," ",F212, " ; ",G212," ; ", H212)</f>
+        <v xml:space="preserve"> to contest, dispute   ; ယှဉ်ပြိုင်သည်၊ စကားများသည် ; ယွဥ္ၿပိဳင္သည္၊ စကားမ်ားသည္</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TRY N2 Vocab.xlsx -> Day15 Definition updated
</commit_message>
<xml_diff>
--- a/preparing/TRY N2 Vocab.xlsx
+++ b/preparing/TRY N2 Vocab.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="684">
   <si>
     <t>お知らせ</t>
   </si>
@@ -2064,6 +2064,15 @@
   </si>
   <si>
     <t>Day15 added</t>
+  </si>
+  <si>
+    <t>သတ္မွတ္ေနာက္ဆံုးေန႔ရက္</t>
+  </si>
+  <si>
+    <t>သတ်မှတ်နောက်ဆုံးနေ့ရက်</t>
+  </si>
+  <si>
+    <t>Day15 =&gt; MM Definition updated</t>
   </si>
 </sst>
 </file>
@@ -2170,7 +2179,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2236,6 +2245,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2544,7 +2557,7 @@
   <dimension ref="B2:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2808,10 +2821,18 @@
       </c>
     </row>
     <row r="20" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="23"/>
+      <c r="B20" s="14">
+        <v>17</v>
+      </c>
+      <c r="C20" s="15">
+        <v>43502</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="21" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
@@ -2829,7 +2850,7 @@
   <dimension ref="A1:I212"/>
   <sheetViews>
     <sheetView topLeftCell="A199" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B212" sqref="B212"/>
+      <selection activeCell="G207" sqref="G207:H207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.55000000000000004"/>
@@ -2840,7 +2861,7 @@
     <col min="4" max="4" width="6.42578125" customWidth="1"/>
     <col min="5" max="5" width="31" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="27" style="10" customWidth="1"/>
     <col min="8" max="8" width="15" style="10" customWidth="1"/>
     <col min="9" max="9" width="42.140625" customWidth="1"/>
   </cols>
@@ -6236,7 +6257,7 @@
         <v>669</v>
       </c>
       <c r="I206" s="10" t="str">
-        <f t="shared" ref="I206" si="21">CONCATENATE(D206," ",E206," ",F206, " ; ",G206," ; ", H206)</f>
+        <f t="shared" ref="I206:I207" si="21">CONCATENATE(D206," ",E206," ",F206, " ; ",G206," ; ", H206)</f>
         <v xml:space="preserve"> to handle  ; ကိုင္တြယ္သည္ ; ကိုင္တြယ္သည္</v>
       </c>
     </row>
@@ -6250,9 +6271,15 @@
       <c r="E207" t="s">
         <v>265</v>
       </c>
+      <c r="G207" s="25" t="s">
+        <v>682</v>
+      </c>
+      <c r="H207" s="26" t="s">
+        <v>681</v>
+      </c>
       <c r="I207" s="10" t="str">
-        <f>CONCATENATE(D207," ",E207," ",F207)</f>
-        <v xml:space="preserve"> deadline </v>
+        <f t="shared" si="21"/>
+        <v xml:space="preserve"> deadline  ; သတ်မှတ်နောက်ဆုံးနေ့ရက် ; သတ္မွတ္ေနာက္ဆံုးေန႔ရက္</v>
       </c>
     </row>
     <row r="208" spans="2:9" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
TRY N2 Vocab.xlsx -> Day15 Eng Definition updated
</commit_message>
<xml_diff>
--- a/preparing/TRY N2 Vocab.xlsx
+++ b/preparing/TRY N2 Vocab.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="685">
   <si>
     <t>お知らせ</t>
   </si>
@@ -2073,6 +2073,9 @@
   </si>
   <si>
     <t>Day15 =&gt; MM Definition updated</t>
+  </si>
+  <si>
+    <t>Day15 =&gt; Eng Definition updated</t>
   </si>
 </sst>
 </file>
@@ -2557,7 +2560,7 @@
   <dimension ref="B2:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2835,10 +2838,18 @@
       </c>
     </row>
     <row r="21" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="23"/>
+      <c r="B21" s="14">
+        <v>18</v>
+      </c>
+      <c r="C21" s="15">
+        <v>43502</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>684</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2850,7 +2861,7 @@
   <dimension ref="A1:I212"/>
   <sheetViews>
     <sheetView topLeftCell="A199" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G207" sqref="G207:H207"/>
+      <selection activeCell="I201" sqref="I201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.55000000000000004"/>
@@ -6158,6 +6169,10 @@
       <c r="E201" t="s">
         <v>611</v>
       </c>
+      <c r="I201" s="26" t="str">
+        <f>CONCATENATE(D201," ",E201," ",F201)</f>
+        <v xml:space="preserve"> researching companies </v>
+      </c>
     </row>
     <row r="202" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B202" t="s">

</xml_diff>

<commit_message>
TRY N2 Vocab.xlsx -> Day16, Day17 words are added.
</commit_message>
<xml_diff>
--- a/preparing/TRY N2 Vocab.xlsx
+++ b/preparing/TRY N2 Vocab.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="579"/>
@@ -10,12 +10,12 @@
     <sheet name="Data History" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="783">
   <si>
     <t>お知らせ</t>
   </si>
@@ -2076,13 +2076,307 @@
   </si>
   <si>
     <t>Day15 =&gt; Eng Definition updated</t>
+  </si>
+  <si>
+    <t>Day 15</t>
+  </si>
+  <si>
+    <t>Day 16</t>
+  </si>
+  <si>
+    <t>障害</t>
+  </si>
+  <si>
+    <t>終える</t>
+  </si>
+  <si>
+    <t>あふれる</t>
+  </si>
+  <si>
+    <t>業績</t>
+  </si>
+  <si>
+    <t>収入</t>
+  </si>
+  <si>
+    <t>減少</t>
+  </si>
+  <si>
+    <t>貯金額</t>
+  </si>
+  <si>
+    <t>増加</t>
+  </si>
+  <si>
+    <t>真実</t>
+  </si>
+  <si>
+    <t>フリーソフト</t>
+  </si>
+  <si>
+    <t>優れる</t>
+  </si>
+  <si>
+    <t>高熱</t>
+  </si>
+  <si>
+    <t>天候</t>
+  </si>
+  <si>
+    <t>規則</t>
+  </si>
+  <si>
+    <t>一員</t>
+  </si>
+  <si>
+    <t>心構え</t>
+  </si>
+  <si>
+    <t>処理</t>
+  </si>
+  <si>
+    <t>クレーム</t>
+  </si>
+  <si>
+    <t>正当な</t>
+  </si>
+  <si>
+    <t>不快な</t>
+  </si>
+  <si>
+    <t>質</t>
+  </si>
+  <si>
+    <t>追求</t>
+  </si>
+  <si>
+    <t>シンガポール</t>
+  </si>
+  <si>
+    <t>代理</t>
+  </si>
+  <si>
+    <t>しょうがい</t>
+  </si>
+  <si>
+    <t>おえる</t>
+  </si>
+  <si>
+    <t>ぎょうせき</t>
+  </si>
+  <si>
+    <t>しゅうにゅう</t>
+  </si>
+  <si>
+    <t>げんしょう</t>
+  </si>
+  <si>
+    <t>ちょきんがく</t>
+  </si>
+  <si>
+    <t>ぞうか</t>
+  </si>
+  <si>
+    <t>しんじつ</t>
+  </si>
+  <si>
+    <t>すぐれる</t>
+  </si>
+  <si>
+    <t>こうねつ</t>
+  </si>
+  <si>
+    <t>てんこう</t>
+  </si>
+  <si>
+    <t>きそく</t>
+  </si>
+  <si>
+    <t>いちいん</t>
+  </si>
+  <si>
+    <t>こころがまえ</t>
+  </si>
+  <si>
+    <t>くじょう</t>
+  </si>
+  <si>
+    <t>しょり</t>
+  </si>
+  <si>
+    <t>苦情</t>
+  </si>
+  <si>
+    <t>せいとうな</t>
+  </si>
+  <si>
+    <t>ふかいな</t>
+  </si>
+  <si>
+    <t>しつ</t>
+  </si>
+  <si>
+    <t>ついきゅう</t>
+  </si>
+  <si>
+    <t>だいり</t>
+  </si>
+  <si>
+    <t>one's life</t>
+  </si>
+  <si>
+    <t>to end</t>
+  </si>
+  <si>
+    <t>to overflow</t>
+  </si>
+  <si>
+    <t>business performance</t>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
+    <t>reduction (to reduce)</t>
+  </si>
+  <si>
+    <t>savings</t>
+  </si>
+  <si>
+    <t>increase (to increase)</t>
+  </si>
+  <si>
+    <t>reality, truth</t>
+  </si>
+  <si>
+    <t>freeware</t>
+  </si>
+  <si>
+    <t>to be excellent or superior</t>
+  </si>
+  <si>
+    <t>a high fever</t>
+  </si>
+  <si>
+    <t>weather</t>
+  </si>
+  <si>
+    <t>rule</t>
+  </si>
+  <si>
+    <t>one member</t>
+  </si>
+  <si>
+    <t>mental attitude</t>
+  </si>
+  <si>
+    <t>complaint</t>
+  </si>
+  <si>
+    <t>dealing with, handling (to deal with, handle)</t>
+  </si>
+  <si>
+    <t>justified</t>
+  </si>
+  <si>
+    <t>uncomfortable</t>
+  </si>
+  <si>
+    <t>quality</t>
+  </si>
+  <si>
+    <t>pursuit (to pursue)</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>replacement, proxy</t>
+  </si>
+  <si>
+    <t>တစ္ဘ၀လံုး</t>
+  </si>
+  <si>
+    <t>ၿပီးဆံုးေစသည္</t>
+  </si>
+  <si>
+    <t>လွ်ံက်သည္</t>
+  </si>
+  <si>
+    <t>၀င္ေငြ</t>
+  </si>
+  <si>
+    <t>支出</t>
+  </si>
+  <si>
+    <t>ししゅつ</t>
+  </si>
+  <si>
+    <t>expense</t>
+  </si>
+  <si>
+    <t>အသံုးစရိတ္</t>
+  </si>
+  <si>
+    <t>(が)</t>
+  </si>
+  <si>
+    <t>ေလ်ာ့က်သည္</t>
+  </si>
+  <si>
+    <t>စုေငြပမာဏ</t>
+  </si>
+  <si>
+    <t>တိုးပြားသည္</t>
+  </si>
+  <si>
+    <t>မွန္ကန္ေျဖာင့္မတ္ေသာ</t>
+  </si>
+  <si>
+    <t>ရွာေဖြသည္၊ ေလ႔လာလိုက္စားသည္</t>
+  </si>
+  <si>
+    <t>Day 17</t>
+  </si>
+  <si>
+    <t>တစ်ဘဝလုံး</t>
+  </si>
+  <si>
+    <t>ပြီးဆုံးစေသည်</t>
+  </si>
+  <si>
+    <t>လျှံကျသည်</t>
+  </si>
+  <si>
+    <t>၀င်ငွေ</t>
+  </si>
+  <si>
+    <t>အသုံးစရိတ်</t>
+  </si>
+  <si>
+    <t>လျော့ကျသည်</t>
+  </si>
+  <si>
+    <t>စုငွေပမာဏ</t>
+  </si>
+  <si>
+    <t>တိုးပွားသည်</t>
+  </si>
+  <si>
+    <t>မှန်ကန်ဖြောင့်မတ်သော</t>
+  </si>
+  <si>
+    <t>ရှာဖွေသည်၊ လေ့လာလိုက်စားသည်</t>
+  </si>
+  <si>
+    <t>Day16, Day17 added</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2313,7 +2607,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2345,10 +2639,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2380,7 +2673,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2556,14 +2848,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="1" customWidth="1"/>
@@ -2571,7 +2863,7 @@
     <col min="5" max="5" width="51.85546875" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" ht="15.75">
       <c r="B2" s="13" t="s">
         <v>181</v>
       </c>
@@ -2585,7 +2877,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5">
       <c r="B3" s="14">
         <v>0</v>
       </c>
@@ -2599,7 +2891,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="20.25" customHeight="1">
       <c r="B4" s="14">
         <v>1</v>
       </c>
@@ -2613,7 +2905,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="20.25" customHeight="1">
       <c r="B5" s="14">
         <v>2</v>
       </c>
@@ -2627,7 +2919,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="20.25" customHeight="1">
       <c r="B6" s="14">
         <v>3</v>
       </c>
@@ -2641,7 +2933,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" ht="20.25" customHeight="1">
       <c r="B7" s="14">
         <v>4</v>
       </c>
@@ -2655,7 +2947,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" ht="20.25" customHeight="1">
       <c r="B8" s="14">
         <v>5</v>
       </c>
@@ -2669,7 +2961,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" ht="20.25" customHeight="1">
       <c r="B9" s="14">
         <v>6</v>
       </c>
@@ -2683,7 +2975,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" ht="20.25" customHeight="1">
       <c r="B10" s="14">
         <v>7</v>
       </c>
@@ -2697,7 +2989,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" ht="20.25" customHeight="1">
       <c r="B11" s="14">
         <v>8</v>
       </c>
@@ -2711,7 +3003,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" ht="20.25" customHeight="1">
       <c r="B12" s="14">
         <v>9</v>
       </c>
@@ -2725,7 +3017,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" ht="20.25" customHeight="1">
       <c r="B13" s="14">
         <v>10</v>
       </c>
@@ -2739,7 +3031,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" ht="20.25" customHeight="1">
       <c r="B14" s="14">
         <v>11</v>
       </c>
@@ -2753,7 +3045,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" ht="20.25" customHeight="1">
       <c r="B15" s="14">
         <v>12</v>
       </c>
@@ -2767,7 +3059,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" ht="30">
       <c r="B16" s="14">
         <v>13</v>
       </c>
@@ -2781,7 +3073,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" ht="20.25" customHeight="1">
       <c r="B17" s="14">
         <v>14</v>
       </c>
@@ -2795,7 +3087,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" ht="20.25" customHeight="1">
       <c r="B18" s="14">
         <v>15</v>
       </c>
@@ -2809,7 +3101,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" ht="20.25" customHeight="1">
       <c r="B19" s="14">
         <v>16</v>
       </c>
@@ -2823,7 +3115,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" ht="20.25" customHeight="1">
       <c r="B20" s="14">
         <v>17</v>
       </c>
@@ -2837,7 +3129,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" ht="20.25" customHeight="1">
       <c r="B21" s="14">
         <v>18</v>
       </c>
@@ -2850,6 +3142,68 @@
       <c r="E21" s="23" t="s">
         <v>684</v>
       </c>
+    </row>
+    <row r="22" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B22" s="14">
+        <v>19</v>
+      </c>
+      <c r="C22" s="15">
+        <v>43508</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="23"/>
+    </row>
+    <row r="24" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="23"/>
+    </row>
+    <row r="25" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="23"/>
+    </row>
+    <row r="26" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="23"/>
+    </row>
+    <row r="27" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="23"/>
+    </row>
+    <row r="28" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B28" s="14"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="23"/>
+    </row>
+    <row r="29" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B29" s="14"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="23"/>
+    </row>
+    <row r="30" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B30" s="14"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2857,27 +3211,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I212"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I244"/>
   <sheetViews>
-    <sheetView topLeftCell="A199" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I201" sqref="I201"/>
+    <sheetView topLeftCell="A230" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B240" sqref="B240"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="21.75"/>
   <cols>
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" customWidth="1"/>
-    <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" customWidth="1"/>
-    <col min="7" max="7" width="27" style="10" customWidth="1"/>
-    <col min="8" max="8" width="15" style="10" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="31" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="27" style="10" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="10" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="65.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="43.5">
       <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
@@ -2903,7 +3257,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="5" customFormat="1">
       <c r="A2" s="9" t="s">
         <v>133</v>
       </c>
@@ -2916,7 +3270,7 @@
       <c r="H2" s="12"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -2931,7 +3285,7 @@
         <v xml:space="preserve"> notice, announcement </v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -2946,7 +3300,7 @@
         <v xml:space="preserve"> employees, staff, human resources </v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -2961,7 +3315,7 @@
         <v xml:space="preserve"> to seek, to want </v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -2979,7 +3333,7 @@
         <v xml:space="preserve"> opening a store (to open a store) (する)</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -2997,7 +3351,7 @@
         <v xml:space="preserve"> closing a store (to close a store) (する)</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -3012,7 +3366,7 @@
         <v xml:space="preserve"> duty </v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -3030,7 +3384,7 @@
         <v xml:space="preserve"> selling, sales (to sell) (する)</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -3048,7 +3402,7 @@
         <v xml:space="preserve"> cleaning (to clean) (する)</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -3063,7 +3417,7 @@
         <v xml:space="preserve"> nationality </v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -3078,7 +3432,7 @@
         <v xml:space="preserve"> to be motivated </v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -3093,7 +3447,7 @@
         <v xml:space="preserve"> very much welcomed </v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -3111,7 +3465,7 @@
         <v xml:space="preserve"> customer service (to serve customers) (する)</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:9">
       <c r="B15" t="s">
         <v>16</v>
       </c>
@@ -3129,7 +3483,7 @@
         <v xml:space="preserve"> dealing with (to deal with) (する)</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:9">
       <c r="B16" t="s">
         <v>17</v>
       </c>
@@ -3144,7 +3498,7 @@
         <v xml:space="preserve"> can ～: When placed after a noun, this shows that the noun is allowed or possible. </v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:9">
       <c r="B17" t="s">
         <v>18</v>
       </c>
@@ -3159,7 +3513,7 @@
         <v xml:space="preserve"> pay, salary, wage </v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:9">
       <c r="B18" t="s">
         <v>19</v>
       </c>
@@ -3177,7 +3531,7 @@
         <v xml:space="preserve"> consideration (to take into consideration) (する)</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:9">
       <c r="B19" t="s">
         <v>20</v>
       </c>
@@ -3195,7 +3549,7 @@
         <v xml:space="preserve"> roundtrip (to go somewhere roundtrip) (する)</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:9">
       <c r="B20" t="s">
         <v>21</v>
       </c>
@@ -3213,7 +3567,7 @@
         <v xml:space="preserve"> provision (to provide) (する)</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:9">
       <c r="B21" t="s">
         <v>22</v>
       </c>
@@ -3228,7 +3582,7 @@
         <v xml:space="preserve"> prescribed, certain </v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:9">
       <c r="B22" t="s">
         <v>23</v>
       </c>
@@ -3243,7 +3597,7 @@
         <v xml:space="preserve"> document screening </v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:9">
       <c r="B23" t="s">
         <v>24</v>
       </c>
@@ -3261,7 +3615,7 @@
         <v xml:space="preserve"> taking something (to take) (する)</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:9">
       <c r="B24" t="s">
         <v>25</v>
       </c>
@@ -3276,13 +3630,13 @@
         <v xml:space="preserve"> doctor, physician </v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:9">
       <c r="I25" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="5" customFormat="1">
       <c r="A26" s="9" t="s">
         <v>134</v>
       </c>
@@ -3295,10 +3649,10 @@
       <c r="H26" s="12"/>
       <c r="I26" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="B27" t="s">
         <v>26</v>
       </c>
@@ -3313,7 +3667,7 @@
         <v xml:space="preserve"> absence (of a doctor or physician) </v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:9">
       <c r="B28" t="s">
         <v>27</v>
       </c>
@@ -3328,7 +3682,7 @@
         <v xml:space="preserve"> remodeling work </v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:9">
       <c r="B29" t="s">
         <v>28</v>
       </c>
@@ -3343,7 +3697,7 @@
         <v xml:space="preserve"> written to the left </v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:9">
       <c r="B30" t="s">
         <v>29</v>
       </c>
@@ -3358,7 +3712,7 @@
         <v xml:space="preserve"> temporary shop </v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:9">
       <c r="B31" t="s">
         <v>30</v>
       </c>
@@ -3373,7 +3727,7 @@
         <v xml:space="preserve"> promotional/sales campaign </v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:9">
       <c r="B32" t="s">
         <v>31</v>
       </c>
@@ -3388,7 +3742,7 @@
         <v xml:space="preserve"> raw food </v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:9">
       <c r="B33" t="s">
         <v>32</v>
       </c>
@@ -3406,7 +3760,7 @@
         <v xml:space="preserve"> inspection (to inspect) (する)</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:9">
       <c r="B34" t="s">
         <v>33</v>
       </c>
@@ -3421,7 +3775,7 @@
         <v xml:space="preserve"> temporary closing </v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:9">
       <c r="B35" t="s">
         <v>34</v>
       </c>
@@ -3439,7 +3793,7 @@
         <v xml:space="preserve"> closing a business (to close a business) (する)</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:9">
       <c r="B36" t="s">
         <v>35</v>
       </c>
@@ -3454,7 +3808,7 @@
         <v xml:space="preserve"> day and night </v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:9">
       <c r="B37" t="s">
         <v>36</v>
       </c>
@@ -3469,7 +3823,7 @@
         <v xml:space="preserve"> late at night </v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:9">
       <c r="B38" t="s">
         <v>37</v>
       </c>
@@ -3484,7 +3838,7 @@
         <v xml:space="preserve"> presence, existence </v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:9">
       <c r="B39" t="s">
         <v>38</v>
       </c>
@@ -3499,7 +3853,7 @@
         <v xml:space="preserve"> old and young, men and women (i.e. any age or gender) </v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:9">
       <c r="B40" t="s">
         <v>39</v>
       </c>
@@ -3514,7 +3868,7 @@
         <v xml:space="preserve"> occupation, job </v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:9">
       <c r="B41" t="s">
         <v>40</v>
       </c>
@@ -3529,7 +3883,7 @@
         <v xml:space="preserve"> academic background </v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:9">
       <c r="B42" t="s">
         <v>41</v>
       </c>
@@ -3544,13 +3898,13 @@
         <v xml:space="preserve"> interest (in something) </v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:9">
       <c r="I43" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="5" customFormat="1">
       <c r="A44" s="9" t="s">
         <v>135</v>
       </c>
@@ -3563,10 +3917,10 @@
       <c r="H44" s="12"/>
       <c r="I44" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="B45" t="s">
         <v>42</v>
       </c>
@@ -3581,7 +3935,7 @@
         <v xml:space="preserve"> regular, normal </v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:9">
       <c r="B46" t="s">
         <v>43</v>
       </c>
@@ -3605,7 +3959,7 @@
         <v xml:space="preserve"> offering, providing (to offer, provide) (する) ; ကမ်းလှမ်းသည်၊ ထောက်ပံ့သည် ; ကမ္းလွမ္းသည္၊ ေထာက္ပံ႔သည္</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:9">
       <c r="B47" t="s">
         <v>44</v>
       </c>
@@ -3620,7 +3974,7 @@
         <v xml:space="preserve"> corner, section </v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:9">
       <c r="B48" t="s">
         <v>45</v>
       </c>
@@ -3641,7 +3995,7 @@
         <v xml:space="preserve"> surroundings  ; ပတ်ပတ်လည် ; ပတ္ပတ္လည္</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:9">
       <c r="B49" t="s">
         <v>46</v>
       </c>
@@ -3665,7 +4019,7 @@
         <v xml:space="preserve"> shoplifting (to shoplift) (する) ; အလစ်သုတ်သည် ; အလစ္သုတ္သည္</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:9">
       <c r="B50" t="s">
         <v>47</v>
       </c>
@@ -3689,7 +4043,7 @@
         <v xml:space="preserve"> cheating on someone (to cheat on someone) (する) ; (ရည်းစား၊ အိမ်ထောင်) ဖောက်ပြန်သည် ; (ရည္းစား၊ အိမ္ေထာင္) ေဖာက္ျပန္သည္</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:9">
       <c r="B51" t="s">
         <v>48</v>
       </c>
@@ -3704,7 +4058,7 @@
         <v xml:space="preserve"> simple, mere </v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:9">
       <c r="B52" t="s">
         <v>49</v>
       </c>
@@ -3719,10 +4073,10 @@
         <v xml:space="preserve"> counterfeit item, fake </v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:9">
       <c r="I53" s="10"/>
     </row>
-    <row r="54" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:9" s="5" customFormat="1">
       <c r="A54" s="9" t="s">
         <v>137</v>
       </c>
@@ -3735,10 +4089,10 @@
       <c r="H54" s="12"/>
       <c r="I54" s="10" t="str">
         <f>CONCATENATE(D54," ",E54," ",F54)</f>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="B55" t="s">
         <v>50</v>
       </c>
@@ -3753,7 +4107,7 @@
         <v xml:space="preserve"> New Year's party </v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:9">
       <c r="B56" t="s">
         <v>51</v>
       </c>
@@ -3774,7 +4128,7 @@
         <v xml:space="preserve"> clothing  ; အဝတ်အစားမျိုးစုံ ; အ၀တ္အစားမ်ိဳးစံု</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:9">
       <c r="B57" t="s">
         <v>52</v>
       </c>
@@ -3795,7 +4149,7 @@
         <v xml:space="preserve"> to bear in mind  ; (တခုခုလုပ်ဖို့) စိတ်မွေးသည် ; (တခုခုလုပ္ဖို႔) စိတ္ေမြးသည္</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:9">
       <c r="B58" t="s">
         <v>53</v>
       </c>
@@ -3819,7 +4173,7 @@
         <v xml:space="preserve"> request (する) ; တောင်းဆိုမှု ; ေတာင္းဆုိမႈ</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:9">
       <c r="B59" t="s">
         <v>54</v>
       </c>
@@ -3834,10 +4188,10 @@
         <v xml:space="preserve"> allowance: money paid separately from wages or salary </v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:9">
       <c r="I60" s="10"/>
     </row>
-    <row r="61" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:9" s="5" customFormat="1">
       <c r="A61" s="9" t="s">
         <v>188</v>
       </c>
@@ -3850,10 +4204,10 @@
       <c r="H61" s="12"/>
       <c r="I61" s="10" t="str">
         <f>CONCATENATE(D61," ",E61," ",F61)</f>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="B62" t="s">
         <v>55</v>
       </c>
@@ -3871,7 +4225,7 @@
         <v xml:space="preserve"> returning an item (to return an item) (する)</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:9">
       <c r="B63" t="s">
         <v>56</v>
       </c>
@@ -3895,7 +4249,7 @@
         <v xml:space="preserve"> statement (to state) (する) ; ထုတ်ဖော်ပြောဆိုသည် ; ထုတ္ေဖာ္ေျပာဆိုသည္</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:9">
       <c r="B64" t="s">
         <v>57</v>
       </c>
@@ -3910,7 +4264,7 @@
         <v xml:space="preserve"> clear or rainy weather </v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:9">
       <c r="B65" t="s">
         <v>58</v>
       </c>
@@ -3925,7 +4279,7 @@
         <v xml:space="preserve"> to summarize (one's opinion) </v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:9">
       <c r="B66" t="s">
         <v>59</v>
       </c>
@@ -3943,7 +4297,7 @@
         <v xml:space="preserve"> contribution, donation (to contribute, donate) (する)</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:9">
       <c r="B67" t="s">
         <v>60</v>
       </c>
@@ -3958,7 +4312,7 @@
         <v xml:space="preserve"> environmental pollution </v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:9">
       <c r="B68" t="s">
         <v>61</v>
       </c>
@@ -3976,7 +4330,7 @@
         <v xml:space="preserve"> pollution (to pollute) (する)</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:9">
       <c r="B69" t="s">
         <v>62</v>
       </c>
@@ -3991,7 +4345,7 @@
         <v xml:space="preserve"> good luck, fortune </v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:9">
       <c r="B70" t="s">
         <v>199</v>
       </c>
@@ -4006,7 +4360,7 @@
         <v xml:space="preserve"> wind power </v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:9">
       <c r="B71" t="s">
         <v>200</v>
       </c>
@@ -4021,7 +4375,7 @@
         <v xml:space="preserve"> natural energy </v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:9">
       <c r="B72" t="s">
         <v>203</v>
       </c>
@@ -4039,11 +4393,11 @@
         <v xml:space="preserve"> losing a job (to lose a job) (する)</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:9">
       <c r="F73" s="1"/>
       <c r="I73" s="10"/>
     </row>
-    <row r="74" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:9" s="5" customFormat="1">
       <c r="A74" s="9" t="s">
         <v>276</v>
       </c>
@@ -4056,10 +4410,10 @@
       <c r="H74" s="12"/>
       <c r="I74" s="10" t="str">
         <f>CONCATENATE(D74," ",E74," ",F74)</f>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
       <c r="B75" t="s">
         <v>218</v>
       </c>
@@ -4077,7 +4431,7 @@
         <v xml:space="preserve"> loss of an object (to lose something) (する)</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:9">
       <c r="B76" t="s">
         <v>219</v>
       </c>
@@ -4098,7 +4452,7 @@
         <v xml:space="preserve"> taking off or landing  ; ထွက်ခွာ ဆင်းသက်ခြင်း ; ထြက္ခြာ ဆင္းသက္ျခင္း</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:9">
       <c r="B77" t="s">
         <v>220</v>
       </c>
@@ -4119,7 +4473,7 @@
         <v xml:space="preserve"> fire (disaster)  ; မီးဘေး ; မီးေဘး</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:9">
       <c r="B78" t="s">
         <v>221</v>
       </c>
@@ -4134,7 +4488,7 @@
         <v xml:space="preserve"> rainy weather </v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:9">
       <c r="B79" t="s">
         <v>222</v>
       </c>
@@ -4149,7 +4503,7 @@
         <v xml:space="preserve"> indoors </v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:9">
       <c r="B80" t="s">
         <v>223</v>
       </c>
@@ -4164,7 +4518,7 @@
         <v xml:space="preserve"> password </v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:9">
       <c r="B81" t="s">
         <v>224</v>
       </c>
@@ -4182,7 +4536,7 @@
         <v xml:space="preserve"> wearing (to wear) (する) (use in writing)</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:9">
       <c r="B82" t="s">
         <v>225</v>
       </c>
@@ -4197,7 +4551,7 @@
         <v xml:space="preserve"> emergency button </v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:9">
       <c r="B83" t="s">
         <v>226</v>
       </c>
@@ -4212,7 +4566,7 @@
         <v xml:space="preserve"> deadline </v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:9">
       <c r="B84" t="s">
         <v>227</v>
       </c>
@@ -4236,10 +4590,10 @@
         <v xml:space="preserve"> compliance (to comply) (する) ; မဖြစ်မနေ ကာကွယ်သည် ; မျဖစ္မေန ကာကြယ္သည္</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:9">
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:9" s="5" customFormat="1">
       <c r="A86" s="9" t="s">
         <v>277</v>
       </c>
@@ -4252,10 +4606,10 @@
       <c r="H86" s="12"/>
       <c r="I86" s="10" t="str">
         <f>CONCATENATE(D86," ",E86," ",F86)</f>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
       <c r="B87" t="s">
         <v>228</v>
       </c>
@@ -4270,7 +4624,7 @@
         <v xml:space="preserve"> request form, application form (入学) </v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:9">
       <c r="B88" t="s">
         <v>229</v>
       </c>
@@ -4285,7 +4639,7 @@
         <v xml:space="preserve"> counter, desk, liaison </v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:9">
       <c r="B89" t="s">
         <v>230</v>
       </c>
@@ -4300,7 +4654,7 @@
         <v xml:space="preserve"> writing implement (pencil, eraser, book,etc..) </v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:9">
       <c r="B90" t="s">
         <v>231</v>
       </c>
@@ -4315,7 +4669,7 @@
         <v xml:space="preserve"> poolside </v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:9">
       <c r="B91" t="s">
         <v>288</v>
       </c>
@@ -4342,10 +4696,10 @@
         <v>(ゴミを) 1.separation, 2.discernment, judgment (する) ; သီးသန့်ခွဲသည်၊ အမြော်အမြင်ရှိသည် ; သီးသန္႔ခြဲသည္၊ အေျမာ္အျမင္ရွိသည္</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:9">
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:9" s="5" customFormat="1">
       <c r="A93" s="9" t="s">
         <v>286</v>
       </c>
@@ -4358,10 +4712,10 @@
       <c r="H93" s="12"/>
       <c r="I93" s="10" t="str">
         <f>CONCATENATE(D93," ",E93," ",F93)</f>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
       <c r="B94" t="s">
         <v>232</v>
       </c>
@@ -4379,7 +4733,7 @@
         <v xml:space="preserve"> change of post (to change one's post) (する)</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:9">
       <c r="B95" t="s">
         <v>233</v>
       </c>
@@ -4394,7 +4748,7 @@
         <v xml:space="preserve"> to appoint, assign, order </v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:9">
       <c r="B96" t="s">
         <v>234</v>
       </c>
@@ -4409,7 +4763,7 @@
         <v xml:space="preserve"> gene </v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:9">
       <c r="B97" t="s">
         <v>235</v>
       </c>
@@ -4424,7 +4778,7 @@
         <v xml:space="preserve"> welcome party </v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:9">
       <c r="B98" t="s">
         <v>236</v>
       </c>
@@ -4439,7 +4793,7 @@
         <v xml:space="preserve"> to review, reconsider </v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:9">
       <c r="B99" t="s">
         <v>237</v>
       </c>
@@ -4454,7 +4808,7 @@
         <v xml:space="preserve"> spice </v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:9">
       <c r="B100" t="s">
         <v>238</v>
       </c>
@@ -4469,7 +4823,7 @@
         <v xml:space="preserve"> microwave oven </v>
       </c>
     </row>
-    <row r="102" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:9" s="5" customFormat="1">
       <c r="A102" s="9" t="s">
         <v>302</v>
       </c>
@@ -4482,10 +4836,10 @@
       <c r="H102" s="12"/>
       <c r="I102" s="10" t="str">
         <f>CONCATENATE(D102," ",E102," ",F102)</f>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
       <c r="B103" t="s">
         <v>303</v>
       </c>
@@ -4500,7 +4854,7 @@
         <v xml:space="preserve"> jacket </v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:9">
       <c r="B104" t="s">
         <v>304</v>
       </c>
@@ -4518,7 +4872,7 @@
         <v xml:space="preserve"> arrival, receipt (to arrive, receive) (する)</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:9">
       <c r="B105" t="s">
         <v>305</v>
       </c>
@@ -4533,7 +4887,7 @@
         <v xml:space="preserve"> celebrity </v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:9">
       <c r="B106" t="s">
         <v>306</v>
       </c>
@@ -4548,7 +4902,7 @@
         <v xml:space="preserve"> instructor, teacher </v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:9">
       <c r="B107" t="s">
         <v>307</v>
       </c>
@@ -4563,7 +4917,7 @@
         <v xml:space="preserve"> Southeast Asia </v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:9">
       <c r="B108" t="s">
         <v>308</v>
       </c>
@@ -4584,7 +4938,7 @@
         <v xml:space="preserve"> streamlining  ; တွက်ခြေကိုက်အောင် လုပ်သည် ; တြက္ေျခကိုက္ေအာင္ လုပ္သည္</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:9">
       <c r="B109" t="s">
         <v>309</v>
       </c>
@@ -4600,7 +4954,7 @@
         <v xml:space="preserve"> many </v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:9">
       <c r="B110" t="s">
         <v>310</v>
       </c>
@@ -4621,7 +4975,7 @@
         <v xml:space="preserve"> employee  ; လုပ်ငန်းခွင်ထဲက အလုပ်သမား ; လုပ္ငန္းခြင္ထဲက အလုပ္သမား</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:9">
       <c r="B111" t="s">
         <v>311</v>
       </c>
@@ -4645,7 +4999,7 @@
         <v xml:space="preserve"> dismissal (to dismiss) (する) ; အလုပ်ထုတ်ခြင်း၊ ထွက်ခိုင်းခြင်း ; အလုပ္ထုတ္ျခင္း၊ ထြက္ခိုင္းျခင္း</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:9">
       <c r="B112" t="s">
         <v>312</v>
       </c>
@@ -4661,7 +5015,7 @@
         <v xml:space="preserve"> to accept, recognize </v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:9">
       <c r="B113" t="s">
         <v>313</v>
       </c>
@@ -4685,7 +5039,7 @@
         <v xml:space="preserve"> respect (to respect) (する) ; လေးစားအားကျခြင်း ; ေလးစားအားက်ျခင္း</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:9">
       <c r="B114" t="s">
         <v>314</v>
       </c>
@@ -4701,7 +5055,7 @@
         <v xml:space="preserve"> coast </v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:9">
       <c r="B115" t="s">
         <v>7</v>
       </c>
@@ -4720,7 +5074,7 @@
         <v xml:space="preserve"> cleaning (to clean) (する)</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:9">
       <c r="B116" t="s">
         <v>315</v>
       </c>
@@ -4744,7 +5098,7 @@
         <v xml:space="preserve"> consent (to consent) (する) ; သဘောတူလက်ခံခြင်း ; သေဘာတူလက္ခံျခင္း</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:9">
       <c r="B117" t="s">
         <v>316</v>
       </c>
@@ -4760,7 +5114,7 @@
         <v xml:space="preserve"> grandparents </v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:9">
       <c r="B118" t="s">
         <v>317</v>
       </c>
@@ -4781,7 +5135,7 @@
         <v xml:space="preserve"> sleeping  ; အိပ်ပျော်ခြင်း ; အိပ္ေပ်ာ္ျခင္း</v>
       </c>
     </row>
-    <row r="120" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:9" s="5" customFormat="1">
       <c r="A120" s="9" t="s">
         <v>361</v>
       </c>
@@ -4794,10 +5148,10 @@
       <c r="H120" s="12"/>
       <c r="I120" s="10" t="str">
         <f>CONCATENATE(D120," ",E120," ",F120)</f>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v/>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
       <c r="B121" t="s">
         <v>1</v>
       </c>
@@ -4812,7 +5166,7 @@
         <v xml:space="preserve"> employees, staff, human resources </v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:9">
       <c r="B122" t="s">
         <v>362</v>
       </c>
@@ -4836,7 +5190,7 @@
         <v xml:space="preserve"> getting, securing (to get, secure) (する) ; ရအောင်ယူသည်၊ (နေရာ)ဦးသည် ; ရေအာင္ယူသည္၊ (ေနရာ)ဦးသည္</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:9">
       <c r="B123" t="s">
         <v>363</v>
       </c>
@@ -4851,7 +5205,7 @@
         <v xml:space="preserve"> small- and medium-sized enterprises (SMEs) </v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:9">
       <c r="B124" t="s">
         <v>364</v>
       </c>
@@ -4866,7 +5220,7 @@
         <v xml:space="preserve"> crime </v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:9">
       <c r="B125" t="s">
         <v>365</v>
       </c>
@@ -4884,7 +5238,7 @@
         <v xml:space="preserve"> prevention (to prevent) (する)</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:9">
       <c r="B126" t="s">
         <v>366</v>
       </c>
@@ -4899,7 +5253,7 @@
         <v xml:space="preserve"> South America </v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:9">
       <c r="B127" t="s">
         <v>367</v>
       </c>
@@ -4914,7 +5268,7 @@
         <v xml:space="preserve"> to learn, acquire; to put on </v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="34.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:9" ht="34.5">
       <c r="B128" t="s">
         <v>368</v>
       </c>
@@ -4926,11 +5280,10 @@
       </c>
       <c r="I128" s="10" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> bilateral (literally "between both 
-countries")  </v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v xml:space="preserve"> bilateral (literally "between both countries")  </v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" s="5" customFormat="1">
       <c r="A130" s="9" t="s">
         <v>395</v>
       </c>
@@ -4943,10 +5296,10 @@
       <c r="H130" s="12"/>
       <c r="I130" s="10" t="str">
         <f>CONCATENATE(D130," ",E130," ",F130)</f>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v/>
+      </c>
+    </row>
+    <row r="131" spans="1:9">
       <c r="B131" t="s">
         <v>369</v>
       </c>
@@ -4967,7 +5320,7 @@
         <v xml:space="preserve"> active, lively, vigorous  ; သွက်လက်ဖြတ်လတ်သော ; သြက္လက္ျဖတ္လတ္ေသာ</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:9">
       <c r="B132" t="s">
         <v>370</v>
       </c>
@@ -4991,7 +5344,7 @@
         <v xml:space="preserve"> talking back (to talk back) (する) ; ပြန်ခံပြောသည်၊ ဘုကလန့်လုပ်သည် ; ျပန္ခံေျပာသည္၊ ဘုကလန္႔လုပ္သည္</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:9">
       <c r="B133" t="s">
         <v>371</v>
       </c>
@@ -5012,7 +5365,7 @@
         <v xml:space="preserve"> not ～ at all  ; လုံးဝ~မ~ဘူး ; လံုး၀~မ~ဘူး</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:9">
       <c r="B134" t="s">
         <v>372</v>
       </c>
@@ -5036,7 +5389,7 @@
         <v xml:space="preserve"> rebellion (to rebel) (する) ; မနာခံခြင်း၊ ပုန်ကန်ခြင်း ; မနာခံျခင္း၊ ပုန္ကန္ျခင္း</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:9">
       <c r="B135" t="s">
         <v>373</v>
       </c>
@@ -5054,7 +5407,7 @@
         <v xml:space="preserve"> lost love (to lose a lover) (する)</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:9">
       <c r="B136" t="s">
         <v>374</v>
       </c>
@@ -5075,7 +5428,7 @@
         <v xml:space="preserve"> with all one's might  ; အစွမ်းကုန် ; အစြမ္းကုန္</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:9">
       <c r="B137" t="s">
         <v>375</v>
       </c>
@@ -5093,7 +5446,7 @@
         <v xml:space="preserve"> style (to be stylish) (する)</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:9">
       <c r="B138" t="s">
         <v>376</v>
       </c>
@@ -5108,7 +5461,7 @@
         <v xml:space="preserve"> attitude </v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:9">
       <c r="B139" t="s">
         <v>377</v>
       </c>
@@ -5123,7 +5476,7 @@
         <v xml:space="preserve"> point </v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:9">
       <c r="B140" t="s">
         <v>401</v>
       </c>
@@ -5138,7 +5491,7 @@
         <v xml:space="preserve"> religion </v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:9">
       <c r="B141" t="s">
         <v>402</v>
       </c>
@@ -5153,7 +5506,7 @@
         <v xml:space="preserve"> shop </v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:9">
       <c r="B142" t="s">
         <v>403</v>
       </c>
@@ -5171,7 +5524,7 @@
         <v xml:space="preserve"> setting up, establishment (する)</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:9">
       <c r="B143" t="s">
         <v>404</v>
       </c>
@@ -5186,7 +5539,7 @@
         <v xml:space="preserve"> surrounding, nearby </v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:9">
       <c r="B144" t="s">
         <v>405</v>
       </c>
@@ -5201,7 +5554,7 @@
         <v xml:space="preserve"> marketing </v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:9">
       <c r="B145" t="s">
         <v>406</v>
       </c>
@@ -5222,7 +5575,7 @@
         <v xml:space="preserve"> essential, vital  ; မရှိမဖြစ်သော ; မရွိမျဖစ္ေသာ</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:9">
       <c r="B146" t="s">
         <v>407</v>
       </c>
@@ -5243,7 +5596,7 @@
         <v xml:space="preserve"> cost performance  ; ကုန်ကျမှု ပြန်ရမှု နှိုင်းယှဉ်ချက် ; ကုန္က်မႈ ျပန္ရမႈ ႏိႈင္းယွဥ္ခ်က္</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:9">
       <c r="B147" t="s">
         <v>408</v>
       </c>
@@ -5264,7 +5617,7 @@
         <v xml:space="preserve"> a strong yen  ; ယန်းဈေးခိုင်မာမှု ; ယန္းေစ်းခိုင္မာမႈ</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:9">
       <c r="B148" t="s">
         <v>409</v>
       </c>
@@ -5279,7 +5632,7 @@
         <v xml:space="preserve"> course, lecture </v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:9">
       <c r="B149" t="s">
         <v>410</v>
       </c>
@@ -5294,7 +5647,7 @@
         <v xml:space="preserve"> knowledge </v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:9">
       <c r="B150" t="s">
         <v>411</v>
       </c>
@@ -5315,7 +5668,7 @@
         <v xml:space="preserve"> a higher-level school to enter  ; တက်ရမယ့် ပိုမြင့်တဲ့ကျောင်း ; တက္ရမယ့္ ပိုျမင့္တဲ႔ေက်ာင္း</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:9">
       <c r="B151" t="s">
         <v>412</v>
       </c>
@@ -5336,7 +5689,7 @@
         <v xml:space="preserve"> job-finding rate, employment rate  ; အလုပ်ဝင်နှုန်း ; အလုပ္၀င္ႏႈန္း</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:9">
       <c r="B152" t="s">
         <v>413</v>
       </c>
@@ -5357,7 +5710,7 @@
         <v xml:space="preserve"> agriculture  ; စိုက်ပျိုးရေး ; စိုက္ပ်ိဳးေရး</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:9">
       <c r="B153" t="s">
         <v>414</v>
       </c>
@@ -5378,7 +5731,7 @@
         <v xml:space="preserve"> farming village  ; စိုက်ပျိုးရေးလုပ်တဲ့ရွာ ; စိုက္ပ်ိဳးေရးလုပ္တဲ႔ရြာ</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:9">
       <c r="B154" t="s">
         <v>415</v>
       </c>
@@ -5399,7 +5752,7 @@
         <v xml:space="preserve"> terrain  ; မြေအနေအထား ; ေျမအေနအထား</v>
       </c>
     </row>
-    <row r="156" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:9" s="5" customFormat="1">
       <c r="A156" s="9" t="s">
         <v>534</v>
       </c>
@@ -5412,10 +5765,10 @@
       <c r="H156" s="12"/>
       <c r="I156" s="10" t="str">
         <f>CONCATENATE(D156," ",E156," ",F156)</f>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v/>
+      </c>
+    </row>
+    <row r="157" spans="1:9">
       <c r="B157" t="s">
         <v>416</v>
       </c>
@@ -5430,7 +5783,7 @@
         <v xml:space="preserve"> leader </v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:9">
       <c r="B158" s="21" t="s">
         <v>591</v>
       </c>
@@ -5445,7 +5798,7 @@
         <v xml:space="preserve"> digital voice recorder </v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:9">
       <c r="B159" t="s">
         <v>417</v>
       </c>
@@ -5460,7 +5813,7 @@
         <v xml:space="preserve"> small type </v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:9">
       <c r="B160" t="s">
         <v>418</v>
       </c>
@@ -5478,7 +5831,7 @@
         <v xml:space="preserve"> recording sound (to record sound) (する)</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:9">
       <c r="B161" t="s">
         <v>419</v>
       </c>
@@ -5493,7 +5846,7 @@
         <v xml:space="preserve"> possible </v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:9">
       <c r="B162" t="s">
         <v>420</v>
       </c>
@@ -5517,7 +5870,7 @@
         <v xml:space="preserve"> display, exhibition (する) ; ခင်းကျင်းပြသခြင်း ; ခင္းက်င္းျပသျခင္း</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:9">
       <c r="B163" t="s">
         <v>421</v>
       </c>
@@ -5532,7 +5885,7 @@
         <v xml:space="preserve"> old type </v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:9">
       <c r="B164" t="s">
         <v>422</v>
       </c>
@@ -5550,7 +5903,7 @@
         <v xml:space="preserve"> enlargement (to enlarge) (する)</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:9">
       <c r="B165" t="s">
         <v>423</v>
       </c>
@@ -5568,7 +5921,7 @@
         <v xml:space="preserve"> trying, challenging oneself (する)</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:9">
       <c r="B166" t="s">
         <v>424</v>
       </c>
@@ -5583,7 +5936,7 @@
         <v xml:space="preserve"> full effort </v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:9">
       <c r="B167" t="s">
         <v>427</v>
       </c>
@@ -5604,7 +5957,7 @@
         <v xml:space="preserve"> to become familiar with  ; ရင်းနှီးကျွမ်းဝင်သည် ; ရင္းႏွီးကၽြမ္း၀င္သည္</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:9">
       <c r="B168" t="s">
         <v>428</v>
       </c>
@@ -5625,7 +5978,7 @@
         <v xml:space="preserve"> consideration (for others), care  ; အလိုက်သိတတ်နားလည်သော ; အလိုက္သိတတ္နားလည္ေသာ</v>
       </c>
     </row>
-    <row r="170" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:9" s="5" customFormat="1">
       <c r="A170" s="9" t="s">
         <v>556</v>
       </c>
@@ -5638,10 +5991,10 @@
       <c r="H170" s="12"/>
       <c r="I170" s="10" t="str">
         <f>CONCATENATE(D170," ",E170," ",F170)</f>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v/>
+      </c>
+    </row>
+    <row r="171" spans="1:9">
       <c r="B171" t="s">
         <v>429</v>
       </c>
@@ -5662,7 +6015,7 @@
         <v xml:space="preserve"> organization  ; အဖွဲ့အစည်း(အကြီး) ; အဖြဲ႔အစည္း(အႀကီး)</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:9">
       <c r="B172" s="21" t="s">
         <v>590</v>
       </c>
@@ -5677,7 +6030,7 @@
         <v xml:space="preserve"> traditional performing arts </v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:9">
       <c r="B173" t="s">
         <v>430</v>
       </c>
@@ -5698,7 +6051,7 @@
         <v xml:space="preserve"> symposium  ; ခေါင်းစဉ်တစ်ခုနှင့် ပတ်သက်သော သီးသန့်ဆွေးနွေးပွဲ ; ေခါင္းစဥ္တစ္ခုႏွင့္ ပတ္သက္ေသာ သီးသန္႔ေဆြးေႏြးပြဲ</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:9">
       <c r="B174" t="s">
         <v>431</v>
       </c>
@@ -5719,7 +6072,7 @@
         <v xml:space="preserve"> consensus opinion  ; အများရဲ့သဘောအကြံဉာဏ် ; အမ်ားရဲ႕သေဘာအႀကံဉာဏ္</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:9">
       <c r="B175" t="s">
         <v>432</v>
       </c>
@@ -5740,7 +6093,7 @@
         <v xml:space="preserve"> model  ; စံပြပုံစံ ; စံျပပံုစံ</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:9">
       <c r="B176" t="s">
         <v>433</v>
       </c>
@@ -5758,7 +6111,7 @@
         <v xml:space="preserve"> engineer (kana)</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:9">
       <c r="B177" t="s">
         <v>434</v>
       </c>
@@ -5779,7 +6132,7 @@
         <v xml:space="preserve"> assumption  ; ကြိုတင်ယူဆချက် ; ႀကိဳတင္ယူဆခ်က္</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:9">
       <c r="B178" t="s">
         <v>435</v>
       </c>
@@ -5803,7 +6156,7 @@
         <v xml:space="preserve"> association; society; acquaintance (する) ; ၁။ပေါင်းသင်းဆက်ဆံသည်၊ ၂။ Date လုပ်သည် ; ၁။ေပါင္းသင္းဆက္ဆံသည္၊ ၂။ Date လုပ္သည္</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:9">
       <c r="B179" t="s">
         <v>436</v>
       </c>
@@ -5818,7 +6171,7 @@
         <v xml:space="preserve"> profit </v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:9">
       <c r="B180" t="s">
         <v>437</v>
       </c>
@@ -5833,7 +6186,7 @@
         <v xml:space="preserve"> economic activity </v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:9">
       <c r="B181" t="s">
         <v>438</v>
       </c>
@@ -5851,7 +6204,7 @@
         <v xml:space="preserve"> hire, use; adoption; acceptance (する)</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:9">
       <c r="B182" t="s">
         <v>439</v>
       </c>
@@ -5866,7 +6219,7 @@
         <v xml:space="preserve"> captain </v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:9">
       <c r="B183" t="s">
         <v>440</v>
       </c>
@@ -5881,7 +6234,7 @@
         <v xml:space="preserve"> all together </v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:9">
       <c r="B184" t="s">
         <v>557</v>
       </c>
@@ -5902,7 +6255,7 @@
         <v xml:space="preserve"> with all one's strength  ; စိတ်အားရတဲ့အထိ ; စိတ္အားရတဲ႔အထိ</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:9">
       <c r="B185" t="s">
         <v>558</v>
       </c>
@@ -5917,7 +6270,7 @@
         <v xml:space="preserve"> coach, manager </v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:9">
       <c r="B186" t="s">
         <v>559</v>
       </c>
@@ -5941,7 +6294,7 @@
         <v xml:space="preserve"> a letter (to submit a letter) (する) ; ကိုယ့်ထင်မြင်ချက်ကို ဖော်ပြတဲ့စာ ; ကိုယ့္ထင္ျမင္ခ်က္ကို ေဖာ္ျပတဲ႔စာ</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:9">
       <c r="B187" t="s">
         <v>560</v>
       </c>
@@ -5956,7 +6309,7 @@
         <v xml:space="preserve"> insect </v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:9">
       <c r="B188" t="s">
         <v>561</v>
       </c>
@@ -5972,7 +6325,7 @@
         <v xml:space="preserve"> Souvenirs Entomologiques (a book name written by Jean-Henri Fabre) </v>
       </c>
     </row>
-    <row r="190" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:9" s="5" customFormat="1">
       <c r="A190" s="9" t="s">
         <v>595</v>
       </c>
@@ -5985,10 +6338,10 @@
       <c r="H190" s="12"/>
       <c r="I190" s="10" t="str">
         <f>CONCATENATE(D190," ",E190," ",F190)</f>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v/>
+      </c>
+    </row>
+    <row r="191" spans="1:9">
       <c r="B191" t="s">
         <v>596</v>
       </c>
@@ -6012,7 +6365,7 @@
         <v xml:space="preserve"> taking a post (to take a post for high position) (する) ; ရာထူးရယူသည် ; ရာထူးရယူသည္</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:9">
       <c r="B192" t="s">
         <v>597</v>
       </c>
@@ -6036,7 +6389,7 @@
         <v xml:space="preserve"> growth (to grow) (する) ; ဖွံ့ဖြိုးတိုးတက်သည် ; ဖြံ႔ၿဖိဳးတိုးတက္သည္</v>
       </c>
     </row>
-    <row r="193" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:9">
       <c r="B193" t="s">
         <v>598</v>
       </c>
@@ -6051,7 +6404,7 @@
         <v xml:space="preserve"> Nobel Prize </v>
       </c>
     </row>
-    <row r="194" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:9">
       <c r="B194" t="s">
         <v>599</v>
       </c>
@@ -6075,7 +6428,7 @@
         <v xml:space="preserve"> receiving a prize (to receive a prize) (する) ; ဆုလက်ခံရရှိသည် ; ဆုလက္ခံရရွိသည္</v>
       </c>
     </row>
-    <row r="195" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:9">
       <c r="B195" t="s">
         <v>600</v>
       </c>
@@ -6090,7 +6443,7 @@
         <v xml:space="preserve"> test taker </v>
       </c>
     </row>
-    <row r="196" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:9">
       <c r="B196" t="s">
         <v>601</v>
       </c>
@@ -6111,7 +6464,7 @@
         <v xml:space="preserve"> involving the whole area/region  ; နယ်မြေတစ်ခုလုံးပါဝင်မှု ; နယ္ေျမတစ္ခုလံုးပါ၀င္မႈ</v>
       </c>
     </row>
-    <row r="197" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:9">
       <c r="B197" t="s">
         <v>602</v>
       </c>
@@ -6135,7 +6488,7 @@
         <v xml:space="preserve"> opening a port (to open a port) (する) ; (လေယာဉ်၊ သင်္ဘော၊…)ဆိပ်ဖွင့်လှစ်သည် ; (ေလယာဥ္၊ သေဘၤာ၊…)ဆိပ္ဖြင့္လွစ္သည္</v>
       </c>
     </row>
-    <row r="198" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:9">
       <c r="B198" t="s">
         <v>603</v>
       </c>
@@ -6159,7 +6512,23 @@
         <v>(1,2,…)+ ～anniversary  ; ～နှစ်ပတ်လည် ; ～ႏွစ္ပတ္လည္</v>
       </c>
     </row>
-    <row r="201" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:9" s="5" customFormat="1">
+      <c r="A200" s="9" t="s">
+        <v>685</v>
+      </c>
+      <c r="B200" s="6"/>
+      <c r="C200" s="6"/>
+      <c r="D200" s="7"/>
+      <c r="E200" s="6"/>
+      <c r="F200" s="7"/>
+      <c r="G200" s="12"/>
+      <c r="H200" s="12"/>
+      <c r="I200" s="10" t="str">
+        <f>CONCATENATE(D200," ",E200," ",F200)</f>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="201" spans="1:9">
       <c r="B201" t="s">
         <v>604</v>
       </c>
@@ -6174,7 +6543,7 @@
         <v xml:space="preserve"> researching companies </v>
       </c>
     </row>
-    <row r="202" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:9">
       <c r="B202" t="s">
         <v>636</v>
       </c>
@@ -6198,7 +6567,7 @@
         <v xml:space="preserve"> pastry chef (kana) ; မုန့်အချိုပွဲလုပ်တဲ့သူ ; မုန္႔အခ်ိဳပြဲလုပ္တဲ႔သူ</v>
       </c>
     </row>
-    <row r="203" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:9">
       <c r="B203" t="s">
         <v>637</v>
       </c>
@@ -6216,7 +6585,7 @@
         <v xml:space="preserve"> contest (kana)</v>
       </c>
     </row>
-    <row r="204" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:9">
       <c r="B204" t="s">
         <v>638</v>
       </c>
@@ -6240,7 +6609,7 @@
         <v xml:space="preserve"> entry (to enter) (する) ; တက်ရောက်သည် ; တက္ေရာက္သည္</v>
       </c>
     </row>
-    <row r="205" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:9">
       <c r="B205" t="s">
         <v>639</v>
       </c>
@@ -6255,7 +6624,7 @@
         <v xml:space="preserve"> three-star restaurant </v>
       </c>
     </row>
-    <row r="206" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:9">
       <c r="B206" t="s">
         <v>640</v>
       </c>
@@ -6276,7 +6645,7 @@
         <v xml:space="preserve"> to handle  ; ကိုင္တြယ္သည္ ; ကိုင္တြယ္သည္</v>
       </c>
     </row>
-    <row r="207" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:9">
       <c r="B207" t="s">
         <v>641</v>
       </c>
@@ -6297,7 +6666,7 @@
         <v xml:space="preserve"> deadline  ; သတ်မှတ်နောက်ဆုံးနေ့ရက် ; သတ္မွတ္ေနာက္ဆံုးေန႔ရက္</v>
       </c>
     </row>
-    <row r="208" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:9">
       <c r="B208" t="s">
         <v>642</v>
       </c>
@@ -6318,7 +6687,7 @@
         <v xml:space="preserve"> to meet, be in time  ; အချိန်မီ ဖြစ်စေသည် ; အခ်ိန္မီ ျဖစ္ေစသည္</v>
       </c>
     </row>
-    <row r="209" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:9">
       <c r="B209" t="s">
         <v>643</v>
       </c>
@@ -6339,7 +6708,7 @@
         <v xml:space="preserve"> pride  ; ဂုဏ်၊ ဂုဏ်ယူခြင်း ; ဂုဏ္၊ ဂုဏ္ယူျခင္း</v>
       </c>
     </row>
-    <row r="210" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:9">
       <c r="B210" t="s">
         <v>644</v>
       </c>
@@ -6360,7 +6729,7 @@
         <v xml:space="preserve"> to make a full effort  ; အင်အားစိုက်ထုတ်ကြိုးပမ်းသည် ; အင္အားစိုက္ထုတ္ႀကိဳးပမ္းသည္</v>
       </c>
     </row>
-    <row r="211" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:9">
       <c r="B211" t="s">
         <v>645</v>
       </c>
@@ -6375,7 +6744,7 @@
         <v xml:space="preserve"> tax </v>
       </c>
     </row>
-    <row r="212" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:9">
       <c r="B212" t="s">
         <v>646</v>
       </c>
@@ -6394,6 +6763,501 @@
       <c r="I212" s="10" t="str">
         <f t="shared" ref="I212" si="23">CONCATENATE(D212," ",E212," ",F212, " ; ",G212," ; ", H212)</f>
         <v xml:space="preserve"> to contest, dispute   ; ယှဉ်ပြိုင်သည်၊ စကားများသည် ; ယွဥ္ၿပိဳင္သည္၊ စကားမ်ားသည္</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" s="5" customFormat="1">
+      <c r="A214" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="B214" s="6"/>
+      <c r="C214" s="6"/>
+      <c r="D214" s="7"/>
+      <c r="E214" s="6"/>
+      <c r="F214" s="7"/>
+      <c r="G214" s="12"/>
+      <c r="H214" s="12"/>
+      <c r="I214" s="10" t="str">
+        <f>CONCATENATE(D214," ",E214," ",F214)</f>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="215" spans="1:9">
+      <c r="B215" t="s">
+        <v>687</v>
+      </c>
+      <c r="C215" t="s">
+        <v>711</v>
+      </c>
+      <c r="E215" t="s">
+        <v>733</v>
+      </c>
+      <c r="G215" s="10" t="s">
+        <v>772</v>
+      </c>
+      <c r="H215" s="10" t="s">
+        <v>757</v>
+      </c>
+      <c r="I215" s="10" t="str">
+        <f t="shared" ref="I215:I217" si="24">CONCATENATE(D215," ",E215," ",F215, " ; ",G215," ; ", H215)</f>
+        <v xml:space="preserve"> one's life  ; တစ်ဘဝလုံး ; တစ္ဘ၀လံုး</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9">
+      <c r="B216" t="s">
+        <v>688</v>
+      </c>
+      <c r="C216" t="s">
+        <v>712</v>
+      </c>
+      <c r="E216" t="s">
+        <v>734</v>
+      </c>
+      <c r="G216" s="10" t="s">
+        <v>773</v>
+      </c>
+      <c r="H216" s="10" t="s">
+        <v>758</v>
+      </c>
+      <c r="I216" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve"> to end  ; ပြီးဆုံးစေသည် ; ၿပီးဆံုးေစသည္</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9">
+      <c r="B217" t="s">
+        <v>689</v>
+      </c>
+      <c r="C217" t="s">
+        <v>689</v>
+      </c>
+      <c r="E217" t="s">
+        <v>735</v>
+      </c>
+      <c r="G217" s="10" t="s">
+        <v>774</v>
+      </c>
+      <c r="H217" s="10" t="s">
+        <v>759</v>
+      </c>
+      <c r="I217" s="10" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve"> to overflow  ; လျှံကျသည် ; လွ်ံက်သည္</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9">
+      <c r="B218" t="s">
+        <v>690</v>
+      </c>
+      <c r="C218" t="s">
+        <v>713</v>
+      </c>
+      <c r="E218" t="s">
+        <v>736</v>
+      </c>
+      <c r="I218" s="10" t="str">
+        <f>CONCATENATE(D218," ",E218," ",F218)</f>
+        <v xml:space="preserve"> business performance </v>
+      </c>
+    </row>
+    <row r="219" spans="1:9">
+      <c r="B219" t="s">
+        <v>691</v>
+      </c>
+      <c r="C219" t="s">
+        <v>714</v>
+      </c>
+      <c r="E219" t="s">
+        <v>737</v>
+      </c>
+      <c r="G219" s="10" t="s">
+        <v>775</v>
+      </c>
+      <c r="H219" s="10" t="s">
+        <v>760</v>
+      </c>
+      <c r="I219" s="10" t="str">
+        <f t="shared" ref="I219:I223" si="25">CONCATENATE(D219," ",E219," ",F219, " ; ",G219," ; ", H219)</f>
+        <v xml:space="preserve"> income  ; ၀င်ငွေ ; ၀င္ေငြ</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9">
+      <c r="B220" t="s">
+        <v>761</v>
+      </c>
+      <c r="C220" t="s">
+        <v>762</v>
+      </c>
+      <c r="E220" t="s">
+        <v>763</v>
+      </c>
+      <c r="G220" s="10" t="s">
+        <v>776</v>
+      </c>
+      <c r="H220" s="10" t="s">
+        <v>764</v>
+      </c>
+      <c r="I220" s="10" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve"> expense  ; အသုံးစရိတ် ; အသံုးစရိတ္</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9">
+      <c r="B221" t="s">
+        <v>692</v>
+      </c>
+      <c r="C221" t="s">
+        <v>715</v>
+      </c>
+      <c r="D221" t="s">
+        <v>765</v>
+      </c>
+      <c r="E221" t="s">
+        <v>738</v>
+      </c>
+      <c r="F221" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G221" s="10" t="s">
+        <v>777</v>
+      </c>
+      <c r="H221" s="10" t="s">
+        <v>766</v>
+      </c>
+      <c r="I221" s="10" t="str">
+        <f t="shared" si="25"/>
+        <v>(が) reduction (to reduce) (する) ; လျော့ကျသည် ; ေလ်ာ့က်သည္</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9">
+      <c r="B222" t="s">
+        <v>693</v>
+      </c>
+      <c r="C222" t="s">
+        <v>716</v>
+      </c>
+      <c r="E222" t="s">
+        <v>739</v>
+      </c>
+      <c r="G222" s="10" t="s">
+        <v>778</v>
+      </c>
+      <c r="H222" s="10" t="s">
+        <v>767</v>
+      </c>
+      <c r="I222" s="10" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve"> savings  ; စုငွေပမာဏ ; စုေငြပမာဏ</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9">
+      <c r="B223" t="s">
+        <v>694</v>
+      </c>
+      <c r="C223" t="s">
+        <v>717</v>
+      </c>
+      <c r="D223" t="s">
+        <v>765</v>
+      </c>
+      <c r="E223" t="s">
+        <v>740</v>
+      </c>
+      <c r="F223" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G223" s="10" t="s">
+        <v>779</v>
+      </c>
+      <c r="H223" s="10" t="s">
+        <v>768</v>
+      </c>
+      <c r="I223" s="10" t="str">
+        <f t="shared" si="25"/>
+        <v>(が) increase (to increase) (する) ; တိုးပွားသည် ; တိုးပြားသည္</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9">
+      <c r="B224" t="s">
+        <v>695</v>
+      </c>
+      <c r="C224" t="s">
+        <v>718</v>
+      </c>
+      <c r="E224" t="s">
+        <v>741</v>
+      </c>
+      <c r="I224" s="10" t="str">
+        <f t="shared" ref="I224:I229" si="26">CONCATENATE(D224," ",E224," ",F224)</f>
+        <v xml:space="preserve"> reality, truth </v>
+      </c>
+    </row>
+    <row r="225" spans="1:9">
+      <c r="B225" t="s">
+        <v>696</v>
+      </c>
+      <c r="C225" t="s">
+        <v>696</v>
+      </c>
+      <c r="E225" t="s">
+        <v>742</v>
+      </c>
+      <c r="I225" s="10" t="str">
+        <f t="shared" si="26"/>
+        <v xml:space="preserve"> freeware </v>
+      </c>
+    </row>
+    <row r="226" spans="1:9">
+      <c r="B226" t="s">
+        <v>697</v>
+      </c>
+      <c r="C226" t="s">
+        <v>719</v>
+      </c>
+      <c r="E226" t="s">
+        <v>743</v>
+      </c>
+      <c r="I226" s="10" t="str">
+        <f t="shared" si="26"/>
+        <v xml:space="preserve"> to be excellent or superior </v>
+      </c>
+    </row>
+    <row r="227" spans="1:9">
+      <c r="B227" t="s">
+        <v>698</v>
+      </c>
+      <c r="C227" t="s">
+        <v>720</v>
+      </c>
+      <c r="E227" t="s">
+        <v>744</v>
+      </c>
+      <c r="I227" s="10" t="str">
+        <f t="shared" si="26"/>
+        <v xml:space="preserve"> a high fever </v>
+      </c>
+    </row>
+    <row r="228" spans="1:9">
+      <c r="B228" t="s">
+        <v>699</v>
+      </c>
+      <c r="C228" t="s">
+        <v>721</v>
+      </c>
+      <c r="E228" t="s">
+        <v>745</v>
+      </c>
+      <c r="I228" s="10" t="str">
+        <f t="shared" si="26"/>
+        <v xml:space="preserve"> weather </v>
+      </c>
+    </row>
+    <row r="229" spans="1:9">
+      <c r="B229" t="s">
+        <v>700</v>
+      </c>
+      <c r="C229" t="s">
+        <v>722</v>
+      </c>
+      <c r="E229" t="s">
+        <v>746</v>
+      </c>
+      <c r="I229" s="10" t="str">
+        <f t="shared" si="26"/>
+        <v xml:space="preserve"> rule </v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" s="5" customFormat="1">
+      <c r="A231" s="9" t="s">
+        <v>771</v>
+      </c>
+      <c r="B231" s="6"/>
+      <c r="C231" s="6"/>
+      <c r="D231" s="7"/>
+      <c r="E231" s="6"/>
+      <c r="F231" s="7"/>
+      <c r="G231" s="12"/>
+      <c r="H231" s="12"/>
+      <c r="I231" s="10" t="str">
+        <f>CONCATENATE(D231," ",E231," ",F231)</f>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="232" spans="1:9">
+      <c r="B232" t="s">
+        <v>701</v>
+      </c>
+      <c r="C232" t="s">
+        <v>723</v>
+      </c>
+      <c r="E232" t="s">
+        <v>747</v>
+      </c>
+      <c r="I232" s="10" t="str">
+        <f t="shared" ref="I232:I236" si="27">CONCATENATE(D232," ",E232," ",F232)</f>
+        <v xml:space="preserve"> one member </v>
+      </c>
+    </row>
+    <row r="233" spans="1:9">
+      <c r="B233" t="s">
+        <v>702</v>
+      </c>
+      <c r="C233" t="s">
+        <v>724</v>
+      </c>
+      <c r="E233" t="s">
+        <v>748</v>
+      </c>
+      <c r="I233" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v xml:space="preserve"> mental attitude </v>
+      </c>
+    </row>
+    <row r="234" spans="1:9">
+      <c r="B234" t="s">
+        <v>727</v>
+      </c>
+      <c r="C234" t="s">
+        <v>725</v>
+      </c>
+      <c r="E234" t="s">
+        <v>749</v>
+      </c>
+      <c r="I234" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v xml:space="preserve"> complaint </v>
+      </c>
+    </row>
+    <row r="235" spans="1:9">
+      <c r="B235" t="s">
+        <v>703</v>
+      </c>
+      <c r="C235" t="s">
+        <v>726</v>
+      </c>
+      <c r="E235" t="s">
+        <v>750</v>
+      </c>
+      <c r="F235" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I235" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v xml:space="preserve"> dealing with, handling (to deal with, handle) (する)</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9">
+      <c r="B236" t="s">
+        <v>704</v>
+      </c>
+      <c r="C236" t="s">
+        <v>704</v>
+      </c>
+      <c r="E236" t="s">
+        <v>749</v>
+      </c>
+      <c r="F236" t="s">
+        <v>587</v>
+      </c>
+      <c r="I236" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v xml:space="preserve"> complaint (kana)</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9">
+      <c r="B237" t="s">
+        <v>705</v>
+      </c>
+      <c r="C237" t="s">
+        <v>728</v>
+      </c>
+      <c r="E237" t="s">
+        <v>751</v>
+      </c>
+      <c r="G237" s="10" t="s">
+        <v>780</v>
+      </c>
+      <c r="H237" s="10" t="s">
+        <v>769</v>
+      </c>
+      <c r="I237" s="10" t="str">
+        <f t="shared" ref="I237" si="28">CONCATENATE(D237," ",E237," ",F237, " ; ",G237," ; ", H237)</f>
+        <v xml:space="preserve"> justified  ; မှန်ကန်ဖြောင့်မတ်သော ; မွန္ကန္ေျဖာင့္မတ္ေသာ</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9">
+      <c r="B238" t="s">
+        <v>706</v>
+      </c>
+      <c r="C238" t="s">
+        <v>729</v>
+      </c>
+      <c r="E238" t="s">
+        <v>752</v>
+      </c>
+      <c r="I238" s="10" t="str">
+        <f t="shared" ref="I238:I239" si="29">CONCATENATE(D238," ",E238," ",F238)</f>
+        <v xml:space="preserve"> uncomfortable </v>
+      </c>
+    </row>
+    <row r="239" spans="1:9">
+      <c r="B239" t="s">
+        <v>707</v>
+      </c>
+      <c r="C239" t="s">
+        <v>730</v>
+      </c>
+      <c r="E239" t="s">
+        <v>753</v>
+      </c>
+      <c r="I239" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v xml:space="preserve"> quality </v>
+      </c>
+    </row>
+    <row r="240" spans="1:9">
+      <c r="B240" t="s">
+        <v>708</v>
+      </c>
+      <c r="C240" t="s">
+        <v>731</v>
+      </c>
+      <c r="E240" t="s">
+        <v>754</v>
+      </c>
+      <c r="F240" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G240" s="10" t="s">
+        <v>781</v>
+      </c>
+      <c r="H240" s="10" t="s">
+        <v>770</v>
+      </c>
+      <c r="I240" s="10" t="str">
+        <f t="shared" ref="I240" si="30">CONCATENATE(D240," ",E240," ",F240, " ; ",G240," ; ", H240)</f>
+        <v xml:space="preserve"> pursuit (to pursue) (する) ; ရှာဖွေသည်၊ လေ့လာလိုက်စားသည် ; ရွာေဖြသည္၊ ေလ႔လာလိုက္စားသည္</v>
+      </c>
+    </row>
+    <row r="243" spans="2:5">
+      <c r="B243" t="s">
+        <v>709</v>
+      </c>
+      <c r="C243" t="s">
+        <v>709</v>
+      </c>
+      <c r="E243" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="244" spans="2:5">
+      <c r="B244" t="s">
+        <v>710</v>
+      </c>
+      <c r="C244" t="s">
+        <v>732</v>
+      </c>
+      <c r="E244" t="s">
+        <v>756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TRY N2 Vocab.xlsx -> Day17 definition updated.
</commit_message>
<xml_diff>
--- a/preparing/TRY N2 Vocab.xlsx
+++ b/preparing/TRY N2 Vocab.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="786">
   <si>
     <t>お知らせ</t>
   </si>
@@ -2370,12 +2370,24 @@
   </si>
   <si>
     <t>Day16, Day17 added</t>
+  </si>
+  <si>
+    <t>စိတ္ႀကိဳတင္ျပင္ဆင္ထားမႈ</t>
+  </si>
+  <si>
+    <t>စိတ်ကြိုတင်ပြင်ဆင်ထားမှု</t>
+  </si>
+  <si>
+    <t>Day17 Definition updated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-10000455]0"/>
+  </numFmts>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -2476,7 +2488,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2546,6 +2558,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2851,8 +2866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3158,10 +3173,18 @@
       </c>
     </row>
     <row r="23" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="23"/>
+      <c r="B23" s="27">
+        <v>20</v>
+      </c>
+      <c r="C23" s="15">
+        <v>43508</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>785</v>
+      </c>
     </row>
     <row r="24" spans="2:5" ht="18.75" customHeight="1">
       <c r="B24" s="14"/>
@@ -3214,8 +3237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I244"/>
   <sheetViews>
-    <sheetView topLeftCell="A230" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B240" sqref="B240"/>
+    <sheetView topLeftCell="A227" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G233" sqref="G233:I233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75"/>
@@ -3223,11 +3246,11 @@
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="31" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="27" style="10" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="10" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" customWidth="1"/>
+    <col min="5" max="5" width="31" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+    <col min="7" max="7" width="27" style="10" customWidth="1"/>
+    <col min="8" max="8" width="15" style="10" customWidth="1"/>
     <col min="9" max="9" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7107,9 +7130,15 @@
       <c r="E233" t="s">
         <v>748</v>
       </c>
-      <c r="I233" s="10" t="str">
-        <f t="shared" si="27"/>
-        <v xml:space="preserve"> mental attitude </v>
+      <c r="G233" s="26" t="s">
+        <v>784</v>
+      </c>
+      <c r="H233" s="26" t="s">
+        <v>783</v>
+      </c>
+      <c r="I233" s="26" t="str">
+        <f t="shared" ref="I233" si="28">CONCATENATE(D233," ",E233," ",F233, " ; ",G233," ; ", H233)</f>
+        <v xml:space="preserve"> mental attitude  ; စိတ်ကြိုတင်ပြင်ဆင်ထားမှု ; စိတ္ႀကိဳတင္ျပင္ဆင္ထားမႈ</v>
       </c>
     </row>
     <row r="234" spans="1:9">
@@ -7180,7 +7209,7 @@
         <v>769</v>
       </c>
       <c r="I237" s="10" t="str">
-        <f t="shared" ref="I237" si="28">CONCATENATE(D237," ",E237," ",F237, " ; ",G237," ; ", H237)</f>
+        <f t="shared" ref="I237" si="29">CONCATENATE(D237," ",E237," ",F237, " ; ",G237," ; ", H237)</f>
         <v xml:space="preserve"> justified  ; မှန်ကန်ဖြောင့်မတ်သော ; မွန္ကန္ေျဖာင့္မတ္ေသာ</v>
       </c>
     </row>
@@ -7195,7 +7224,7 @@
         <v>752</v>
       </c>
       <c r="I238" s="10" t="str">
-        <f t="shared" ref="I238:I239" si="29">CONCATENATE(D238," ",E238," ",F238)</f>
+        <f t="shared" ref="I238:I239" si="30">CONCATENATE(D238," ",E238," ",F238)</f>
         <v xml:space="preserve"> uncomfortable </v>
       </c>
     </row>
@@ -7210,7 +7239,7 @@
         <v>753</v>
       </c>
       <c r="I239" s="10" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v xml:space="preserve"> quality </v>
       </c>
     </row>
@@ -7234,7 +7263,7 @@
         <v>770</v>
       </c>
       <c r="I240" s="10" t="str">
-        <f t="shared" ref="I240" si="30">CONCATENATE(D240," ",E240," ",F240, " ; ",G240," ; ", H240)</f>
+        <f t="shared" ref="I240" si="31">CONCATENATE(D240," ",E240," ",F240, " ; ",G240," ; ", H240)</f>
         <v xml:space="preserve"> pursuit (to pursue) (する) ; ရှာဖွေသည်၊ လေ့လာလိုက်စားသည် ; ရွာေဖြသည္၊ ေလ႔လာလိုက္စားသည္</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Soumatome-N2 Vocab, Kanji.xlsx -> Kanji -> Myanmar Definition udpated.
</commit_message>
<xml_diff>
--- a/preparing/TRY N2 Vocab.xlsx
+++ b/preparing/TRY N2 Vocab.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="579"/>
@@ -10,7 +10,7 @@
     <sheet name="Data History" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -2372,23 +2372,23 @@
     <t>Day16, Day17 added</t>
   </si>
   <si>
-    <t>စိတ္ႀကိဳတင္ျပင္ဆင္ထားမႈ</t>
-  </si>
-  <si>
-    <t>စိတ်ကြိုတင်ပြင်ဆင်ထားမှု</t>
-  </si>
-  <si>
     <t>Day17 Definition updated</t>
+  </si>
+  <si>
+    <t>စိတ္ႀကိဳတင္ ျပင္ဆင္ထားမႈ</t>
+  </si>
+  <si>
+    <t>စိတ်ကြိုတင် ပြင်ဆင်ထားမှု</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-10000455]0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2622,7 +2622,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2654,9 +2654,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2688,6 +2689,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2863,14 +2865,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="1" customWidth="1"/>
@@ -2878,7 +2880,7 @@
     <col min="5" max="5" width="51.85546875" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15.75">
+    <row r="2" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
         <v>181</v>
       </c>
@@ -2892,7 +2894,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="14">
         <v>0</v>
       </c>
@@ -2906,7 +2908,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="20.25" customHeight="1">
+    <row r="4" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="14">
         <v>1</v>
       </c>
@@ -2920,7 +2922,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="20.25" customHeight="1">
+    <row r="5" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="14">
         <v>2</v>
       </c>
@@ -2934,7 +2936,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="20.25" customHeight="1">
+    <row r="6" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="14">
         <v>3</v>
       </c>
@@ -2948,7 +2950,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="20.25" customHeight="1">
+    <row r="7" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="14">
         <v>4</v>
       </c>
@@ -2962,7 +2964,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="20.25" customHeight="1">
+    <row r="8" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="14">
         <v>5</v>
       </c>
@@ -2976,7 +2978,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="20.25" customHeight="1">
+    <row r="9" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="14">
         <v>6</v>
       </c>
@@ -2990,7 +2992,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="20.25" customHeight="1">
+    <row r="10" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="14">
         <v>7</v>
       </c>
@@ -3004,7 +3006,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="20.25" customHeight="1">
+    <row r="11" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="14">
         <v>8</v>
       </c>
@@ -3018,7 +3020,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="20.25" customHeight="1">
+    <row r="12" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="14">
         <v>9</v>
       </c>
@@ -3032,7 +3034,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="20.25" customHeight="1">
+    <row r="13" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="14">
         <v>10</v>
       </c>
@@ -3046,7 +3048,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="20.25" customHeight="1">
+    <row r="14" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="14">
         <v>11</v>
       </c>
@@ -3060,7 +3062,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="20.25" customHeight="1">
+    <row r="15" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="14">
         <v>12</v>
       </c>
@@ -3074,7 +3076,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="30">
+    <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="14">
         <v>13</v>
       </c>
@@ -3088,7 +3090,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="20.25" customHeight="1">
+    <row r="17" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="14">
         <v>14</v>
       </c>
@@ -3102,7 +3104,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="20.25" customHeight="1">
+    <row r="18" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="14">
         <v>15</v>
       </c>
@@ -3116,7 +3118,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="20.25" customHeight="1">
+    <row r="19" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="14">
         <v>16</v>
       </c>
@@ -3130,7 +3132,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="20.25" customHeight="1">
+    <row r="20" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="14">
         <v>17</v>
       </c>
@@ -3144,7 +3146,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="20.25" customHeight="1">
+    <row r="21" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="14">
         <v>18</v>
       </c>
@@ -3158,7 +3160,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="18.75" customHeight="1">
+    <row r="22" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="14">
         <v>19</v>
       </c>
@@ -3172,7 +3174,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="18.75" customHeight="1">
+    <row r="23" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="27">
         <v>20</v>
       </c>
@@ -3183,46 +3185,46 @@
         <v>186</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="18.75" customHeight="1">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
       <c r="D24" s="16"/>
       <c r="E24" s="23"/>
     </row>
-    <row r="25" spans="2:5" ht="18.75" customHeight="1">
+    <row r="25" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
       <c r="D25" s="16"/>
       <c r="E25" s="23"/>
     </row>
-    <row r="26" spans="2:5" ht="18.75" customHeight="1">
+    <row r="26" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
       <c r="D26" s="16"/>
       <c r="E26" s="23"/>
     </row>
-    <row r="27" spans="2:5" ht="18.75" customHeight="1">
+    <row r="27" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
       <c r="D27" s="16"/>
       <c r="E27" s="23"/>
     </row>
-    <row r="28" spans="2:5" ht="18.75" customHeight="1">
+    <row r="28" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
       <c r="D28" s="16"/>
       <c r="E28" s="23"/>
     </row>
-    <row r="29" spans="2:5" ht="18.75" customHeight="1">
+    <row r="29" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>
       <c r="D29" s="16"/>
       <c r="E29" s="23"/>
     </row>
-    <row r="30" spans="2:5" ht="18.75" customHeight="1">
+    <row r="30" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="14"/>
       <c r="C30" s="15"/>
       <c r="D30" s="16"/>
@@ -3234,14 +3236,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I244"/>
   <sheetViews>
     <sheetView topLeftCell="A227" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G233" sqref="G233:I233"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21.75"/>
+  <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
@@ -3254,7 +3256,7 @@
     <col min="9" max="9" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="43.5">
+    <row r="1" spans="1:9" ht="43.5" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
@@ -3280,7 +3282,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1">
+    <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>133</v>
       </c>
@@ -3293,7 +3295,7 @@
       <c r="H2" s="12"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -3308,7 +3310,7 @@
         <v xml:space="preserve"> notice, announcement </v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -3323,7 +3325,7 @@
         <v xml:space="preserve"> employees, staff, human resources </v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -3338,7 +3340,7 @@
         <v xml:space="preserve"> to seek, to want </v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -3356,7 +3358,7 @@
         <v xml:space="preserve"> opening a store (to open a store) (する)</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -3374,7 +3376,7 @@
         <v xml:space="preserve"> closing a store (to close a store) (する)</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -3389,7 +3391,7 @@
         <v xml:space="preserve"> duty </v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -3407,7 +3409,7 @@
         <v xml:space="preserve"> selling, sales (to sell) (する)</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -3425,7 +3427,7 @@
         <v xml:space="preserve"> cleaning (to clean) (する)</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -3440,7 +3442,7 @@
         <v xml:space="preserve"> nationality </v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -3455,7 +3457,7 @@
         <v xml:space="preserve"> to be motivated </v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -3470,7 +3472,7 @@
         <v xml:space="preserve"> very much welcomed </v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -3488,7 +3490,7 @@
         <v xml:space="preserve"> customer service (to serve customers) (する)</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" t="s">
         <v>16</v>
       </c>
@@ -3506,7 +3508,7 @@
         <v xml:space="preserve"> dealing with (to deal with) (する)</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" t="s">
         <v>17</v>
       </c>
@@ -3521,7 +3523,7 @@
         <v xml:space="preserve"> can ～: When placed after a noun, this shows that the noun is allowed or possible. </v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
         <v>18</v>
       </c>
@@ -3536,7 +3538,7 @@
         <v xml:space="preserve"> pay, salary, wage </v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" t="s">
         <v>19</v>
       </c>
@@ -3554,7 +3556,7 @@
         <v xml:space="preserve"> consideration (to take into consideration) (する)</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" t="s">
         <v>20</v>
       </c>
@@ -3572,7 +3574,7 @@
         <v xml:space="preserve"> roundtrip (to go somewhere roundtrip) (する)</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
         <v>21</v>
       </c>
@@ -3590,7 +3592,7 @@
         <v xml:space="preserve"> provision (to provide) (する)</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" t="s">
         <v>22</v>
       </c>
@@ -3605,7 +3607,7 @@
         <v xml:space="preserve"> prescribed, certain </v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="s">
         <v>23</v>
       </c>
@@ -3620,7 +3622,7 @@
         <v xml:space="preserve"> document screening </v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" t="s">
         <v>24</v>
       </c>
@@ -3638,7 +3640,7 @@
         <v xml:space="preserve"> taking something (to take) (する)</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" t="s">
         <v>25</v>
       </c>
@@ -3653,13 +3655,13 @@
         <v xml:space="preserve"> doctor, physician </v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="I25" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="5" customFormat="1">
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="9" t="s">
         <v>134</v>
       </c>
@@ -3672,10 +3674,10 @@
       <c r="H26" s="12"/>
       <c r="I26" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" t="s">
         <v>26</v>
       </c>
@@ -3690,7 +3692,7 @@
         <v xml:space="preserve"> absence (of a doctor or physician) </v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" t="s">
         <v>27</v>
       </c>
@@ -3705,7 +3707,7 @@
         <v xml:space="preserve"> remodeling work </v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" t="s">
         <v>28</v>
       </c>
@@ -3720,7 +3722,7 @@
         <v xml:space="preserve"> written to the left </v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" t="s">
         <v>29</v>
       </c>
@@ -3735,7 +3737,7 @@
         <v xml:space="preserve"> temporary shop </v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" t="s">
         <v>30</v>
       </c>
@@ -3750,7 +3752,7 @@
         <v xml:space="preserve"> promotional/sales campaign </v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" t="s">
         <v>31</v>
       </c>
@@ -3765,7 +3767,7 @@
         <v xml:space="preserve"> raw food </v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" t="s">
         <v>32</v>
       </c>
@@ -3783,7 +3785,7 @@
         <v xml:space="preserve"> inspection (to inspect) (する)</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" t="s">
         <v>33</v>
       </c>
@@ -3798,7 +3800,7 @@
         <v xml:space="preserve"> temporary closing </v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" t="s">
         <v>34</v>
       </c>
@@ -3816,7 +3818,7 @@
         <v xml:space="preserve"> closing a business (to close a business) (する)</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" t="s">
         <v>35</v>
       </c>
@@ -3831,7 +3833,7 @@
         <v xml:space="preserve"> day and night </v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" t="s">
         <v>36</v>
       </c>
@@ -3846,7 +3848,7 @@
         <v xml:space="preserve"> late at night </v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" t="s">
         <v>37</v>
       </c>
@@ -3861,7 +3863,7 @@
         <v xml:space="preserve"> presence, existence </v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" t="s">
         <v>38</v>
       </c>
@@ -3876,7 +3878,7 @@
         <v xml:space="preserve"> old and young, men and women (i.e. any age or gender) </v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" t="s">
         <v>39</v>
       </c>
@@ -3891,7 +3893,7 @@
         <v xml:space="preserve"> occupation, job </v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" t="s">
         <v>40</v>
       </c>
@@ -3906,7 +3908,7 @@
         <v xml:space="preserve"> academic background </v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B42" t="s">
         <v>41</v>
       </c>
@@ -3921,13 +3923,13 @@
         <v xml:space="preserve"> interest (in something) </v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="I43" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="5" customFormat="1">
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="9" t="s">
         <v>135</v>
       </c>
@@ -3940,10 +3942,10 @@
       <c r="H44" s="12"/>
       <c r="I44" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B45" t="s">
         <v>42</v>
       </c>
@@ -3958,7 +3960,7 @@
         <v xml:space="preserve"> regular, normal </v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B46" t="s">
         <v>43</v>
       </c>
@@ -3982,7 +3984,7 @@
         <v xml:space="preserve"> offering, providing (to offer, provide) (する) ; ကမ်းလှမ်းသည်၊ ထောက်ပံ့သည် ; ကမ္းလွမ္းသည္၊ ေထာက္ပံ႔သည္</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B47" t="s">
         <v>44</v>
       </c>
@@ -3997,7 +3999,7 @@
         <v xml:space="preserve"> corner, section </v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B48" t="s">
         <v>45</v>
       </c>
@@ -4018,7 +4020,7 @@
         <v xml:space="preserve"> surroundings  ; ပတ်ပတ်လည် ; ပတ္ပတ္လည္</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B49" t="s">
         <v>46</v>
       </c>
@@ -4042,7 +4044,7 @@
         <v xml:space="preserve"> shoplifting (to shoplift) (する) ; အလစ်သုတ်သည် ; အလစ္သုတ္သည္</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B50" t="s">
         <v>47</v>
       </c>
@@ -4066,7 +4068,7 @@
         <v xml:space="preserve"> cheating on someone (to cheat on someone) (する) ; (ရည်းစား၊ အိမ်ထောင်) ဖောက်ပြန်သည် ; (ရည္းစား၊ အိမ္ေထာင္) ေဖာက္ျပန္သည္</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B51" t="s">
         <v>48</v>
       </c>
@@ -4081,7 +4083,7 @@
         <v xml:space="preserve"> simple, mere </v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B52" t="s">
         <v>49</v>
       </c>
@@ -4096,10 +4098,10 @@
         <v xml:space="preserve"> counterfeit item, fake </v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="I53" s="10"/>
     </row>
-    <row r="54" spans="1:9" s="5" customFormat="1">
+    <row r="54" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="9" t="s">
         <v>137</v>
       </c>
@@ -4112,10 +4114,10 @@
       <c r="H54" s="12"/>
       <c r="I54" s="10" t="str">
         <f>CONCATENATE(D54," ",E54," ",F54)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B55" t="s">
         <v>50</v>
       </c>
@@ -4130,7 +4132,7 @@
         <v xml:space="preserve"> New Year's party </v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B56" t="s">
         <v>51</v>
       </c>
@@ -4151,7 +4153,7 @@
         <v xml:space="preserve"> clothing  ; အဝတ်အစားမျိုးစုံ ; အ၀တ္အစားမ်ိဳးစံု</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B57" t="s">
         <v>52</v>
       </c>
@@ -4172,7 +4174,7 @@
         <v xml:space="preserve"> to bear in mind  ; (တခုခုလုပ်ဖို့) စိတ်မွေးသည် ; (တခုခုလုပ္ဖို႔) စိတ္ေမြးသည္</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B58" t="s">
         <v>53</v>
       </c>
@@ -4196,7 +4198,7 @@
         <v xml:space="preserve"> request (する) ; တောင်းဆိုမှု ; ေတာင္းဆုိမႈ</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B59" t="s">
         <v>54</v>
       </c>
@@ -4211,10 +4213,10 @@
         <v xml:space="preserve"> allowance: money paid separately from wages or salary </v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="I60" s="10"/>
     </row>
-    <row r="61" spans="1:9" s="5" customFormat="1">
+    <row r="61" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="9" t="s">
         <v>188</v>
       </c>
@@ -4227,10 +4229,10 @@
       <c r="H61" s="12"/>
       <c r="I61" s="10" t="str">
         <f>CONCATENATE(D61," ",E61," ",F61)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B62" t="s">
         <v>55</v>
       </c>
@@ -4248,7 +4250,7 @@
         <v xml:space="preserve"> returning an item (to return an item) (する)</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B63" t="s">
         <v>56</v>
       </c>
@@ -4272,7 +4274,7 @@
         <v xml:space="preserve"> statement (to state) (する) ; ထုတ်ဖော်ပြောဆိုသည် ; ထုတ္ေဖာ္ေျပာဆိုသည္</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B64" t="s">
         <v>57</v>
       </c>
@@ -4287,7 +4289,7 @@
         <v xml:space="preserve"> clear or rainy weather </v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B65" t="s">
         <v>58</v>
       </c>
@@ -4302,7 +4304,7 @@
         <v xml:space="preserve"> to summarize (one's opinion) </v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B66" t="s">
         <v>59</v>
       </c>
@@ -4320,7 +4322,7 @@
         <v xml:space="preserve"> contribution, donation (to contribute, donate) (する)</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B67" t="s">
         <v>60</v>
       </c>
@@ -4335,7 +4337,7 @@
         <v xml:space="preserve"> environmental pollution </v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B68" t="s">
         <v>61</v>
       </c>
@@ -4353,7 +4355,7 @@
         <v xml:space="preserve"> pollution (to pollute) (する)</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B69" t="s">
         <v>62</v>
       </c>
@@ -4368,7 +4370,7 @@
         <v xml:space="preserve"> good luck, fortune </v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B70" t="s">
         <v>199</v>
       </c>
@@ -4383,7 +4385,7 @@
         <v xml:space="preserve"> wind power </v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B71" t="s">
         <v>200</v>
       </c>
@@ -4398,7 +4400,7 @@
         <v xml:space="preserve"> natural energy </v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B72" t="s">
         <v>203</v>
       </c>
@@ -4416,11 +4418,11 @@
         <v xml:space="preserve"> losing a job (to lose a job) (する)</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="F73" s="1"/>
       <c r="I73" s="10"/>
     </row>
-    <row r="74" spans="1:9" s="5" customFormat="1">
+    <row r="74" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="9" t="s">
         <v>276</v>
       </c>
@@ -4433,10 +4435,10 @@
       <c r="H74" s="12"/>
       <c r="I74" s="10" t="str">
         <f>CONCATENATE(D74," ",E74," ",F74)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="75" spans="1:9">
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B75" t="s">
         <v>218</v>
       </c>
@@ -4454,7 +4456,7 @@
         <v xml:space="preserve"> loss of an object (to lose something) (する)</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B76" t="s">
         <v>219</v>
       </c>
@@ -4475,7 +4477,7 @@
         <v xml:space="preserve"> taking off or landing  ; ထွက်ခွာ ဆင်းသက်ခြင်း ; ထြက္ခြာ ဆင္းသက္ျခင္း</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B77" t="s">
         <v>220</v>
       </c>
@@ -4496,7 +4498,7 @@
         <v xml:space="preserve"> fire (disaster)  ; မီးဘေး ; မီးေဘး</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B78" t="s">
         <v>221</v>
       </c>
@@ -4511,7 +4513,7 @@
         <v xml:space="preserve"> rainy weather </v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B79" t="s">
         <v>222</v>
       </c>
@@ -4526,7 +4528,7 @@
         <v xml:space="preserve"> indoors </v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B80" t="s">
         <v>223</v>
       </c>
@@ -4541,7 +4543,7 @@
         <v xml:space="preserve"> password </v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B81" t="s">
         <v>224</v>
       </c>
@@ -4559,7 +4561,7 @@
         <v xml:space="preserve"> wearing (to wear) (する) (use in writing)</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B82" t="s">
         <v>225</v>
       </c>
@@ -4574,7 +4576,7 @@
         <v xml:space="preserve"> emergency button </v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B83" t="s">
         <v>226</v>
       </c>
@@ -4589,7 +4591,7 @@
         <v xml:space="preserve"> deadline </v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B84" t="s">
         <v>227</v>
       </c>
@@ -4613,10 +4615,10 @@
         <v xml:space="preserve"> compliance (to comply) (する) ; မဖြစ်မနေ ကာကွယ်သည် ; မျဖစ္မေန ကာကြယ္သည္</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="1:9" s="5" customFormat="1">
+    <row r="86" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="9" t="s">
         <v>277</v>
       </c>
@@ -4629,10 +4631,10 @@
       <c r="H86" s="12"/>
       <c r="I86" s="10" t="str">
         <f>CONCATENATE(D86," ",E86," ",F86)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="87" spans="1:9">
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B87" t="s">
         <v>228</v>
       </c>
@@ -4647,7 +4649,7 @@
         <v xml:space="preserve"> request form, application form (入学) </v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B88" t="s">
         <v>229</v>
       </c>
@@ -4662,7 +4664,7 @@
         <v xml:space="preserve"> counter, desk, liaison </v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B89" t="s">
         <v>230</v>
       </c>
@@ -4677,7 +4679,7 @@
         <v xml:space="preserve"> writing implement (pencil, eraser, book,etc..) </v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B90" t="s">
         <v>231</v>
       </c>
@@ -4692,7 +4694,7 @@
         <v xml:space="preserve"> poolside </v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B91" t="s">
         <v>288</v>
       </c>
@@ -4719,10 +4721,10 @@
         <v>(ゴミを) 1.separation, 2.discernment, judgment (する) ; သီးသန့်ခွဲသည်၊ အမြော်အမြင်ရှိသည် ; သီးသန္႔ခြဲသည္၊ အေျမာ္အျမင္ရွိသည္</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="1:9" s="5" customFormat="1">
+    <row r="93" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="9" t="s">
         <v>286</v>
       </c>
@@ -4735,10 +4737,10 @@
       <c r="H93" s="12"/>
       <c r="I93" s="10" t="str">
         <f>CONCATENATE(D93," ",E93," ",F93)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="94" spans="1:9">
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B94" t="s">
         <v>232</v>
       </c>
@@ -4756,7 +4758,7 @@
         <v xml:space="preserve"> change of post (to change one's post) (する)</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B95" t="s">
         <v>233</v>
       </c>
@@ -4771,7 +4773,7 @@
         <v xml:space="preserve"> to appoint, assign, order </v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B96" t="s">
         <v>234</v>
       </c>
@@ -4786,7 +4788,7 @@
         <v xml:space="preserve"> gene </v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B97" t="s">
         <v>235</v>
       </c>
@@ -4801,7 +4803,7 @@
         <v xml:space="preserve"> welcome party </v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B98" t="s">
         <v>236</v>
       </c>
@@ -4816,7 +4818,7 @@
         <v xml:space="preserve"> to review, reconsider </v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B99" t="s">
         <v>237</v>
       </c>
@@ -4831,7 +4833,7 @@
         <v xml:space="preserve"> spice </v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B100" t="s">
         <v>238</v>
       </c>
@@ -4846,7 +4848,7 @@
         <v xml:space="preserve"> microwave oven </v>
       </c>
     </row>
-    <row r="102" spans="1:9" s="5" customFormat="1">
+    <row r="102" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="9" t="s">
         <v>302</v>
       </c>
@@ -4859,10 +4861,10 @@
       <c r="H102" s="12"/>
       <c r="I102" s="10" t="str">
         <f>CONCATENATE(D102," ",E102," ",F102)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="103" spans="1:9">
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B103" t="s">
         <v>303</v>
       </c>
@@ -4877,7 +4879,7 @@
         <v xml:space="preserve"> jacket </v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B104" t="s">
         <v>304</v>
       </c>
@@ -4895,7 +4897,7 @@
         <v xml:space="preserve"> arrival, receipt (to arrive, receive) (する)</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B105" t="s">
         <v>305</v>
       </c>
@@ -4910,7 +4912,7 @@
         <v xml:space="preserve"> celebrity </v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B106" t="s">
         <v>306</v>
       </c>
@@ -4925,7 +4927,7 @@
         <v xml:space="preserve"> instructor, teacher </v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B107" t="s">
         <v>307</v>
       </c>
@@ -4940,7 +4942,7 @@
         <v xml:space="preserve"> Southeast Asia </v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B108" t="s">
         <v>308</v>
       </c>
@@ -4961,7 +4963,7 @@
         <v xml:space="preserve"> streamlining  ; တွက်ခြေကိုက်အောင် လုပ်သည် ; တြက္ေျခကိုက္ေအာင္ လုပ္သည္</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B109" t="s">
         <v>309</v>
       </c>
@@ -4977,7 +4979,7 @@
         <v xml:space="preserve"> many </v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B110" t="s">
         <v>310</v>
       </c>
@@ -4998,7 +5000,7 @@
         <v xml:space="preserve"> employee  ; လုပ်ငန်းခွင်ထဲက အလုပ်သမား ; လုပ္ငန္းခြင္ထဲက အလုပ္သမား</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B111" t="s">
         <v>311</v>
       </c>
@@ -5022,7 +5024,7 @@
         <v xml:space="preserve"> dismissal (to dismiss) (する) ; အလုပ်ထုတ်ခြင်း၊ ထွက်ခိုင်းခြင်း ; အလုပ္ထုတ္ျခင္း၊ ထြက္ခိုင္းျခင္း</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B112" t="s">
         <v>312</v>
       </c>
@@ -5038,7 +5040,7 @@
         <v xml:space="preserve"> to accept, recognize </v>
       </c>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B113" t="s">
         <v>313</v>
       </c>
@@ -5062,7 +5064,7 @@
         <v xml:space="preserve"> respect (to respect) (する) ; လေးစားအားကျခြင်း ; ေလးစားအားက်ျခင္း</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B114" t="s">
         <v>314</v>
       </c>
@@ -5078,7 +5080,7 @@
         <v xml:space="preserve"> coast </v>
       </c>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B115" t="s">
         <v>7</v>
       </c>
@@ -5097,7 +5099,7 @@
         <v xml:space="preserve"> cleaning (to clean) (する)</v>
       </c>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B116" t="s">
         <v>315</v>
       </c>
@@ -5121,7 +5123,7 @@
         <v xml:space="preserve"> consent (to consent) (する) ; သဘောတူလက်ခံခြင်း ; သေဘာတူလက္ခံျခင္း</v>
       </c>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B117" t="s">
         <v>316</v>
       </c>
@@ -5137,7 +5139,7 @@
         <v xml:space="preserve"> grandparents </v>
       </c>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B118" t="s">
         <v>317</v>
       </c>
@@ -5158,7 +5160,7 @@
         <v xml:space="preserve"> sleeping  ; အိပ်ပျော်ခြင်း ; အိပ္ေပ်ာ္ျခင္း</v>
       </c>
     </row>
-    <row r="120" spans="1:9" s="5" customFormat="1">
+    <row r="120" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="9" t="s">
         <v>361</v>
       </c>
@@ -5171,10 +5173,10 @@
       <c r="H120" s="12"/>
       <c r="I120" s="10" t="str">
         <f>CONCATENATE(D120," ",E120," ",F120)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="121" spans="1:9">
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B121" t="s">
         <v>1</v>
       </c>
@@ -5189,7 +5191,7 @@
         <v xml:space="preserve"> employees, staff, human resources </v>
       </c>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B122" t="s">
         <v>362</v>
       </c>
@@ -5213,7 +5215,7 @@
         <v xml:space="preserve"> getting, securing (to get, secure) (する) ; ရအောင်ယူသည်၊ (နေရာ)ဦးသည် ; ရေအာင္ယူသည္၊ (ေနရာ)ဦးသည္</v>
       </c>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B123" t="s">
         <v>363</v>
       </c>
@@ -5228,7 +5230,7 @@
         <v xml:space="preserve"> small- and medium-sized enterprises (SMEs) </v>
       </c>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B124" t="s">
         <v>364</v>
       </c>
@@ -5243,7 +5245,7 @@
         <v xml:space="preserve"> crime </v>
       </c>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B125" t="s">
         <v>365</v>
       </c>
@@ -5261,7 +5263,7 @@
         <v xml:space="preserve"> prevention (to prevent) (する)</v>
       </c>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B126" t="s">
         <v>366</v>
       </c>
@@ -5276,7 +5278,7 @@
         <v xml:space="preserve"> South America </v>
       </c>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B127" t="s">
         <v>367</v>
       </c>
@@ -5291,7 +5293,7 @@
         <v xml:space="preserve"> to learn, acquire; to put on </v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="34.5">
+    <row r="128" spans="1:9" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B128" t="s">
         <v>368</v>
       </c>
@@ -5303,10 +5305,11 @@
       </c>
       <c r="I128" s="10" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> bilateral (literally "between both countries")  </v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" s="5" customFormat="1">
+        <v xml:space="preserve"> bilateral (literally "between both 
+countries")  </v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="9" t="s">
         <v>395</v>
       </c>
@@ -5319,10 +5322,10 @@
       <c r="H130" s="12"/>
       <c r="I130" s="10" t="str">
         <f>CONCATENATE(D130," ",E130," ",F130)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="131" spans="1:9">
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B131" t="s">
         <v>369</v>
       </c>
@@ -5343,7 +5346,7 @@
         <v xml:space="preserve"> active, lively, vigorous  ; သွက်လက်ဖြတ်လတ်သော ; သြက္လက္ျဖတ္လတ္ေသာ</v>
       </c>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B132" t="s">
         <v>370</v>
       </c>
@@ -5367,7 +5370,7 @@
         <v xml:space="preserve"> talking back (to talk back) (する) ; ပြန်ခံပြောသည်၊ ဘုကလန့်လုပ်သည် ; ျပန္ခံေျပာသည္၊ ဘုကလန္႔လုပ္သည္</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B133" t="s">
         <v>371</v>
       </c>
@@ -5388,7 +5391,7 @@
         <v xml:space="preserve"> not ～ at all  ; လုံးဝ~မ~ဘူး ; လံုး၀~မ~ဘူး</v>
       </c>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B134" t="s">
         <v>372</v>
       </c>
@@ -5412,7 +5415,7 @@
         <v xml:space="preserve"> rebellion (to rebel) (する) ; မနာခံခြင်း၊ ပုန်ကန်ခြင်း ; မနာခံျခင္း၊ ပုန္ကန္ျခင္း</v>
       </c>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B135" t="s">
         <v>373</v>
       </c>
@@ -5430,7 +5433,7 @@
         <v xml:space="preserve"> lost love (to lose a lover) (する)</v>
       </c>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B136" t="s">
         <v>374</v>
       </c>
@@ -5451,7 +5454,7 @@
         <v xml:space="preserve"> with all one's might  ; အစွမ်းကုန် ; အစြမ္းကုန္</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B137" t="s">
         <v>375</v>
       </c>
@@ -5469,7 +5472,7 @@
         <v xml:space="preserve"> style (to be stylish) (する)</v>
       </c>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B138" t="s">
         <v>376</v>
       </c>
@@ -5484,7 +5487,7 @@
         <v xml:space="preserve"> attitude </v>
       </c>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B139" t="s">
         <v>377</v>
       </c>
@@ -5499,7 +5502,7 @@
         <v xml:space="preserve"> point </v>
       </c>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B140" t="s">
         <v>401</v>
       </c>
@@ -5514,7 +5517,7 @@
         <v xml:space="preserve"> religion </v>
       </c>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B141" t="s">
         <v>402</v>
       </c>
@@ -5529,7 +5532,7 @@
         <v xml:space="preserve"> shop </v>
       </c>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B142" t="s">
         <v>403</v>
       </c>
@@ -5547,7 +5550,7 @@
         <v xml:space="preserve"> setting up, establishment (する)</v>
       </c>
     </row>
-    <row r="143" spans="1:9">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B143" t="s">
         <v>404</v>
       </c>
@@ -5562,7 +5565,7 @@
         <v xml:space="preserve"> surrounding, nearby </v>
       </c>
     </row>
-    <row r="144" spans="1:9">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B144" t="s">
         <v>405</v>
       </c>
@@ -5577,7 +5580,7 @@
         <v xml:space="preserve"> marketing </v>
       </c>
     </row>
-    <row r="145" spans="1:9">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B145" t="s">
         <v>406</v>
       </c>
@@ -5598,7 +5601,7 @@
         <v xml:space="preserve"> essential, vital  ; မရှိမဖြစ်သော ; မရွိမျဖစ္ေသာ</v>
       </c>
     </row>
-    <row r="146" spans="1:9">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B146" t="s">
         <v>407</v>
       </c>
@@ -5619,7 +5622,7 @@
         <v xml:space="preserve"> cost performance  ; ကုန်ကျမှု ပြန်ရမှု နှိုင်းယှဉ်ချက် ; ကုန္က်မႈ ျပန္ရမႈ ႏိႈင္းယွဥ္ခ်က္</v>
       </c>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B147" t="s">
         <v>408</v>
       </c>
@@ -5640,7 +5643,7 @@
         <v xml:space="preserve"> a strong yen  ; ယန်းဈေးခိုင်မာမှု ; ယန္းေစ်းခိုင္မာမႈ</v>
       </c>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B148" t="s">
         <v>409</v>
       </c>
@@ -5655,7 +5658,7 @@
         <v xml:space="preserve"> course, lecture </v>
       </c>
     </row>
-    <row r="149" spans="1:9">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B149" t="s">
         <v>410</v>
       </c>
@@ -5670,7 +5673,7 @@
         <v xml:space="preserve"> knowledge </v>
       </c>
     </row>
-    <row r="150" spans="1:9">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B150" t="s">
         <v>411</v>
       </c>
@@ -5691,7 +5694,7 @@
         <v xml:space="preserve"> a higher-level school to enter  ; တက်ရမယ့် ပိုမြင့်တဲ့ကျောင်း ; တက္ရမယ့္ ပိုျမင့္တဲ႔ေက်ာင္း</v>
       </c>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B151" t="s">
         <v>412</v>
       </c>
@@ -5712,7 +5715,7 @@
         <v xml:space="preserve"> job-finding rate, employment rate  ; အလုပ်ဝင်နှုန်း ; အလုပ္၀င္ႏႈန္း</v>
       </c>
     </row>
-    <row r="152" spans="1:9">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B152" t="s">
         <v>413</v>
       </c>
@@ -5733,7 +5736,7 @@
         <v xml:space="preserve"> agriculture  ; စိုက်ပျိုးရေး ; စိုက္ပ်ိဳးေရး</v>
       </c>
     </row>
-    <row r="153" spans="1:9">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B153" t="s">
         <v>414</v>
       </c>
@@ -5754,7 +5757,7 @@
         <v xml:space="preserve"> farming village  ; စိုက်ပျိုးရေးလုပ်တဲ့ရွာ ; စိုက္ပ်ိဳးေရးလုပ္တဲ႔ရြာ</v>
       </c>
     </row>
-    <row r="154" spans="1:9">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B154" t="s">
         <v>415</v>
       </c>
@@ -5775,7 +5778,7 @@
         <v xml:space="preserve"> terrain  ; မြေအနေအထား ; ေျမအေနအထား</v>
       </c>
     </row>
-    <row r="156" spans="1:9" s="5" customFormat="1">
+    <row r="156" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="9" t="s">
         <v>534</v>
       </c>
@@ -5788,10 +5791,10 @@
       <c r="H156" s="12"/>
       <c r="I156" s="10" t="str">
         <f>CONCATENATE(D156," ",E156," ",F156)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="157" spans="1:9">
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B157" t="s">
         <v>416</v>
       </c>
@@ -5806,7 +5809,7 @@
         <v xml:space="preserve"> leader </v>
       </c>
     </row>
-    <row r="158" spans="1:9">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B158" s="21" t="s">
         <v>591</v>
       </c>
@@ -5821,7 +5824,7 @@
         <v xml:space="preserve"> digital voice recorder </v>
       </c>
     </row>
-    <row r="159" spans="1:9">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B159" t="s">
         <v>417</v>
       </c>
@@ -5836,7 +5839,7 @@
         <v xml:space="preserve"> small type </v>
       </c>
     </row>
-    <row r="160" spans="1:9">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B160" t="s">
         <v>418</v>
       </c>
@@ -5854,7 +5857,7 @@
         <v xml:space="preserve"> recording sound (to record sound) (する)</v>
       </c>
     </row>
-    <row r="161" spans="1:9">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B161" t="s">
         <v>419</v>
       </c>
@@ -5869,7 +5872,7 @@
         <v xml:space="preserve"> possible </v>
       </c>
     </row>
-    <row r="162" spans="1:9">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B162" t="s">
         <v>420</v>
       </c>
@@ -5893,7 +5896,7 @@
         <v xml:space="preserve"> display, exhibition (する) ; ခင်းကျင်းပြသခြင်း ; ခင္းက်င္းျပသျခင္း</v>
       </c>
     </row>
-    <row r="163" spans="1:9">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B163" t="s">
         <v>421</v>
       </c>
@@ -5908,7 +5911,7 @@
         <v xml:space="preserve"> old type </v>
       </c>
     </row>
-    <row r="164" spans="1:9">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B164" t="s">
         <v>422</v>
       </c>
@@ -5926,7 +5929,7 @@
         <v xml:space="preserve"> enlargement (to enlarge) (する)</v>
       </c>
     </row>
-    <row r="165" spans="1:9">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B165" t="s">
         <v>423</v>
       </c>
@@ -5944,7 +5947,7 @@
         <v xml:space="preserve"> trying, challenging oneself (する)</v>
       </c>
     </row>
-    <row r="166" spans="1:9">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B166" t="s">
         <v>424</v>
       </c>
@@ -5959,7 +5962,7 @@
         <v xml:space="preserve"> full effort </v>
       </c>
     </row>
-    <row r="167" spans="1:9">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B167" t="s">
         <v>427</v>
       </c>
@@ -5980,7 +5983,7 @@
         <v xml:space="preserve"> to become familiar with  ; ရင်းနှီးကျွမ်းဝင်သည် ; ရင္းႏွီးကၽြမ္း၀င္သည္</v>
       </c>
     </row>
-    <row r="168" spans="1:9">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B168" t="s">
         <v>428</v>
       </c>
@@ -6001,7 +6004,7 @@
         <v xml:space="preserve"> consideration (for others), care  ; အလိုက်သိတတ်နားလည်သော ; အလိုက္သိတတ္နားလည္ေသာ</v>
       </c>
     </row>
-    <row r="170" spans="1:9" s="5" customFormat="1">
+    <row r="170" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="9" t="s">
         <v>556</v>
       </c>
@@ -6014,10 +6017,10 @@
       <c r="H170" s="12"/>
       <c r="I170" s="10" t="str">
         <f>CONCATENATE(D170," ",E170," ",F170)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="171" spans="1:9">
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B171" t="s">
         <v>429</v>
       </c>
@@ -6038,7 +6041,7 @@
         <v xml:space="preserve"> organization  ; အဖွဲ့အစည်း(အကြီး) ; အဖြဲ႔အစည္း(အႀကီး)</v>
       </c>
     </row>
-    <row r="172" spans="1:9">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B172" s="21" t="s">
         <v>590</v>
       </c>
@@ -6053,7 +6056,7 @@
         <v xml:space="preserve"> traditional performing arts </v>
       </c>
     </row>
-    <row r="173" spans="1:9">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B173" t="s">
         <v>430</v>
       </c>
@@ -6074,7 +6077,7 @@
         <v xml:space="preserve"> symposium  ; ခေါင်းစဉ်တစ်ခုနှင့် ပတ်သက်သော သီးသန့်ဆွေးနွေးပွဲ ; ေခါင္းစဥ္တစ္ခုႏွင့္ ပတ္သက္ေသာ သီးသန္႔ေဆြးေႏြးပြဲ</v>
       </c>
     </row>
-    <row r="174" spans="1:9">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B174" t="s">
         <v>431</v>
       </c>
@@ -6095,7 +6098,7 @@
         <v xml:space="preserve"> consensus opinion  ; အများရဲ့သဘောအကြံဉာဏ် ; အမ်ားရဲ႕သေဘာအႀကံဉာဏ္</v>
       </c>
     </row>
-    <row r="175" spans="1:9">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B175" t="s">
         <v>432</v>
       </c>
@@ -6116,7 +6119,7 @@
         <v xml:space="preserve"> model  ; စံပြပုံစံ ; စံျပပံုစံ</v>
       </c>
     </row>
-    <row r="176" spans="1:9">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B176" t="s">
         <v>433</v>
       </c>
@@ -6134,7 +6137,7 @@
         <v xml:space="preserve"> engineer (kana)</v>
       </c>
     </row>
-    <row r="177" spans="1:9">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B177" t="s">
         <v>434</v>
       </c>
@@ -6155,7 +6158,7 @@
         <v xml:space="preserve"> assumption  ; ကြိုတင်ယူဆချက် ; ႀကိဳတင္ယူဆခ်က္</v>
       </c>
     </row>
-    <row r="178" spans="1:9">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B178" t="s">
         <v>435</v>
       </c>
@@ -6179,7 +6182,7 @@
         <v xml:space="preserve"> association; society; acquaintance (する) ; ၁။ပေါင်းသင်းဆက်ဆံသည်၊ ၂။ Date လုပ်သည် ; ၁။ေပါင္းသင္းဆက္ဆံသည္၊ ၂။ Date လုပ္သည္</v>
       </c>
     </row>
-    <row r="179" spans="1:9">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B179" t="s">
         <v>436</v>
       </c>
@@ -6194,7 +6197,7 @@
         <v xml:space="preserve"> profit </v>
       </c>
     </row>
-    <row r="180" spans="1:9">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B180" t="s">
         <v>437</v>
       </c>
@@ -6209,7 +6212,7 @@
         <v xml:space="preserve"> economic activity </v>
       </c>
     </row>
-    <row r="181" spans="1:9">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B181" t="s">
         <v>438</v>
       </c>
@@ -6227,7 +6230,7 @@
         <v xml:space="preserve"> hire, use; adoption; acceptance (する)</v>
       </c>
     </row>
-    <row r="182" spans="1:9">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B182" t="s">
         <v>439</v>
       </c>
@@ -6242,7 +6245,7 @@
         <v xml:space="preserve"> captain </v>
       </c>
     </row>
-    <row r="183" spans="1:9">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B183" t="s">
         <v>440</v>
       </c>
@@ -6257,7 +6260,7 @@
         <v xml:space="preserve"> all together </v>
       </c>
     </row>
-    <row r="184" spans="1:9">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B184" t="s">
         <v>557</v>
       </c>
@@ -6278,7 +6281,7 @@
         <v xml:space="preserve"> with all one's strength  ; စိတ်အားရတဲ့အထိ ; စိတ္အားရတဲ႔အထိ</v>
       </c>
     </row>
-    <row r="185" spans="1:9">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B185" t="s">
         <v>558</v>
       </c>
@@ -6293,7 +6296,7 @@
         <v xml:space="preserve"> coach, manager </v>
       </c>
     </row>
-    <row r="186" spans="1:9">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B186" t="s">
         <v>559</v>
       </c>
@@ -6317,7 +6320,7 @@
         <v xml:space="preserve"> a letter (to submit a letter) (する) ; ကိုယ့်ထင်မြင်ချက်ကို ဖော်ပြတဲ့စာ ; ကိုယ့္ထင္ျမင္ခ်က္ကို ေဖာ္ျပတဲ႔စာ</v>
       </c>
     </row>
-    <row r="187" spans="1:9">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B187" t="s">
         <v>560</v>
       </c>
@@ -6332,7 +6335,7 @@
         <v xml:space="preserve"> insect </v>
       </c>
     </row>
-    <row r="188" spans="1:9">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B188" t="s">
         <v>561</v>
       </c>
@@ -6348,7 +6351,7 @@
         <v xml:space="preserve"> Souvenirs Entomologiques (a book name written by Jean-Henri Fabre) </v>
       </c>
     </row>
-    <row r="190" spans="1:9" s="5" customFormat="1">
+    <row r="190" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="9" t="s">
         <v>595</v>
       </c>
@@ -6361,10 +6364,10 @@
       <c r="H190" s="12"/>
       <c r="I190" s="10" t="str">
         <f>CONCATENATE(D190," ",E190," ",F190)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="191" spans="1:9">
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B191" t="s">
         <v>596</v>
       </c>
@@ -6388,7 +6391,7 @@
         <v xml:space="preserve"> taking a post (to take a post for high position) (する) ; ရာထူးရယူသည် ; ရာထူးရယူသည္</v>
       </c>
     </row>
-    <row r="192" spans="1:9">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B192" t="s">
         <v>597</v>
       </c>
@@ -6412,7 +6415,7 @@
         <v xml:space="preserve"> growth (to grow) (する) ; ဖွံ့ဖြိုးတိုးတက်သည် ; ဖြံ႔ၿဖိဳးတိုးတက္သည္</v>
       </c>
     </row>
-    <row r="193" spans="1:9">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B193" t="s">
         <v>598</v>
       </c>
@@ -6427,7 +6430,7 @@
         <v xml:space="preserve"> Nobel Prize </v>
       </c>
     </row>
-    <row r="194" spans="1:9">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B194" t="s">
         <v>599</v>
       </c>
@@ -6451,7 +6454,7 @@
         <v xml:space="preserve"> receiving a prize (to receive a prize) (する) ; ဆုလက်ခံရရှိသည် ; ဆုလက္ခံရရွိသည္</v>
       </c>
     </row>
-    <row r="195" spans="1:9">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B195" t="s">
         <v>600</v>
       </c>
@@ -6466,7 +6469,7 @@
         <v xml:space="preserve"> test taker </v>
       </c>
     </row>
-    <row r="196" spans="1:9">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B196" t="s">
         <v>601</v>
       </c>
@@ -6487,7 +6490,7 @@
         <v xml:space="preserve"> involving the whole area/region  ; နယ်မြေတစ်ခုလုံးပါဝင်မှု ; နယ္ေျမတစ္ခုလံုးပါ၀င္မႈ</v>
       </c>
     </row>
-    <row r="197" spans="1:9">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B197" t="s">
         <v>602</v>
       </c>
@@ -6511,7 +6514,7 @@
         <v xml:space="preserve"> opening a port (to open a port) (する) ; (လေယာဉ်၊ သင်္ဘော၊…)ဆိပ်ဖွင့်လှစ်သည် ; (ေလယာဥ္၊ သေဘၤာ၊…)ဆိပ္ဖြင့္လွစ္သည္</v>
       </c>
     </row>
-    <row r="198" spans="1:9">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B198" t="s">
         <v>603</v>
       </c>
@@ -6535,7 +6538,7 @@
         <v>(1,2,…)+ ～anniversary  ; ～နှစ်ပတ်လည် ; ～ႏွစ္ပတ္လည္</v>
       </c>
     </row>
-    <row r="200" spans="1:9" s="5" customFormat="1">
+    <row r="200" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="9" t="s">
         <v>685</v>
       </c>
@@ -6551,7 +6554,7 @@
         <v xml:space="preserve">  </v>
       </c>
     </row>
-    <row r="201" spans="1:9">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B201" t="s">
         <v>604</v>
       </c>
@@ -6566,7 +6569,7 @@
         <v xml:space="preserve"> researching companies </v>
       </c>
     </row>
-    <row r="202" spans="1:9">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B202" t="s">
         <v>636</v>
       </c>
@@ -6590,7 +6593,7 @@
         <v xml:space="preserve"> pastry chef (kana) ; မုန့်အချိုပွဲလုပ်တဲ့သူ ; မုန္႔အခ်ိဳပြဲလုပ္တဲ႔သူ</v>
       </c>
     </row>
-    <row r="203" spans="1:9">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B203" t="s">
         <v>637</v>
       </c>
@@ -6608,7 +6611,7 @@
         <v xml:space="preserve"> contest (kana)</v>
       </c>
     </row>
-    <row r="204" spans="1:9">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B204" t="s">
         <v>638</v>
       </c>
@@ -6632,7 +6635,7 @@
         <v xml:space="preserve"> entry (to enter) (する) ; တက်ရောက်သည် ; တက္ေရာက္သည္</v>
       </c>
     </row>
-    <row r="205" spans="1:9">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B205" t="s">
         <v>639</v>
       </c>
@@ -6647,7 +6650,7 @@
         <v xml:space="preserve"> three-star restaurant </v>
       </c>
     </row>
-    <row r="206" spans="1:9">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B206" t="s">
         <v>640</v>
       </c>
@@ -6668,7 +6671,7 @@
         <v xml:space="preserve"> to handle  ; ကိုင္တြယ္သည္ ; ကိုင္တြယ္သည္</v>
       </c>
     </row>
-    <row r="207" spans="1:9">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B207" t="s">
         <v>641</v>
       </c>
@@ -6689,7 +6692,7 @@
         <v xml:space="preserve"> deadline  ; သတ်မှတ်နောက်ဆုံးနေ့ရက် ; သတ္မွတ္ေနာက္ဆံုးေန႔ရက္</v>
       </c>
     </row>
-    <row r="208" spans="1:9">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B208" t="s">
         <v>642</v>
       </c>
@@ -6710,7 +6713,7 @@
         <v xml:space="preserve"> to meet, be in time  ; အချိန်မီ ဖြစ်စေသည် ; အခ်ိန္မီ ျဖစ္ေစသည္</v>
       </c>
     </row>
-    <row r="209" spans="1:9">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B209" t="s">
         <v>643</v>
       </c>
@@ -6731,7 +6734,7 @@
         <v xml:space="preserve"> pride  ; ဂုဏ်၊ ဂုဏ်ယူခြင်း ; ဂုဏ္၊ ဂုဏ္ယူျခင္း</v>
       </c>
     </row>
-    <row r="210" spans="1:9">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B210" t="s">
         <v>644</v>
       </c>
@@ -6752,7 +6755,7 @@
         <v xml:space="preserve"> to make a full effort  ; အင်အားစိုက်ထုတ်ကြိုးပမ်းသည် ; အင္အားစိုက္ထုတ္ႀကိဳးပမ္းသည္</v>
       </c>
     </row>
-    <row r="211" spans="1:9">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B211" t="s">
         <v>645</v>
       </c>
@@ -6767,7 +6770,7 @@
         <v xml:space="preserve"> tax </v>
       </c>
     </row>
-    <row r="212" spans="1:9">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B212" t="s">
         <v>646</v>
       </c>
@@ -6788,7 +6791,7 @@
         <v xml:space="preserve"> to contest, dispute   ; ယှဉ်ပြိုင်သည်၊ စကားများသည် ; ယွဥ္ၿပိဳင္သည္၊ စကားမ်ားသည္</v>
       </c>
     </row>
-    <row r="214" spans="1:9" s="5" customFormat="1">
+    <row r="214" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" s="9" t="s">
         <v>686</v>
       </c>
@@ -6804,7 +6807,7 @@
         <v xml:space="preserve">  </v>
       </c>
     </row>
-    <row r="215" spans="1:9">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B215" t="s">
         <v>687</v>
       </c>
@@ -6825,7 +6828,7 @@
         <v xml:space="preserve"> one's life  ; တစ်ဘဝလုံး ; တစ္ဘ၀လံုး</v>
       </c>
     </row>
-    <row r="216" spans="1:9">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B216" t="s">
         <v>688</v>
       </c>
@@ -6846,7 +6849,7 @@
         <v xml:space="preserve"> to end  ; ပြီးဆုံးစေသည် ; ၿပီးဆံုးေစသည္</v>
       </c>
     </row>
-    <row r="217" spans="1:9">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B217" t="s">
         <v>689</v>
       </c>
@@ -6867,7 +6870,7 @@
         <v xml:space="preserve"> to overflow  ; လျှံကျသည် ; လွ်ံက်သည္</v>
       </c>
     </row>
-    <row r="218" spans="1:9">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B218" t="s">
         <v>690</v>
       </c>
@@ -6882,7 +6885,7 @@
         <v xml:space="preserve"> business performance </v>
       </c>
     </row>
-    <row r="219" spans="1:9">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B219" t="s">
         <v>691</v>
       </c>
@@ -6903,7 +6906,7 @@
         <v xml:space="preserve"> income  ; ၀င်ငွေ ; ၀င္ေငြ</v>
       </c>
     </row>
-    <row r="220" spans="1:9">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B220" t="s">
         <v>761</v>
       </c>
@@ -6924,7 +6927,7 @@
         <v xml:space="preserve"> expense  ; အသုံးစရိတ် ; အသံုးစရိတ္</v>
       </c>
     </row>
-    <row r="221" spans="1:9">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B221" t="s">
         <v>692</v>
       </c>
@@ -6951,7 +6954,7 @@
         <v>(が) reduction (to reduce) (する) ; လျော့ကျသည် ; ေလ်ာ့က်သည္</v>
       </c>
     </row>
-    <row r="222" spans="1:9">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B222" t="s">
         <v>693</v>
       </c>
@@ -6972,7 +6975,7 @@
         <v xml:space="preserve"> savings  ; စုငွေပမာဏ ; စုေငြပမာဏ</v>
       </c>
     </row>
-    <row r="223" spans="1:9">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B223" t="s">
         <v>694</v>
       </c>
@@ -6999,7 +7002,7 @@
         <v>(が) increase (to increase) (する) ; တိုးပွားသည် ; တိုးပြားသည္</v>
       </c>
     </row>
-    <row r="224" spans="1:9">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B224" t="s">
         <v>695</v>
       </c>
@@ -7014,7 +7017,7 @@
         <v xml:space="preserve"> reality, truth </v>
       </c>
     </row>
-    <row r="225" spans="1:9">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B225" t="s">
         <v>696</v>
       </c>
@@ -7029,7 +7032,7 @@
         <v xml:space="preserve"> freeware </v>
       </c>
     </row>
-    <row r="226" spans="1:9">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B226" t="s">
         <v>697</v>
       </c>
@@ -7044,7 +7047,7 @@
         <v xml:space="preserve"> to be excellent or superior </v>
       </c>
     </row>
-    <row r="227" spans="1:9">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B227" t="s">
         <v>698</v>
       </c>
@@ -7059,7 +7062,7 @@
         <v xml:space="preserve"> a high fever </v>
       </c>
     </row>
-    <row r="228" spans="1:9">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B228" t="s">
         <v>699</v>
       </c>
@@ -7074,7 +7077,7 @@
         <v xml:space="preserve"> weather </v>
       </c>
     </row>
-    <row r="229" spans="1:9">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B229" t="s">
         <v>700</v>
       </c>
@@ -7089,7 +7092,7 @@
         <v xml:space="preserve"> rule </v>
       </c>
     </row>
-    <row r="231" spans="1:9" s="5" customFormat="1">
+    <row r="231" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" s="9" t="s">
         <v>771</v>
       </c>
@@ -7105,7 +7108,7 @@
         <v xml:space="preserve">  </v>
       </c>
     </row>
-    <row r="232" spans="1:9">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B232" t="s">
         <v>701</v>
       </c>
@@ -7120,7 +7123,7 @@
         <v xml:space="preserve"> one member </v>
       </c>
     </row>
-    <row r="233" spans="1:9">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B233" t="s">
         <v>702</v>
       </c>
@@ -7131,17 +7134,17 @@
         <v>748</v>
       </c>
       <c r="G233" s="26" t="s">
+        <v>785</v>
+      </c>
+      <c r="H233" s="26" t="s">
         <v>784</v>
-      </c>
-      <c r="H233" s="26" t="s">
-        <v>783</v>
       </c>
       <c r="I233" s="26" t="str">
         <f t="shared" ref="I233" si="28">CONCATENATE(D233," ",E233," ",F233, " ; ",G233," ; ", H233)</f>
-        <v xml:space="preserve"> mental attitude  ; စိတ်ကြိုတင်ပြင်ဆင်ထားမှု ; စိတ္ႀကိဳတင္ျပင္ဆင္ထားမႈ</v>
-      </c>
-    </row>
-    <row r="234" spans="1:9">
+        <v xml:space="preserve"> mental attitude  ; စိတ်ကြိုတင် ပြင်ဆင်ထားမှု ; စိတ္ႀကိဳတင္ ျပင္ဆင္ထားမႈ</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B234" t="s">
         <v>727</v>
       </c>
@@ -7156,7 +7159,7 @@
         <v xml:space="preserve"> complaint </v>
       </c>
     </row>
-    <row r="235" spans="1:9">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B235" t="s">
         <v>703</v>
       </c>
@@ -7174,7 +7177,7 @@
         <v xml:space="preserve"> dealing with, handling (to deal with, handle) (する)</v>
       </c>
     </row>
-    <row r="236" spans="1:9">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B236" t="s">
         <v>704</v>
       </c>
@@ -7192,7 +7195,7 @@
         <v xml:space="preserve"> complaint (kana)</v>
       </c>
     </row>
-    <row r="237" spans="1:9">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B237" t="s">
         <v>705</v>
       </c>
@@ -7213,7 +7216,7 @@
         <v xml:space="preserve"> justified  ; မှန်ကန်ဖြောင့်မတ်သော ; မွန္ကန္ေျဖာင့္မတ္ေသာ</v>
       </c>
     </row>
-    <row r="238" spans="1:9">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B238" t="s">
         <v>706</v>
       </c>
@@ -7228,7 +7231,7 @@
         <v xml:space="preserve"> uncomfortable </v>
       </c>
     </row>
-    <row r="239" spans="1:9">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B239" t="s">
         <v>707</v>
       </c>
@@ -7243,7 +7246,7 @@
         <v xml:space="preserve"> quality </v>
       </c>
     </row>
-    <row r="240" spans="1:9">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B240" t="s">
         <v>708</v>
       </c>
@@ -7267,7 +7270,7 @@
         <v xml:space="preserve"> pursuit (to pursue) (する) ; ရှာဖွေသည်၊ လေ့လာလိုက်စားသည် ; ရွာေဖြသည္၊ ေလ႔လာလိုက္စားသည္</v>
       </c>
     </row>
-    <row r="243" spans="2:5">
+    <row r="243" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B243" t="s">
         <v>709</v>
       </c>
@@ -7278,7 +7281,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="244" spans="2:5">
+    <row r="244" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B244" t="s">
         <v>710</v>
       </c>

</xml_diff>

<commit_message>
TRY N2 Vocab.xlsx -> Day18, Day19, Day20 words are added.
</commit_message>
<xml_diff>
--- a/preparing/TRY N2 Vocab.xlsx
+++ b/preparing/TRY N2 Vocab.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="904">
   <si>
     <t>お知らせ</t>
   </si>
@@ -2291,9 +2291,6 @@
     <t>Singapore</t>
   </si>
   <si>
-    <t>replacement, proxy</t>
-  </si>
-  <si>
     <t>တစ္ဘ၀လံုး</t>
   </si>
   <si>
@@ -2379,15 +2376,369 @@
   </si>
   <si>
     <t>စိတ်ကြိုတင် ပြင်ဆင်ထားမှု</t>
+  </si>
+  <si>
+    <t>replacement, agency, agent, proxy</t>
+  </si>
+  <si>
+    <t>Day 18</t>
+  </si>
+  <si>
+    <t>企業人</t>
+  </si>
+  <si>
+    <t>自覚</t>
+  </si>
+  <si>
+    <t>サービス料</t>
+  </si>
+  <si>
+    <t>高齢者</t>
+  </si>
+  <si>
+    <t>申請</t>
+  </si>
+  <si>
+    <t>入管</t>
+  </si>
+  <si>
+    <t>実行に移す</t>
+  </si>
+  <si>
+    <t>接近</t>
+  </si>
+  <si>
+    <t>野外コンサート</t>
+  </si>
+  <si>
+    <t>命令</t>
+  </si>
+  <si>
+    <t>従う</t>
+  </si>
+  <si>
+    <t>国民感情</t>
+  </si>
+  <si>
+    <t>防ぐ</t>
+  </si>
+  <si>
+    <t>山奥</t>
+  </si>
+  <si>
+    <t>～に恵まれた</t>
+  </si>
+  <si>
+    <t>宅</t>
+  </si>
+  <si>
+    <t>昨今</t>
+  </si>
+  <si>
+    <t>就職難</t>
+  </si>
+  <si>
+    <t>仕事に就く</t>
+  </si>
+  <si>
+    <t>魅力</t>
+  </si>
+  <si>
+    <t>油絵</t>
+  </si>
+  <si>
+    <t>才能</t>
+  </si>
+  <si>
+    <t>限界</t>
+  </si>
+  <si>
+    <t>やりがいがある</t>
+  </si>
+  <si>
+    <t>見た目</t>
+  </si>
+  <si>
+    <t>business person</t>
+  </si>
+  <si>
+    <t>tip</t>
+  </si>
+  <si>
+    <t>elderly person</t>
+  </si>
+  <si>
+    <t>the national mood</t>
+  </si>
+  <si>
+    <t>deep in the mountains</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>nowadays</t>
+  </si>
+  <si>
+    <t>scarcity of jobs</t>
+  </si>
+  <si>
+    <t>appeal</t>
+  </si>
+  <si>
+    <t>oil painting</t>
+  </si>
+  <si>
+    <t>talent</t>
+  </si>
+  <si>
+    <t>limit</t>
+  </si>
+  <si>
+    <t>rewarding</t>
+  </si>
+  <si>
+    <t>appearance</t>
+  </si>
+  <si>
+    <t>self-awareness (to be aware)</t>
+  </si>
+  <si>
+    <t>application (to apply)</t>
+  </si>
+  <si>
+    <t>Immigration Bureau of Japan</t>
+  </si>
+  <si>
+    <t>to carry out</t>
+  </si>
+  <si>
+    <t>approaching (to approach)</t>
+  </si>
+  <si>
+    <t>outdoor concert</t>
+  </si>
+  <si>
+    <t>order, command (to order, command)</t>
+  </si>
+  <si>
+    <t>to follow, obey</t>
+  </si>
+  <si>
+    <t>to avoid, prevent</t>
+  </si>
+  <si>
+    <t>to be blessed with / have a lot of  ～</t>
+  </si>
+  <si>
+    <t>to get a job</t>
+  </si>
+  <si>
+    <t>きぎょうじん</t>
+  </si>
+  <si>
+    <t>じかく</t>
+  </si>
+  <si>
+    <t>サービスりょう</t>
+  </si>
+  <si>
+    <t>こうれいしゃ</t>
+  </si>
+  <si>
+    <t>しんせい</t>
+  </si>
+  <si>
+    <t>にゅうかん</t>
+  </si>
+  <si>
+    <t>入国管理局</t>
+  </si>
+  <si>
+    <t>(short)</t>
+  </si>
+  <si>
+    <t>(long)</t>
+  </si>
+  <si>
+    <t>にゅうこくかんりきょく</t>
+  </si>
+  <si>
+    <t>じっこうにうつす</t>
+  </si>
+  <si>
+    <t>せっきん</t>
+  </si>
+  <si>
+    <t>やがいコンサート</t>
+  </si>
+  <si>
+    <t>めいれい</t>
+  </si>
+  <si>
+    <t>したがう</t>
+  </si>
+  <si>
+    <t>こくみんかんじょう</t>
+  </si>
+  <si>
+    <t>ふせぐ</t>
+  </si>
+  <si>
+    <t>やまおく</t>
+  </si>
+  <si>
+    <t>～にめぐまれた</t>
+  </si>
+  <si>
+    <t>たく</t>
+  </si>
+  <si>
+    <t>さっこん</t>
+  </si>
+  <si>
+    <t>しゅうしょくなん</t>
+  </si>
+  <si>
+    <t>しごとにつく</t>
+  </si>
+  <si>
+    <t>みりょく</t>
+  </si>
+  <si>
+    <t>あぶらえ</t>
+  </si>
+  <si>
+    <t>さいのう</t>
+  </si>
+  <si>
+    <t>げんかい</t>
+  </si>
+  <si>
+    <t>みため</t>
+  </si>
+  <si>
+    <t>ကိုယ့္ကိုကိုယ္ နားလည္သည္</t>
+  </si>
+  <si>
+    <t>(visaを)</t>
+  </si>
+  <si>
+    <t>တကယ္ အေကာင္အထည္ ေဖာ္သည္</t>
+  </si>
+  <si>
+    <t>ခ်ဥ္းကပ္သည္</t>
+  </si>
+  <si>
+    <t>ျပည္သူ႔ဆႏၵ</t>
+  </si>
+  <si>
+    <t>ႀကိဳတင္ ကာကြယ္သည္</t>
+  </si>
+  <si>
+    <t>လူသြားလူလာ နည္းတဲ႔ ေတာင္ႀကိဳ ေတာင္ၾကား</t>
+  </si>
+  <si>
+    <t>ေကာင္းခ်ီးေပးခံရသည္</t>
+  </si>
+  <si>
+    <t>ခုတေလာ</t>
+  </si>
+  <si>
+    <t>အလုပ္ေတာ္ေတာ္နဲ႔မရျခင္း</t>
+  </si>
+  <si>
+    <t>အလုပ္ရျခင္း</t>
+  </si>
+  <si>
+    <t>ဆြဲေဆာင္မႈ</t>
+  </si>
+  <si>
+    <t>ဆီေဆးပန္းခ်ီ</t>
+  </si>
+  <si>
+    <t>水彩画</t>
+  </si>
+  <si>
+    <t>すいさいが</t>
+  </si>
+  <si>
+    <t>ေရေဆးပန္းခ်ီ</t>
+  </si>
+  <si>
+    <t>watercolor painting</t>
+  </si>
+  <si>
+    <t>ပင္ကိုစြမ္းရည္၊ ပါရမီ</t>
+  </si>
+  <si>
+    <t>ကန္႔သတ္ခ်က္</t>
+  </si>
+  <si>
+    <t>အက်ိဳးေက်းဇူးရွိသည္</t>
+  </si>
+  <si>
+    <t>Day 19</t>
+  </si>
+  <si>
+    <t>Day 20</t>
+  </si>
+  <si>
+    <t>ကိုယ့်ကိုကိုယ် နားလည်သည်</t>
+  </si>
+  <si>
+    <t>တကယ် အကောင်အထည် ဖော်သည်</t>
+  </si>
+  <si>
+    <t>ချဉ်းကပ်သည်</t>
+  </si>
+  <si>
+    <t>ပြည်သူ့ဆန္ဒ</t>
+  </si>
+  <si>
+    <t>ကြိုတင် ကာကွယ်သည်</t>
+  </si>
+  <si>
+    <t>လူသွားလူလာ နည်းတဲ့ တောင်ကြို တောင်ကြား</t>
+  </si>
+  <si>
+    <t>ကောင်းချီးပေးခံရသည်</t>
+  </si>
+  <si>
+    <t>ခုတလော</t>
+  </si>
+  <si>
+    <t>အလုပ်တော်တော်နဲ့မရခြင်း</t>
+  </si>
+  <si>
+    <t>အလုပ်ရခြင်း</t>
+  </si>
+  <si>
+    <t>ဆွဲဆောင်မှု</t>
+  </si>
+  <si>
+    <t>ဆီဆေးပန်းချီ</t>
+  </si>
+  <si>
+    <t>ရေဆေးပန်းချီ</t>
+  </si>
+  <si>
+    <t>ပင်ကိုစွမ်းရည်၊ ပါရမီ</t>
+  </si>
+  <si>
+    <t>ကန့်သတ်ချက်</t>
+  </si>
+  <si>
+    <t>အကျိုးကျေးဇူးရှိသည်</t>
+  </si>
+  <si>
+    <t>Day18, Day19, Day20 added</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-10000455]0"/>
-  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2488,7 +2839,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2558,9 +2909,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2868,8 +3216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3171,11 +3519,11 @@
         <v>186</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="27">
+      <c r="B23" s="14">
         <v>20</v>
       </c>
       <c r="C23" s="15">
@@ -3185,14 +3533,22 @@
         <v>186</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="23"/>
+      <c r="B24" s="14">
+        <v>21</v>
+      </c>
+      <c r="C24" s="15">
+        <v>43517</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>903</v>
+      </c>
     </row>
     <row r="25" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="14"/>
@@ -3237,22 +3593,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I244"/>
+  <dimension ref="A1:I277"/>
   <sheetViews>
-    <sheetView topLeftCell="A227" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G233" sqref="G233:I233"/>
+    <sheetView topLeftCell="A260" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B273" sqref="B273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" customWidth="1"/>
-    <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" customWidth="1"/>
-    <col min="7" max="7" width="27" style="10" customWidth="1"/>
-    <col min="8" max="8" width="15" style="10" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="10" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" style="10" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6818,10 +7174,10 @@
         <v>733</v>
       </c>
       <c r="G215" s="10" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H215" s="10" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="I215" s="10" t="str">
         <f t="shared" ref="I215:I217" si="24">CONCATENATE(D215," ",E215," ",F215, " ; ",G215," ; ", H215)</f>
@@ -6839,10 +7195,10 @@
         <v>734</v>
       </c>
       <c r="G216" s="10" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H216" s="10" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="I216" s="10" t="str">
         <f t="shared" si="24"/>
@@ -6860,10 +7216,10 @@
         <v>735</v>
       </c>
       <c r="G217" s="10" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H217" s="10" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="I217" s="10" t="str">
         <f t="shared" si="24"/>
@@ -6896,10 +7252,10 @@
         <v>737</v>
       </c>
       <c r="G219" s="10" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="H219" s="10" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="I219" s="10" t="str">
         <f t="shared" ref="I219:I223" si="25">CONCATENATE(D219," ",E219," ",F219, " ; ",G219," ; ", H219)</f>
@@ -6908,19 +7264,19 @@
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B220" t="s">
+        <v>760</v>
+      </c>
+      <c r="C220" t="s">
         <v>761</v>
       </c>
-      <c r="C220" t="s">
+      <c r="E220" t="s">
         <v>762</v>
       </c>
-      <c r="E220" t="s">
+      <c r="G220" s="10" t="s">
+        <v>775</v>
+      </c>
+      <c r="H220" s="10" t="s">
         <v>763</v>
-      </c>
-      <c r="G220" s="10" t="s">
-        <v>776</v>
-      </c>
-      <c r="H220" s="10" t="s">
-        <v>764</v>
       </c>
       <c r="I220" s="10" t="str">
         <f t="shared" si="25"/>
@@ -6935,7 +7291,7 @@
         <v>715</v>
       </c>
       <c r="D221" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E221" t="s">
         <v>738</v>
@@ -6944,10 +7300,10 @@
         <v>15</v>
       </c>
       <c r="G221" s="10" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="H221" s="10" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="I221" s="10" t="str">
         <f t="shared" si="25"/>
@@ -6965,10 +7321,10 @@
         <v>739</v>
       </c>
       <c r="G222" s="10" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="H222" s="10" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="I222" s="10" t="str">
         <f t="shared" si="25"/>
@@ -6983,7 +7339,7 @@
         <v>717</v>
       </c>
       <c r="D223" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E223" t="s">
         <v>740</v>
@@ -6992,10 +7348,10 @@
         <v>15</v>
       </c>
       <c r="G223" s="10" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="H223" s="10" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="I223" s="10" t="str">
         <f t="shared" si="25"/>
@@ -7094,7 +7450,7 @@
     </row>
     <row r="231" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" s="9" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="B231" s="6"/>
       <c r="C231" s="6"/>
@@ -7134,10 +7490,10 @@
         <v>748</v>
       </c>
       <c r="G233" s="26" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="H233" s="26" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I233" s="26" t="str">
         <f t="shared" ref="I233" si="28">CONCATENATE(D233," ",E233," ",F233, " ; ",G233," ; ", H233)</f>
@@ -7206,10 +7562,10 @@
         <v>751</v>
       </c>
       <c r="G237" s="10" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H237" s="10" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="I237" s="10" t="str">
         <f t="shared" ref="I237" si="29">CONCATENATE(D237," ",E237," ",F237, " ; ",G237," ; ", H237)</f>
@@ -7260,17 +7616,33 @@
         <v>15</v>
       </c>
       <c r="G240" s="10" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H240" s="10" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="I240" s="10" t="str">
         <f t="shared" ref="I240" si="31">CONCATENATE(D240," ",E240," ",F240, " ; ",G240," ; ", H240)</f>
         <v xml:space="preserve"> pursuit (to pursue) (する) ; ရှာဖွေသည်၊ လေ့လာလိုက်စားသည် ; ရွာေဖြသည္၊ ေလ႔လာလိုက္စားသည္</v>
       </c>
     </row>
-    <row r="243" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A242" s="9" t="s">
+        <v>786</v>
+      </c>
+      <c r="B242" s="6"/>
+      <c r="C242" s="6"/>
+      <c r="D242" s="7"/>
+      <c r="E242" s="6"/>
+      <c r="F242" s="7"/>
+      <c r="G242" s="12"/>
+      <c r="H242" s="12"/>
+      <c r="I242" s="10" t="str">
+        <f>CONCATENATE(D242," ",E242," ",F242)</f>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B243" t="s">
         <v>709</v>
       </c>
@@ -7280,8 +7652,12 @@
       <c r="E243" t="s">
         <v>755</v>
       </c>
-    </row>
-    <row r="244" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="I243" s="10" t="str">
+        <f t="shared" ref="I243:I251" si="32">CONCATENATE(D243," ",E243," ",F243)</f>
+        <v xml:space="preserve"> Singapore </v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B244" t="s">
         <v>710</v>
       </c>
@@ -7289,7 +7665,561 @@
         <v>732</v>
       </c>
       <c r="E244" t="s">
-        <v>756</v>
+        <v>785</v>
+      </c>
+      <c r="I244" s="10" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve"> replacement, agency, agent, proxy </v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B245" t="s">
+        <v>787</v>
+      </c>
+      <c r="C245" t="s">
+        <v>837</v>
+      </c>
+      <c r="E245" t="s">
+        <v>812</v>
+      </c>
+      <c r="I245" s="10" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve"> business person </v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B246" t="s">
+        <v>788</v>
+      </c>
+      <c r="C246" t="s">
+        <v>838</v>
+      </c>
+      <c r="E246" t="s">
+        <v>826</v>
+      </c>
+      <c r="F246" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G246" s="10" t="s">
+        <v>887</v>
+      </c>
+      <c r="H246" s="10" t="s">
+        <v>865</v>
+      </c>
+      <c r="I246" s="10" t="str">
+        <f t="shared" ref="I246" si="33">CONCATENATE(D246," ",E246," ",F246, " ; ",G246," ; ", H246)</f>
+        <v xml:space="preserve"> self-awareness (to be aware) (する) ; ကိုယ့်ကိုကိုယ် နားလည်သည် ; ကိုယ့္ကိုကိုယ္ နားလည္သည္</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B247" t="s">
+        <v>789</v>
+      </c>
+      <c r="C247" t="s">
+        <v>839</v>
+      </c>
+      <c r="E247" t="s">
+        <v>813</v>
+      </c>
+      <c r="I247" s="10" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve"> tip </v>
+      </c>
+    </row>
+    <row r="248" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B248" t="s">
+        <v>790</v>
+      </c>
+      <c r="C248" t="s">
+        <v>840</v>
+      </c>
+      <c r="E248" t="s">
+        <v>814</v>
+      </c>
+      <c r="I248" s="10" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve"> elderly person </v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B249" t="s">
+        <v>791</v>
+      </c>
+      <c r="C249" t="s">
+        <v>841</v>
+      </c>
+      <c r="D249" t="s">
+        <v>866</v>
+      </c>
+      <c r="E249" t="s">
+        <v>827</v>
+      </c>
+      <c r="F249" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I249" s="10" t="str">
+        <f t="shared" si="32"/>
+        <v>(visaを) application (to apply) (する)</v>
+      </c>
+    </row>
+    <row r="250" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B250" t="s">
+        <v>792</v>
+      </c>
+      <c r="C250" t="s">
+        <v>842</v>
+      </c>
+      <c r="D250" t="s">
+        <v>844</v>
+      </c>
+      <c r="E250" t="s">
+        <v>828</v>
+      </c>
+      <c r="I250" s="10" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">(short) Immigration Bureau of Japan </v>
+      </c>
+    </row>
+    <row r="251" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B251" t="s">
+        <v>843</v>
+      </c>
+      <c r="C251" t="s">
+        <v>846</v>
+      </c>
+      <c r="D251" t="s">
+        <v>845</v>
+      </c>
+      <c r="E251" t="s">
+        <v>828</v>
+      </c>
+      <c r="I251" s="10" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">(long) Immigration Bureau of Japan </v>
+      </c>
+    </row>
+    <row r="252" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B252" t="s">
+        <v>793</v>
+      </c>
+      <c r="C252" t="s">
+        <v>847</v>
+      </c>
+      <c r="E252" t="s">
+        <v>829</v>
+      </c>
+      <c r="G252" s="10" t="s">
+        <v>888</v>
+      </c>
+      <c r="H252" s="10" t="s">
+        <v>867</v>
+      </c>
+      <c r="I252" s="10" t="str">
+        <f t="shared" ref="I252" si="34">CONCATENATE(D252," ",E252," ",F252, " ; ",G252," ; ", H252)</f>
+        <v xml:space="preserve"> to carry out  ; တကယ် အကောင်အထည် ဖော်သည် ; တကယ္ အေကာင္အထည္ ေဖာ္သည္</v>
+      </c>
+    </row>
+    <row r="254" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A254" s="9" t="s">
+        <v>885</v>
+      </c>
+      <c r="B254" s="6"/>
+      <c r="C254" s="6"/>
+      <c r="D254" s="7"/>
+      <c r="E254" s="6"/>
+      <c r="F254" s="7"/>
+      <c r="G254" s="12"/>
+      <c r="H254" s="12"/>
+      <c r="I254" s="10" t="str">
+        <f>CONCATENATE(D254," ",E254," ",F254)</f>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="255" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B255" t="s">
+        <v>794</v>
+      </c>
+      <c r="C255" t="s">
+        <v>848</v>
+      </c>
+      <c r="E255" t="s">
+        <v>830</v>
+      </c>
+      <c r="F255" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G255" s="10" t="s">
+        <v>889</v>
+      </c>
+      <c r="H255" s="10" t="s">
+        <v>868</v>
+      </c>
+      <c r="I255" s="10" t="str">
+        <f t="shared" ref="I255" si="35">CONCATENATE(D255," ",E255," ",F255, " ; ",G255," ; ", H255)</f>
+        <v xml:space="preserve"> approaching (to approach) (する) ; ချဉ်းကပ်သည် ; ခ်ဥ္းကပ္သည္</v>
+      </c>
+    </row>
+    <row r="256" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B256" t="s">
+        <v>795</v>
+      </c>
+      <c r="C256" t="s">
+        <v>849</v>
+      </c>
+      <c r="E256" t="s">
+        <v>831</v>
+      </c>
+      <c r="I256" s="10" t="str">
+        <f t="shared" ref="I256:I258" si="36">CONCATENATE(D256," ",E256," ",F256)</f>
+        <v xml:space="preserve"> outdoor concert </v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B257" t="s">
+        <v>796</v>
+      </c>
+      <c r="C257" t="s">
+        <v>850</v>
+      </c>
+      <c r="E257" t="s">
+        <v>832</v>
+      </c>
+      <c r="F257" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I257" s="10" t="str">
+        <f t="shared" si="36"/>
+        <v xml:space="preserve"> order, command (to order, command) (する)</v>
+      </c>
+    </row>
+    <row r="258" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B258" t="s">
+        <v>797</v>
+      </c>
+      <c r="C258" t="s">
+        <v>851</v>
+      </c>
+      <c r="E258" t="s">
+        <v>833</v>
+      </c>
+      <c r="I258" s="10" t="str">
+        <f t="shared" si="36"/>
+        <v xml:space="preserve"> to follow, obey </v>
+      </c>
+    </row>
+    <row r="259" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B259" t="s">
+        <v>798</v>
+      </c>
+      <c r="C259" t="s">
+        <v>852</v>
+      </c>
+      <c r="E259" t="s">
+        <v>815</v>
+      </c>
+      <c r="G259" s="10" t="s">
+        <v>890</v>
+      </c>
+      <c r="H259" s="10" t="s">
+        <v>869</v>
+      </c>
+      <c r="I259" s="10" t="str">
+        <f t="shared" ref="I259" si="37">CONCATENATE(D259," ",E259," ",F259, " ; ",G259," ; ", H259)</f>
+        <v xml:space="preserve"> the national mood  ; ပြည်သူ့ဆန္ဒ ; ျပည္သူ႔ဆႏၵ</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A261" s="9" t="s">
+        <v>886</v>
+      </c>
+      <c r="B261" s="6"/>
+      <c r="C261" s="6"/>
+      <c r="D261" s="7"/>
+      <c r="E261" s="6"/>
+      <c r="F261" s="7"/>
+      <c r="G261" s="12"/>
+      <c r="H261" s="12"/>
+      <c r="I261" s="10" t="str">
+        <f>CONCATENATE(D261," ",E261," ",F261)</f>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B262" t="s">
+        <v>799</v>
+      </c>
+      <c r="C262" t="s">
+        <v>853</v>
+      </c>
+      <c r="E262" t="s">
+        <v>834</v>
+      </c>
+      <c r="G262" s="10" t="s">
+        <v>891</v>
+      </c>
+      <c r="H262" s="10" t="s">
+        <v>870</v>
+      </c>
+      <c r="I262" s="10" t="str">
+        <f t="shared" ref="I262:I264" si="38">CONCATENATE(D262," ",E262," ",F262, " ; ",G262," ; ", H262)</f>
+        <v xml:space="preserve"> to avoid, prevent  ; ကြိုတင် ကာကွယ်သည် ; ႀကိဳတင္ ကာကြယ္သည္</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B263" t="s">
+        <v>800</v>
+      </c>
+      <c r="C263" t="s">
+        <v>854</v>
+      </c>
+      <c r="E263" t="s">
+        <v>816</v>
+      </c>
+      <c r="G263" s="10" t="s">
+        <v>892</v>
+      </c>
+      <c r="H263" s="10" t="s">
+        <v>871</v>
+      </c>
+      <c r="I263" s="10" t="str">
+        <f t="shared" si="38"/>
+        <v xml:space="preserve"> deep in the mountains  ; လူသွားလူလာ နည်းတဲ့ တောင်ကြို တောင်ကြား ; လူသြားလူလာ နည္းတဲ႔ ေတာင္ႀကိဳ ေတာင္ၾကား</v>
+      </c>
+    </row>
+    <row r="264" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B264" t="s">
+        <v>801</v>
+      </c>
+      <c r="C264" t="s">
+        <v>855</v>
+      </c>
+      <c r="E264" t="s">
+        <v>835</v>
+      </c>
+      <c r="G264" s="10" t="s">
+        <v>893</v>
+      </c>
+      <c r="H264" s="10" t="s">
+        <v>872</v>
+      </c>
+      <c r="I264" s="10" t="str">
+        <f t="shared" si="38"/>
+        <v xml:space="preserve"> to be blessed with / have a lot of  ～  ; ကောင်းချီးပေးခံရသည် ; ေကာင္းခ်ီးေပးခံရသည္</v>
+      </c>
+    </row>
+    <row r="265" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B265" t="s">
+        <v>802</v>
+      </c>
+      <c r="C265" t="s">
+        <v>856</v>
+      </c>
+      <c r="E265" t="s">
+        <v>817</v>
+      </c>
+      <c r="I265" s="10" t="str">
+        <f t="shared" ref="I265" si="39">CONCATENATE(D265," ",E265," ",F265)</f>
+        <v xml:space="preserve"> home </v>
+      </c>
+    </row>
+    <row r="266" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B266" t="s">
+        <v>803</v>
+      </c>
+      <c r="C266" t="s">
+        <v>857</v>
+      </c>
+      <c r="E266" t="s">
+        <v>818</v>
+      </c>
+      <c r="G266" s="10" t="s">
+        <v>894</v>
+      </c>
+      <c r="H266" s="10" t="s">
+        <v>873</v>
+      </c>
+      <c r="I266" s="10" t="str">
+        <f t="shared" ref="I266:I273" si="40">CONCATENATE(D266," ",E266," ",F266, " ; ",G266," ; ", H266)</f>
+        <v xml:space="preserve"> nowadays  ; ခုတလော ; ခုတေလာ</v>
+      </c>
+    </row>
+    <row r="267" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B267" t="s">
+        <v>804</v>
+      </c>
+      <c r="C267" t="s">
+        <v>858</v>
+      </c>
+      <c r="E267" t="s">
+        <v>819</v>
+      </c>
+      <c r="G267" s="10" t="s">
+        <v>895</v>
+      </c>
+      <c r="H267" s="10" t="s">
+        <v>874</v>
+      </c>
+      <c r="I267" s="10" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve"> scarcity of jobs  ; အလုပ်တော်တော်နဲ့မရခြင်း ; အလုပ္ေတာ္ေတာ္နဲ႔မရျခင္း</v>
+      </c>
+    </row>
+    <row r="268" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B268" t="s">
+        <v>805</v>
+      </c>
+      <c r="C268" t="s">
+        <v>859</v>
+      </c>
+      <c r="E268" t="s">
+        <v>836</v>
+      </c>
+      <c r="G268" s="10" t="s">
+        <v>896</v>
+      </c>
+      <c r="H268" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="I268" s="10" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve"> to get a job  ; အလုပ်ရခြင်း ; အလုပ္ရျခင္း</v>
+      </c>
+    </row>
+    <row r="269" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B269" t="s">
+        <v>806</v>
+      </c>
+      <c r="C269" t="s">
+        <v>860</v>
+      </c>
+      <c r="E269" t="s">
+        <v>820</v>
+      </c>
+      <c r="G269" s="10" t="s">
+        <v>897</v>
+      </c>
+      <c r="H269" s="10" t="s">
+        <v>876</v>
+      </c>
+      <c r="I269" s="10" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve"> appeal  ; ဆွဲဆောင်မှု ; ဆြဲေဆာင္မႈ</v>
+      </c>
+    </row>
+    <row r="270" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B270" t="s">
+        <v>807</v>
+      </c>
+      <c r="C270" t="s">
+        <v>861</v>
+      </c>
+      <c r="E270" t="s">
+        <v>821</v>
+      </c>
+      <c r="G270" s="10" t="s">
+        <v>898</v>
+      </c>
+      <c r="H270" s="10" t="s">
+        <v>877</v>
+      </c>
+      <c r="I270" s="10" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve"> oil painting  ; ဆီဆေးပန်းချီ ; ဆီေဆးပန္းခ်ီ</v>
+      </c>
+    </row>
+    <row r="271" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B271" t="s">
+        <v>878</v>
+      </c>
+      <c r="C271" t="s">
+        <v>879</v>
+      </c>
+      <c r="E271" t="s">
+        <v>881</v>
+      </c>
+      <c r="G271" s="10" t="s">
+        <v>899</v>
+      </c>
+      <c r="H271" s="10" t="s">
+        <v>880</v>
+      </c>
+      <c r="I271" s="10" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve"> watercolor painting  ; ရေဆေးပန်းချီ ; ေရေဆးပန္းခ်ီ</v>
+      </c>
+    </row>
+    <row r="272" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B272" t="s">
+        <v>808</v>
+      </c>
+      <c r="C272" t="s">
+        <v>862</v>
+      </c>
+      <c r="E272" t="s">
+        <v>822</v>
+      </c>
+      <c r="G272" s="10" t="s">
+        <v>900</v>
+      </c>
+      <c r="H272" s="10" t="s">
+        <v>882</v>
+      </c>
+      <c r="I272" s="10" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve"> talent  ; ပင်ကိုစွမ်းရည်၊ ပါရမီ ; ပင္ကိုစြမ္းရည္၊ ပါရမီ</v>
+      </c>
+    </row>
+    <row r="273" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B273" t="s">
+        <v>809</v>
+      </c>
+      <c r="C273" t="s">
+        <v>863</v>
+      </c>
+      <c r="E273" t="s">
+        <v>823</v>
+      </c>
+      <c r="G273" s="10" t="s">
+        <v>901</v>
+      </c>
+      <c r="H273" s="10" t="s">
+        <v>883</v>
+      </c>
+      <c r="I273" s="10" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve"> limit  ; ကန့်သတ်ချက် ; ကန္႔သတ္ခ်က္</v>
+      </c>
+    </row>
+    <row r="276" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B276" t="s">
+        <v>810</v>
+      </c>
+      <c r="C276" t="s">
+        <v>810</v>
+      </c>
+      <c r="E276" t="s">
+        <v>824</v>
+      </c>
+      <c r="G276" s="10" t="s">
+        <v>902</v>
+      </c>
+      <c r="H276" s="10" t="s">
+        <v>884</v>
+      </c>
+      <c r="I276" s="10" t="str">
+        <f t="shared" ref="I276" si="41">CONCATENATE(D276," ",E276," ",F276, " ; ",G276," ; ", H276)</f>
+        <v xml:space="preserve"> rewarding  ; အကျိုးကျေးဇူးရှိသည် ; အက်ိဳးေက်းဇူးရွိသည္</v>
+      </c>
+    </row>
+    <row r="277" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B277" t="s">
+        <v>811</v>
+      </c>
+      <c r="C277" t="s">
+        <v>864</v>
+      </c>
+      <c r="E277" t="s">
+        <v>825</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TRY N2 Vocab.xlsx -> Day21, Day22, Day23 words are added.
</commit_message>
<xml_diff>
--- a/preparing/TRY N2 Vocab.xlsx
+++ b/preparing/TRY N2 Vocab.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="904">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="997">
   <si>
     <t>お知らせ</t>
   </si>
@@ -2733,6 +2733,285 @@
   </si>
   <si>
     <t>Day18, Day19, Day20 added</t>
+  </si>
+  <si>
+    <t>戦う</t>
+  </si>
+  <si>
+    <t>出演者</t>
+  </si>
+  <si>
+    <t>話題になる</t>
+  </si>
+  <si>
+    <t>特集</t>
+  </si>
+  <si>
+    <t>興味深い</t>
+  </si>
+  <si>
+    <t>配慮</t>
+  </si>
+  <si>
+    <t>骨折</t>
+  </si>
+  <si>
+    <t>悪用</t>
+  </si>
+  <si>
+    <t>詐欺</t>
+  </si>
+  <si>
+    <t>悪化</t>
+  </si>
+  <si>
+    <t>にぎわう</t>
+  </si>
+  <si>
+    <t>女優</t>
+  </si>
+  <si>
+    <t>仕上げる</t>
+  </si>
+  <si>
+    <t>甘える</t>
+  </si>
+  <si>
+    <t>海上</t>
+  </si>
+  <si>
+    <t>気圧</t>
+  </si>
+  <si>
+    <t>ヘクトパスカル</t>
+  </si>
+  <si>
+    <t>最大瞬間風速</t>
+  </si>
+  <si>
+    <t>暴風域</t>
+  </si>
+  <si>
+    <t>広範囲</t>
+  </si>
+  <si>
+    <t>沿岸</t>
+  </si>
+  <si>
+    <t>たたかう</t>
+  </si>
+  <si>
+    <t>しゅつえんしゃ</t>
+  </si>
+  <si>
+    <t>わだいになる</t>
+  </si>
+  <si>
+    <t>とくしゅう</t>
+  </si>
+  <si>
+    <t>きょうみぶかい</t>
+  </si>
+  <si>
+    <t>はいりょ</t>
+  </si>
+  <si>
+    <t>こっせつ</t>
+  </si>
+  <si>
+    <t>あくよう</t>
+  </si>
+  <si>
+    <t>さぎ</t>
+  </si>
+  <si>
+    <t>あっか</t>
+  </si>
+  <si>
+    <t>デビュー</t>
+  </si>
+  <si>
+    <t>じょゆう</t>
+  </si>
+  <si>
+    <t>しあげる</t>
+  </si>
+  <si>
+    <t>あまえる</t>
+  </si>
+  <si>
+    <t>かいじょう</t>
+  </si>
+  <si>
+    <t>きあつ</t>
+  </si>
+  <si>
+    <t>さいだいしゅんかんふうそく</t>
+  </si>
+  <si>
+    <t>ぼうふういき</t>
+  </si>
+  <si>
+    <t>こうはんい</t>
+  </si>
+  <si>
+    <t>えんがん</t>
+  </si>
+  <si>
+    <t>Day 21</t>
+  </si>
+  <si>
+    <t>Day 22</t>
+  </si>
+  <si>
+    <t>Day 23</t>
+  </si>
+  <si>
+    <t>performer, cast member</t>
+  </si>
+  <si>
+    <t>feature article</t>
+  </si>
+  <si>
+    <t>fraud</t>
+  </si>
+  <si>
+    <t>debut (to debut)</t>
+  </si>
+  <si>
+    <t>actress</t>
+  </si>
+  <si>
+    <t>on the ocean</t>
+  </si>
+  <si>
+    <t>air pressure</t>
+  </si>
+  <si>
+    <t>maximum wind speed</t>
+  </si>
+  <si>
+    <t>storm area</t>
+  </si>
+  <si>
+    <t>wide range</t>
+  </si>
+  <si>
+    <t>to try hard; to fight</t>
+  </si>
+  <si>
+    <t>to get in the news</t>
+  </si>
+  <si>
+    <t>deeply interesting</t>
+  </si>
+  <si>
+    <t>consideration (to be considerate)</t>
+  </si>
+  <si>
+    <t>breaking a bone (to break a bone)</t>
+  </si>
+  <si>
+    <t>malicious use (to use maliciously)</t>
+  </si>
+  <si>
+    <t>worsening (to become worse)</t>
+  </si>
+  <si>
+    <t>to be lively, bustle</t>
+  </si>
+  <si>
+    <t>to finish up</t>
+  </si>
+  <si>
+    <t>to be coddled</t>
+  </si>
+  <si>
+    <t>ေျပာစရာေခါင္းစဥ္ ျဖစ္လာသည္</t>
+  </si>
+  <si>
+    <t>ကိုယ္ခ်င္းစာ စဥ္းစားေပးသည္</t>
+  </si>
+  <si>
+    <t>မေကာင္းတဲ႔ေနရာ အသံုးခ်သည္</t>
+  </si>
+  <si>
+    <t>လွည့္ျဖားၿပီး ေငြရယူျခင္း</t>
+  </si>
+  <si>
+    <t>ဆိုး၀ါးလာသည္</t>
+  </si>
+  <si>
+    <t>စည္ကားသည္</t>
+  </si>
+  <si>
+    <t>(မင္းသား၊ မင္းသမီး) ပြဲထုတ္သည္</t>
+  </si>
+  <si>
+    <t>အၿပီးသတ္သည္</t>
+  </si>
+  <si>
+    <t>hectopascal</t>
+  </si>
+  <si>
+    <t>အခ်ိန္တိုအတြင္း အျမန္ဆံုး ေလတိုက္ႏႈန္း</t>
+  </si>
+  <si>
+    <t>က်ယ္ျပန္႔တဲ႔ ဧရိယာ</t>
+  </si>
+  <si>
+    <t>ကမ္းစပ္</t>
+  </si>
+  <si>
+    <t xml:space="preserve">approaching (to approach) </t>
+  </si>
+  <si>
+    <t>နီးကပ္လာသည္</t>
+  </si>
+  <si>
+    <t>အသြင္အျပင္</t>
+  </si>
+  <si>
+    <t>အသွင်အပြင်</t>
+  </si>
+  <si>
+    <t>ပြောစရာခေါင်းစဉ် ဖြစ်လာသည်</t>
+  </si>
+  <si>
+    <t>ကိုယ်ချင်းစာ စဉ်းစားပေးသည်</t>
+  </si>
+  <si>
+    <t>မကောင်းတဲ့နေရာ အသုံးချသည်</t>
+  </si>
+  <si>
+    <t>လှည့်ဖြားပြီး ငွေရယူခြင်း</t>
+  </si>
+  <si>
+    <t>ဆိုးဝါးလာသည်</t>
+  </si>
+  <si>
+    <t>စည်ကားသည်</t>
+  </si>
+  <si>
+    <t>(မင်းသား၊ မင်းသမီး) ပွဲထုတ်သည်</t>
+  </si>
+  <si>
+    <t>အပြီးသတ်သည်</t>
+  </si>
+  <si>
+    <t>အချိန်တိုအတွင်း အမြန်ဆုံး လေတိုက်နှုန်း</t>
+  </si>
+  <si>
+    <t>ကျယ်ပြန့်တဲ့ ဧရိယာ</t>
+  </si>
+  <si>
+    <t>ကမ်းစပ်</t>
+  </si>
+  <si>
+    <t>နီးကပ်လာသည်</t>
+  </si>
+  <si>
+    <t>Day21, Day22, Day23 added</t>
   </si>
 </sst>
 </file>
@@ -3217,7 +3496,7 @@
   <dimension ref="B2:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3551,10 +3830,18 @@
       </c>
     </row>
     <row r="25" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="23"/>
+      <c r="B25" s="14">
+        <v>22</v>
+      </c>
+      <c r="C25" s="15">
+        <v>43528</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>996</v>
+      </c>
     </row>
     <row r="26" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
@@ -3593,10 +3880,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I277"/>
+  <dimension ref="A1:I305"/>
   <sheetViews>
-    <sheetView topLeftCell="A260" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B273" sqref="B273"/>
+    <sheetView topLeftCell="A293" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B305" sqref="B305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.55000000000000004"/>
@@ -5649,7 +5936,7 @@
         <v xml:space="preserve"> to learn, acquire; to put on </v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="34.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:9" ht="49.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B128" t="s">
         <v>368</v>
       </c>
@@ -5888,7 +6175,7 @@
         <v xml:space="preserve"> shop </v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:9" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B142" t="s">
         <v>403</v>
       </c>
@@ -6285,7 +6572,7 @@
         <v xml:space="preserve"> enlargement (to enlarge) (する)</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:9" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B165" t="s">
         <v>423</v>
       </c>
@@ -7027,7 +7314,7 @@
         <v xml:space="preserve"> to handle  ; ကိုင္တြယ္သည္ ; ကိုင္တြယ္သည္</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:9" ht="43.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B207" t="s">
         <v>641</v>
       </c>
@@ -8169,7 +8456,7 @@
         <v xml:space="preserve"> talent  ; ပင်ကိုစွမ်းရည်၊ ပါရမီ ; ပင္ကိုစြမ္းရည္၊ ပါရမီ</v>
       </c>
     </row>
-    <row r="273" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B273" t="s">
         <v>809</v>
       </c>
@@ -8190,7 +8477,23 @@
         <v xml:space="preserve"> limit  ; ကန့်သတ်ချက် ; ကန္႔သတ္ခ်က္</v>
       </c>
     </row>
-    <row r="276" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="275" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A275" s="9" t="s">
+        <v>945</v>
+      </c>
+      <c r="B275" s="6"/>
+      <c r="C275" s="6"/>
+      <c r="D275" s="7"/>
+      <c r="E275" s="6"/>
+      <c r="F275" s="7"/>
+      <c r="G275" s="12"/>
+      <c r="H275" s="12"/>
+      <c r="I275" s="10" t="str">
+        <f>CONCATENATE(D275," ",E275," ",F275)</f>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B276" t="s">
         <v>810</v>
       </c>
@@ -8207,11 +8510,11 @@
         <v>884</v>
       </c>
       <c r="I276" s="10" t="str">
-        <f t="shared" ref="I276" si="41">CONCATENATE(D276," ",E276," ",F276, " ; ",G276," ; ", H276)</f>
+        <f t="shared" ref="I276:I277" si="41">CONCATENATE(D276," ",E276," ",F276, " ; ",G276," ; ", H276)</f>
         <v xml:space="preserve"> rewarding  ; အကျိုးကျေးဇူးရှိသည် ; အက်ိဳးေက်းဇူးရွိသည္</v>
       </c>
     </row>
-    <row r="277" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B277" t="s">
         <v>811</v>
       </c>
@@ -8220,6 +8523,501 @@
       </c>
       <c r="E277" t="s">
         <v>825</v>
+      </c>
+      <c r="G277" s="10" t="s">
+        <v>983</v>
+      </c>
+      <c r="H277" s="10" t="s">
+        <v>982</v>
+      </c>
+      <c r="I277" s="10" t="str">
+        <f t="shared" si="41"/>
+        <v xml:space="preserve"> appearance  ; အသွင်အပြင် ; အသြင္အျပင္</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B278" t="s">
+        <v>424</v>
+      </c>
+      <c r="C278" t="s">
+        <v>425</v>
+      </c>
+      <c r="E278" t="s">
+        <v>426</v>
+      </c>
+      <c r="I278" s="10" t="str">
+        <f t="shared" ref="I278:I280" si="42">CONCATENATE(D278," ",E278," ",F278)</f>
+        <v xml:space="preserve"> full effort </v>
+      </c>
+    </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B279" t="s">
+        <v>904</v>
+      </c>
+      <c r="C279" t="s">
+        <v>925</v>
+      </c>
+      <c r="E279" t="s">
+        <v>958</v>
+      </c>
+      <c r="I279" s="10" t="str">
+        <f t="shared" si="42"/>
+        <v xml:space="preserve"> to try hard; to fight </v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B280" t="s">
+        <v>905</v>
+      </c>
+      <c r="C280" t="s">
+        <v>926</v>
+      </c>
+      <c r="E280" t="s">
+        <v>948</v>
+      </c>
+      <c r="I280" s="10" t="str">
+        <f t="shared" si="42"/>
+        <v xml:space="preserve"> performer, cast member </v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B281" t="s">
+        <v>906</v>
+      </c>
+      <c r="C281" t="s">
+        <v>927</v>
+      </c>
+      <c r="E281" t="s">
+        <v>959</v>
+      </c>
+      <c r="G281" s="10" t="s">
+        <v>984</v>
+      </c>
+      <c r="H281" s="10" t="s">
+        <v>968</v>
+      </c>
+      <c r="I281" s="10" t="str">
+        <f t="shared" ref="I281" si="43">CONCATENATE(D281," ",E281," ",F281, " ; ",G281," ; ", H281)</f>
+        <v xml:space="preserve"> to get in the news  ; ပြောစရာခေါင်းစဉ် ဖြစ်လာသည် ; ေျပာစရာေခါင္းစဥ္ ျဖစ္လာသည္</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B282" t="s">
+        <v>907</v>
+      </c>
+      <c r="C282" t="s">
+        <v>928</v>
+      </c>
+      <c r="E282" t="s">
+        <v>949</v>
+      </c>
+      <c r="I282" s="10" t="str">
+        <f t="shared" ref="I282:I283" si="44">CONCATENATE(D282," ",E282," ",F282)</f>
+        <v xml:space="preserve"> feature article </v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B283" t="s">
+        <v>908</v>
+      </c>
+      <c r="C283" t="s">
+        <v>929</v>
+      </c>
+      <c r="E283" t="s">
+        <v>960</v>
+      </c>
+      <c r="I283" s="10" t="str">
+        <f t="shared" si="44"/>
+        <v xml:space="preserve"> deeply interesting </v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B284" t="s">
+        <v>909</v>
+      </c>
+      <c r="C284" t="s">
+        <v>930</v>
+      </c>
+      <c r="E284" t="s">
+        <v>961</v>
+      </c>
+      <c r="F284" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G284" s="10" t="s">
+        <v>985</v>
+      </c>
+      <c r="H284" s="10" t="s">
+        <v>969</v>
+      </c>
+      <c r="I284" s="10" t="str">
+        <f t="shared" ref="I284" si="45">CONCATENATE(D284," ",E284," ",F284, " ; ",G284," ; ", H284)</f>
+        <v xml:space="preserve"> consideration (to be considerate) (する) ; ကိုယ်ချင်းစာ စဉ်းစားပေးသည် ; ကိုယ္ခ်င္းစာ စဥ္းစားေပးသည္</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B285" t="s">
+        <v>910</v>
+      </c>
+      <c r="C285" t="s">
+        <v>931</v>
+      </c>
+      <c r="E285" t="s">
+        <v>962</v>
+      </c>
+      <c r="F285" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I285" s="10" t="str">
+        <f t="shared" ref="I285" si="46">CONCATENATE(D285," ",E285," ",F285)</f>
+        <v xml:space="preserve"> breaking a bone (to break a bone) (する)</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B286" t="s">
+        <v>911</v>
+      </c>
+      <c r="C286" t="s">
+        <v>932</v>
+      </c>
+      <c r="E286" t="s">
+        <v>963</v>
+      </c>
+      <c r="F286" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G286" s="10" t="s">
+        <v>986</v>
+      </c>
+      <c r="H286" s="10" t="s">
+        <v>970</v>
+      </c>
+      <c r="I286" s="10" t="str">
+        <f t="shared" ref="I286:I288" si="47">CONCATENATE(D286," ",E286," ",F286, " ; ",G286," ; ", H286)</f>
+        <v xml:space="preserve"> malicious use (to use maliciously) (する) ; မကောင်းတဲ့နေရာ အသုံးချသည် ; မေကာင္းတဲ႔ေနရာ အသံုးခ်သည္</v>
+      </c>
+    </row>
+    <row r="287" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B287" t="s">
+        <v>912</v>
+      </c>
+      <c r="C287" t="s">
+        <v>933</v>
+      </c>
+      <c r="E287" t="s">
+        <v>950</v>
+      </c>
+      <c r="G287" s="10" t="s">
+        <v>987</v>
+      </c>
+      <c r="H287" s="10" t="s">
+        <v>971</v>
+      </c>
+      <c r="I287" s="10" t="str">
+        <f t="shared" si="47"/>
+        <v xml:space="preserve"> fraud  ; လှည့်ဖြားပြီး ငွေရယူခြင်း ; လွည့္ျဖားၿပီး ေငြရယူျခင္း</v>
+      </c>
+    </row>
+    <row r="288" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B288" t="s">
+        <v>913</v>
+      </c>
+      <c r="C288" t="s">
+        <v>934</v>
+      </c>
+      <c r="E288" t="s">
+        <v>964</v>
+      </c>
+      <c r="F288" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G288" s="10" t="s">
+        <v>988</v>
+      </c>
+      <c r="H288" s="10" t="s">
+        <v>972</v>
+      </c>
+      <c r="I288" s="10" t="str">
+        <f t="shared" si="47"/>
+        <v xml:space="preserve"> worsening (to become worse) (する) ; ဆိုးဝါးလာသည် ; ဆိုး၀ါးလာသည္</v>
+      </c>
+    </row>
+    <row r="289" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="F289" s="1"/>
+    </row>
+    <row r="290" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A290" s="9" t="s">
+        <v>946</v>
+      </c>
+      <c r="B290" s="6"/>
+      <c r="C290" s="6"/>
+      <c r="D290" s="7"/>
+      <c r="E290" s="6"/>
+      <c r="F290" s="7"/>
+      <c r="G290" s="12"/>
+      <c r="H290" s="12"/>
+      <c r="I290" s="10" t="str">
+        <f>CONCATENATE(D290," ",E290," ",F290)</f>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="291" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B291" t="s">
+        <v>914</v>
+      </c>
+      <c r="C291" t="s">
+        <v>914</v>
+      </c>
+      <c r="E291" t="s">
+        <v>965</v>
+      </c>
+      <c r="G291" s="10" t="s">
+        <v>989</v>
+      </c>
+      <c r="H291" s="10" t="s">
+        <v>973</v>
+      </c>
+      <c r="I291" s="10" t="str">
+        <f t="shared" ref="I291:I292" si="48">CONCATENATE(D291," ",E291," ",F291, " ; ",G291," ; ", H291)</f>
+        <v xml:space="preserve"> to be lively, bustle  ; စည်ကားသည် ; စည္ကားသည္</v>
+      </c>
+    </row>
+    <row r="292" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B292" t="s">
+        <v>935</v>
+      </c>
+      <c r="C292" t="s">
+        <v>935</v>
+      </c>
+      <c r="E292" t="s">
+        <v>951</v>
+      </c>
+      <c r="F292" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G292" s="10" t="s">
+        <v>990</v>
+      </c>
+      <c r="H292" s="10" t="s">
+        <v>974</v>
+      </c>
+      <c r="I292" s="10" t="str">
+        <f t="shared" si="48"/>
+        <v xml:space="preserve"> debut (to debut) (する) ; (မင်းသား၊ မင်းသမီး) ပွဲထုတ်သည် ; (မင္းသား၊ မင္းသမီး) ပြဲထုတ္သည္</v>
+      </c>
+    </row>
+    <row r="293" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B293" t="s">
+        <v>915</v>
+      </c>
+      <c r="C293" t="s">
+        <v>936</v>
+      </c>
+      <c r="E293" t="s">
+        <v>952</v>
+      </c>
+      <c r="I293" s="10" t="str">
+        <f t="shared" ref="I293" si="49">CONCATENATE(D293," ",E293," ",F293)</f>
+        <v xml:space="preserve"> actress </v>
+      </c>
+    </row>
+    <row r="294" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B294" t="s">
+        <v>916</v>
+      </c>
+      <c r="C294" t="s">
+        <v>937</v>
+      </c>
+      <c r="E294" t="s">
+        <v>966</v>
+      </c>
+      <c r="G294" s="10" t="s">
+        <v>991</v>
+      </c>
+      <c r="H294" s="10" t="s">
+        <v>975</v>
+      </c>
+      <c r="I294" s="10" t="str">
+        <f t="shared" ref="I294" si="50">CONCATENATE(D294," ",E294," ",F294, " ; ",G294," ; ", H294)</f>
+        <v xml:space="preserve"> to finish up  ; အပြီးသတ်သည် ; အၿပီးသတ္သည္</v>
+      </c>
+    </row>
+    <row r="295" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B295" t="s">
+        <v>917</v>
+      </c>
+      <c r="C295" t="s">
+        <v>938</v>
+      </c>
+      <c r="E295" t="s">
+        <v>967</v>
+      </c>
+      <c r="I295" s="10" t="str">
+        <f t="shared" ref="I295" si="51">CONCATENATE(D295," ",E295," ",F295)</f>
+        <v xml:space="preserve"> to be coddled </v>
+      </c>
+    </row>
+    <row r="297" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A297" s="9" t="s">
+        <v>947</v>
+      </c>
+      <c r="B297" s="6"/>
+      <c r="C297" s="6"/>
+      <c r="D297" s="7"/>
+      <c r="E297" s="6"/>
+      <c r="F297" s="7"/>
+      <c r="G297" s="12"/>
+      <c r="H297" s="12"/>
+      <c r="I297" s="10" t="str">
+        <f>CONCATENATE(D297," ",E297," ",F297)</f>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="298" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B298" t="s">
+        <v>918</v>
+      </c>
+      <c r="C298" t="s">
+        <v>939</v>
+      </c>
+      <c r="E298" t="s">
+        <v>953</v>
+      </c>
+      <c r="I298" s="10" t="str">
+        <f t="shared" ref="I298:I300" si="52">CONCATENATE(D298," ",E298," ",F298)</f>
+        <v xml:space="preserve"> on the ocean </v>
+      </c>
+    </row>
+    <row r="299" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B299" t="s">
+        <v>919</v>
+      </c>
+      <c r="C299" t="s">
+        <v>940</v>
+      </c>
+      <c r="E299" t="s">
+        <v>954</v>
+      </c>
+      <c r="I299" s="10" t="str">
+        <f t="shared" si="52"/>
+        <v xml:space="preserve"> air pressure </v>
+      </c>
+    </row>
+    <row r="300" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B300" t="s">
+        <v>920</v>
+      </c>
+      <c r="C300" t="s">
+        <v>920</v>
+      </c>
+      <c r="E300" t="s">
+        <v>976</v>
+      </c>
+      <c r="I300" s="10" t="str">
+        <f t="shared" si="52"/>
+        <v xml:space="preserve"> hectopascal </v>
+      </c>
+    </row>
+    <row r="301" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B301" t="s">
+        <v>921</v>
+      </c>
+      <c r="C301" t="s">
+        <v>941</v>
+      </c>
+      <c r="E301" t="s">
+        <v>955</v>
+      </c>
+      <c r="G301" s="10" t="s">
+        <v>992</v>
+      </c>
+      <c r="H301" s="10" t="s">
+        <v>977</v>
+      </c>
+      <c r="I301" s="10" t="str">
+        <f t="shared" ref="I301" si="53">CONCATENATE(D301," ",E301," ",F301, " ; ",G301," ; ", H301)</f>
+        <v xml:space="preserve"> maximum wind speed  ; အချိန်တိုအတွင်း အမြန်ဆုံး လေတိုက်နှုန်း ; အခ်ိန္တိုအတြင္း အျမန္ဆံုး ေလတိုက္ႏႈန္း</v>
+      </c>
+    </row>
+    <row r="302" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B302" t="s">
+        <v>922</v>
+      </c>
+      <c r="C302" t="s">
+        <v>942</v>
+      </c>
+      <c r="E302" t="s">
+        <v>956</v>
+      </c>
+      <c r="I302" s="10" t="str">
+        <f t="shared" ref="I302" si="54">CONCATENATE(D302," ",E302," ",F302)</f>
+        <v xml:space="preserve"> storm area </v>
+      </c>
+    </row>
+    <row r="303" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B303" t="s">
+        <v>923</v>
+      </c>
+      <c r="C303" t="s">
+        <v>943</v>
+      </c>
+      <c r="E303" t="s">
+        <v>957</v>
+      </c>
+      <c r="G303" s="10" t="s">
+        <v>993</v>
+      </c>
+      <c r="H303" s="10" t="s">
+        <v>978</v>
+      </c>
+      <c r="I303" s="10" t="str">
+        <f t="shared" ref="I303:I305" si="55">CONCATENATE(D303," ",E303," ",F303, " ; ",G303," ; ", H303)</f>
+        <v xml:space="preserve"> wide range  ; ကျယ်ပြန့်တဲ့ ဧရိယာ ; က်ယ္ျပန္႔တဲ႔ ဧရိယာ</v>
+      </c>
+    </row>
+    <row r="304" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B304" t="s">
+        <v>924</v>
+      </c>
+      <c r="C304" t="s">
+        <v>944</v>
+      </c>
+      <c r="E304" t="s">
+        <v>343</v>
+      </c>
+      <c r="G304" s="10" t="s">
+        <v>994</v>
+      </c>
+      <c r="H304" s="10" t="s">
+        <v>979</v>
+      </c>
+      <c r="I304" s="10" t="str">
+        <f t="shared" si="55"/>
+        <v xml:space="preserve"> coast  ; ကမ်းစပ် ; ကမ္းစပ္</v>
+      </c>
+    </row>
+    <row r="305" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B305" t="s">
+        <v>794</v>
+      </c>
+      <c r="C305" t="s">
+        <v>848</v>
+      </c>
+      <c r="E305" t="s">
+        <v>980</v>
+      </c>
+      <c r="F305" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G305" s="10" t="s">
+        <v>995</v>
+      </c>
+      <c r="H305" s="10" t="s">
+        <v>981</v>
+      </c>
+      <c r="I305" s="10" t="str">
+        <f t="shared" si="55"/>
+        <v xml:space="preserve"> approaching (to approach)  (する) ; နီးကပ်လာသည် ; နီးကပ္လာသည္</v>
       </c>
     </row>
   </sheetData>

</xml_diff>